<commit_message>
Bug fixes and optimization.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAC18F4-E474-4B5F-BA47-20E541C7FC31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA319D2-523E-4F92-8C39-F17B9B580B35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45360" yWindow="1710" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43335" yWindow="2475" windowWidth="28800" windowHeight="16230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>tc={40A82B49-95A5-4984-90D4-AB59EAD5E8C5}</author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>PSNR</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>V1.02.2</t>
+  </si>
+  <si>
+    <t>V1.03.1</t>
+  </si>
+  <si>
+    <t>V1.03.2</t>
+  </si>
+  <si>
+    <t>V1.01.1</t>
+  </si>
+  <si>
+    <t>V1.02.1</t>
+  </si>
+  <si>
+    <t>V1.01.2</t>
+  </si>
+  <si>
+    <t>V1.01.3</t>
+  </si>
+  <si>
+    <t>V1.01.5</t>
+  </si>
+  <si>
+    <t>V1.03.6</t>
   </si>
 </sst>
 </file>
@@ -420,7 +444,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A9" dT="2021-04-20T10:03:24.42" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
+  <threadedComment ref="A14" dT="2021-04-20T10:03:24.42" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
     <text>Dependencies:
 Albedo --&gt; Transmission Map
 Albedo --&gt; Airlight Estimator V2</text>
@@ -430,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +544,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>9.6412099999999992</v>
@@ -560,6 +584,30 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>9.4274299999999993</v>
+      </c>
+      <c r="C4">
+        <v>0.11418</v>
+      </c>
+      <c r="D4">
+        <v>0.53954999999999997</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>22.260269999999998</v>
+      </c>
+      <c r="H4">
+        <v>5.9899999999999997E-3</v>
+      </c>
+      <c r="I4">
+        <v>0.79791999999999996</v>
+      </c>
       <c r="K4" t="s">
         <v>8</v>
       </c>
@@ -573,8 +621,95 @@
         <v>2.3481999999999998</v>
       </c>
     </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>13.53234</v>
+      </c>
+      <c r="C5">
+        <v>4.4470000000000003E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.56920999999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>20.749400000000001</v>
+      </c>
+      <c r="H5">
+        <v>8.5100000000000002E-3</v>
+      </c>
+      <c r="I5">
+        <v>0.82787999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>13.17601</v>
+      </c>
+      <c r="C6">
+        <v>4.8250000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.53405000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>13.1869</v>
+      </c>
+      <c r="C7">
+        <v>4.811E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.40762999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>18.560929999999999</v>
+      </c>
+      <c r="C8">
+        <v>1.3950000000000001E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.73333999999999999</v>
+      </c>
+    </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>18.985990000000001</v>
+      </c>
+      <c r="C10">
+        <v>1.265E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.70992999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed network architecture of albedo extractor to FFA net style.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA319D2-523E-4F92-8C39-F17B9B580B35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E236A1D-CB87-46A0-92CC-C1AEF8AE3B65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43335" yWindow="2475" windowWidth="28800" windowHeight="16230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8385" yWindow="1725" windowWidth="28530" windowHeight="16230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>tc={40A82B49-95A5-4984-90D4-AB59EAD5E8C5}</author>
   </authors>
   <commentList>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
+    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>PSNR</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>V1.03.6</t>
+  </si>
+  <si>
+    <t>V1.03.4</t>
+  </si>
+  <si>
+    <t>V1.04.1</t>
+  </si>
+  <si>
+    <t>V1.04.2</t>
+  </si>
+  <si>
+    <t>V1.0.3.7</t>
   </si>
 </sst>
 </file>
@@ -444,7 +456,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A14" dT="2021-04-20T10:03:24.42" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
+  <threadedComment ref="A17" dT="2021-04-20T10:03:24.42" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
     <text>Dependencies:
 Albedo --&gt; Transmission Map
 Albedo --&gt; Airlight Estimator V2</text>
@@ -454,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,20 +708,76 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>16.04551</v>
+      </c>
+      <c r="C10">
+        <v>2.487E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.61460000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>18.985990000000001</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>1.265E-2</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>0.70992999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>18.288640000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.485E-2</v>
+      </c>
+      <c r="D12">
+        <v>0.70435999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>18.649069999999998</v>
+      </c>
+      <c r="C13">
+        <v>1.366E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.66188999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>17.952729999999999</v>
+      </c>
+      <c r="C14">
+        <v>1.6029999999999999E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.63197999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Checkpoint for new scripts
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E236A1D-CB87-46A0-92CC-C1AEF8AE3B65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F78EB20-BE6C-40C1-854E-729099B62BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="1725" windowWidth="28530" windowHeight="16230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>PSNR</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>V1.0.3.7</t>
+  </si>
+  <si>
+    <t>V1.04.3</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +675,18 @@
       <c r="D6">
         <v>0.53405000000000002</v>
       </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>21.47146</v>
+      </c>
+      <c r="H6">
+        <v>7.2199999999999999E-3</v>
+      </c>
+      <c r="I6">
+        <v>0.84968999999999995</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -753,13 +768,13 @@
         <v>22</v>
       </c>
       <c r="B13">
-        <v>18.649069999999998</v>
+        <v>24.931889999999999</v>
       </c>
       <c r="C13">
-        <v>1.366E-2</v>
+        <v>3.2200000000000002E-3</v>
       </c>
       <c r="D13">
-        <v>0.66188999999999998</v>
+        <v>0.81723999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -767,13 +782,27 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>17.952729999999999</v>
+        <v>22.571529999999999</v>
       </c>
       <c r="C14">
-        <v>1.6029999999999999E-2</v>
+        <v>5.5500000000000002E-3</v>
       </c>
       <c r="D14">
-        <v>0.63197999999999999</v>
+        <v>0.77834000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>21.37276</v>
+      </c>
+      <c r="C15">
+        <v>7.3099999999999997E-3</v>
+      </c>
+      <c r="D15">
+        <v>0.752</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Checkpoint for new benchmarking test.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F78EB20-BE6C-40C1-854E-729099B62BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123B684-5244-4AAF-A9FC-863A1318990C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41865" yWindow="2790" windowWidth="30180" windowHeight="16995" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,50 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={0FAD6CEB-CB5F-4DFF-8D01-DEFC0CDD8613}</author>
+    <author>tc={E82EA847-54E7-4608-A448-8D64BCF97254}</author>
+    <author>tc={3F86E3B3-8FF0-4088-B742-25CD9983CE5C}</author>
+    <author>tc={DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}</author>
     <author>tc={40A82B49-95A5-4984-90D4-AB59EAD5E8C5}</author>
   </authors>
   <commentList>
-    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{0FAD6CEB-CB5F-4DFF-8D01-DEFC0CDD8613}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Uniform distribution</t>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="1" shapeId="0" xr:uid="{E82EA847-54E7-4608-A448-8D64BCF97254}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V1</t>
+      </text>
+    </comment>
+    <comment ref="Q4" authorId="2" shapeId="0" xr:uid="{3F86E3B3-8FF0-4088-B742-25CD9983CE5C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Gaussian distribution</t>
+      </text>
+    </comment>
+    <comment ref="S4" authorId="3" shapeId="0" xr:uid="{DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V2</t>
+      </text>
+    </comment>
+    <comment ref="A27" authorId="4" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -45,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>PSNR</t>
   </si>
@@ -119,17 +159,32 @@
     <t>V1.04.2</t>
   </si>
   <si>
-    <t>V1.0.3.7</t>
-  </si>
-  <si>
     <t>V1.04.3</t>
+  </si>
+  <si>
+    <t>V1.04.4</t>
+  </si>
+  <si>
+    <t>V1.03.7</t>
+  </si>
+  <si>
+    <t>Mix 1</t>
+  </si>
+  <si>
+    <t>Mix 2</t>
+  </si>
+  <si>
+    <t>O-Haze Performance</t>
+  </si>
+  <si>
+    <t>RESIDE-OTS Performance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +199,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,7 +244,128 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -192,7 +380,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="neil.delgallego@dlsu.edu.ph" id="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" userId="S::neil.delgallego@dlsu.edu.ph::9fccce03-204c-489b-ae7d-5aeb7f0c6bb7" providerId="AD"/>
+  <person displayName="Neil Patrick  A. Del Gallego" id="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" userId="S::neil.delgallego@dlsu.edu.ph::9fccce03-204c-489b-ae7d-5aeb7f0c6bb7" providerId="AD"/>
 </personList>
 </file>
 
@@ -459,7 +647,23 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A17" dT="2021-04-20T10:03:24.42" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
+  <threadedComment ref="Q3" dT="2021-05-18T03:13:43.18" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{0FAD6CEB-CB5F-4DFF-8D01-DEFC0CDD8613}">
+    <text>Uniform distribution</text>
+  </threadedComment>
+  <threadedComment ref="S3" dT="2021-05-18T12:56:43.53" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{E82EA847-54E7-4608-A448-8D64BCF97254}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V1</text>
+  </threadedComment>
+  <threadedComment ref="Q4" dT="2021-05-18T03:13:33.39" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{3F86E3B3-8FF0-4088-B742-25CD9983CE5C}">
+    <text>Gaussian distribution</text>
+  </threadedComment>
+  <threadedComment ref="S4" dT="2021-05-18T12:56:52.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V2</text>
+  </threadedComment>
+  <threadedComment ref="A27" dT="2021-04-20T10:03:24.42" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
     <text>Dependencies:
 Albedo --&gt; Transmission Map
 Albedo --&gt; Airlight Estimator V2</text>
@@ -469,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,9 +686,12 @@
     <col min="12" max="12" width="13.7109375" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="23" max="24" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -512,8 +719,16 @@
       </c>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="3"/>
+      <c r="W1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -556,8 +771,20 @@
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -597,8 +824,17 @@
       <c r="Q3">
         <v>2.8829400000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3">
+        <v>15.36356</v>
+      </c>
+      <c r="U3">
+        <v>0.83669000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -635,8 +871,20 @@
       <c r="O4">
         <v>2.3481999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>4.0149999999999998E-2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4">
+        <v>15.54205</v>
+      </c>
+      <c r="U4">
+        <v>0.83874000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -661,8 +909,20 @@
       <c r="I5">
         <v>0.82787999999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5">
+        <v>1.3610000000000001E-2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5">
+        <v>1.468E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -687,8 +947,20 @@
       <c r="I6">
         <v>0.84968999999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6">
+        <v>1.3820000000000001E-2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6">
+        <v>1.436E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -701,8 +973,32 @@
       <c r="D7">
         <v>0.40762999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>25.76465</v>
+      </c>
+      <c r="H7">
+        <v>2.6900000000000001E-3</v>
+      </c>
+      <c r="I7">
+        <v>0.91974</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7">
+        <v>1.487E-2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7">
+        <v>1.728E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -715,13 +1011,43 @@
       <c r="D8">
         <v>0.73333999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>18.132660000000001</v>
+      </c>
+      <c r="H8">
+        <v>1.5389999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.73133999999999999</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>16.719280000000001</v>
+      </c>
+      <c r="H9">
+        <v>2.1329999999999998E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.74704000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -735,7 +1061,7 @@
         <v>0.61460000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -749,9 +1075,9 @@
         <v>0.70992999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>18.288640000000001</v>
@@ -763,7 +1089,7 @@
         <v>0.70435999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -777,7 +1103,7 @@
         <v>0.81723999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -791,9 +1117,9 @@
         <v>0.77834000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>21.37276</v>
@@ -805,41 +1131,56 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="W1:X1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="T1:U1"/>
   </mergeCells>
-  <conditionalFormatting sqref="O3:O4">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="L3:L15">
+    <cfRule type="top10" dxfId="11" priority="12" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L4">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="O3:O13">
+    <cfRule type="top10" dxfId="10" priority="11" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="top10" dxfId="8" priority="9" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X2">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Checkpoint for refinement network experiment
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123B684-5244-4AAF-A9FC-863A1318990C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2969807C-01A9-48E5-8229-5431A9F2EDA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41865" yWindow="2790" windowWidth="30180" windowHeight="16995" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39600" yWindow="1830" windowWidth="24315" windowHeight="16995" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,12 +205,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -675,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,6 +826,12 @@
       </c>
       <c r="U3">
         <v>0.83669000000000004</v>
+      </c>
+      <c r="W3">
+        <v>21.71951</v>
+      </c>
+      <c r="X3">
+        <v>0.96267000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Checkpoint on scripts and model performances.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2969807C-01A9-48E5-8229-5431A9F2EDA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B4188B-E7ED-44ED-83A0-ABD9E914565D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39600" yWindow="1830" windowWidth="24315" windowHeight="16995" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40380" yWindow="1680" windowWidth="24315" windowHeight="16995" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>PSNR</t>
   </si>
@@ -178,12 +178,24 @@
   </si>
   <si>
     <t>RESIDE-OTS Performance</t>
+  </si>
+  <si>
+    <t>V1.04.5</t>
+  </si>
+  <si>
+    <t>V1.04.6</t>
+  </si>
+  <si>
+    <t>V1.04.7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,10 +239,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -670,7 +683,7 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,41 +699,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="L1" s="4"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="3"/>
+      <c r="O1" s="4"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="U1" s="4"/>
+      <c r="W1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="3"/>
+      <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -883,6 +896,12 @@
       <c r="U4">
         <v>0.83874000000000004</v>
       </c>
+      <c r="W4" s="3">
+        <v>22.3033</v>
+      </c>
+      <c r="X4">
+        <v>0.96426000000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1015,13 +1034,13 @@
         <v>24</v>
       </c>
       <c r="G8">
-        <v>18.132660000000001</v>
+        <v>33.608440000000002</v>
       </c>
       <c r="H8">
-        <v>1.5389999999999999E-2</v>
+        <v>4.4999999999999999E-4</v>
       </c>
       <c r="I8">
-        <v>0.73133999999999999</v>
+        <v>0.97160000000000002</v>
       </c>
       <c r="K8" t="s">
         <v>25</v>
@@ -1038,13 +1057,13 @@
         <v>25</v>
       </c>
       <c r="G9">
-        <v>16.719280000000001</v>
+        <v>29.921849999999999</v>
       </c>
       <c r="H9">
-        <v>2.1329999999999998E-2</v>
+        <v>1.0399999999999999E-3</v>
       </c>
       <c r="I9">
-        <v>0.74704000000000004</v>
+        <v>0.95730000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1060,6 +1079,18 @@
       <c r="D10">
         <v>0.61460000000000004</v>
       </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10">
+        <v>32.728729999999999</v>
+      </c>
+      <c r="H10">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="I10">
+        <v>0.96704999999999997</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1074,6 +1105,18 @@
       <c r="D11">
         <v>0.70992999999999995</v>
       </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>29.98086</v>
+      </c>
+      <c r="H11">
+        <v>1.0200000000000001E-3</v>
+      </c>
+      <c r="I11">
+        <v>0.93915999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1087,6 +1130,18 @@
       </c>
       <c r="D12">
         <v>0.70435999999999999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12">
+        <v>29.826049999999999</v>
+      </c>
+      <c r="H12">
+        <v>1.06E-3</v>
+      </c>
+      <c r="I12">
+        <v>0.93645</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated scripts and benchmark results.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B4188B-E7ED-44ED-83A0-ABD9E914565D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7DC97A-A09D-47AC-ACAC-EC7DD325F9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40380" yWindow="1680" windowWidth="24315" windowHeight="16995" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41625" yWindow="1215" windowWidth="24315" windowHeight="16995" tabRatio="198" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,9 +29,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={0FAD6CEB-CB5F-4DFF-8D01-DEFC0CDD8613}</author>
-    <author>tc={E82EA847-54E7-4608-A448-8D64BCF97254}</author>
     <author>tc={3F86E3B3-8FF0-4088-B742-25CD9983CE5C}</author>
-    <author>tc={DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}</author>
     <author>tc={40A82B49-95A5-4984-90D4-AB59EAD5E8C5}</author>
   </authors>
   <commentList>
@@ -42,17 +41,7 @@
     Uniform distribution</t>
       </text>
     </comment>
-    <comment ref="S3" authorId="1" shapeId="0" xr:uid="{E82EA847-54E7-4608-A448-8D64BCF97254}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Albedo - V1.04.1
-Transmission - V1.04.2
-Airlight - V1.04.1 - V1</t>
-      </text>
-    </comment>
-    <comment ref="Q4" authorId="2" shapeId="0" xr:uid="{3F86E3B3-8FF0-4088-B742-25CD9983CE5C}">
+    <comment ref="Q4" authorId="1" shapeId="0" xr:uid="{3F86E3B3-8FF0-4088-B742-25CD9983CE5C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -60,17 +49,7 @@
     Gaussian distribution</t>
       </text>
     </comment>
-    <comment ref="S4" authorId="3" shapeId="0" xr:uid="{DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Albedo - V1.04.1
-Transmission - V1.04.2
-Airlight - V1.04.1 - V2</t>
-      </text>
-    </comment>
-    <comment ref="A27" authorId="4" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
+    <comment ref="A27" authorId="2" shapeId="0" xr:uid="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -84,8 +63,109 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E82EA847-54E7-4608-A448-8D64BCF97254}</author>
+    <author>tc={DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}</author>
+    <author>tc={21E14CA7-7C70-4824-A24A-24B19D5AC225}</author>
+    <author>tc={B423A14E-6E73-4CA1-8A5E-4AF9FB25AB6A}</author>
+    <author>tc={CC4DD7ED-03B2-42EC-97D0-F81EF4F06185}</author>
+    <author>tc={0E4A7996-D293-44E9-81E2-FFF166AC288C}</author>
+    <author>tc={72DC73A6-4878-4D44-AAEC-1899666F9E0A}</author>
+    <author>tc={E5A81D46-C47A-4F8B-B1AC-CF962EF34B5F}</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{E82EA847-54E7-4608-A448-8D64BCF97254}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V1</t>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="1" shapeId="0" xr:uid="{DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V2</t>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="2" shapeId="0" xr:uid="{21E14CA7-7C70-4824-A24A-24B19D5AC225}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.3
+Airlight - V1.04.1 - V1</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="3" shapeId="0" xr:uid="{B423A14E-6E73-4CA1-8A5E-4AF9FB25AB6A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.06.1
+Airlight - V1.04.1 - V1</t>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="4" shapeId="0" xr:uid="{CC4DD7ED-03B2-42EC-97D0-F81EF4F06185}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V2
+Filter Reduction - 0.7</t>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="5" shapeId="0" xr:uid="{0E4A7996-D293-44E9-81E2-FFF166AC288C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.05.1 - V1
+Filter Reduction - 0.7</t>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="6" shapeId="0" xr:uid="{72DC73A6-4878-4D44-AAEC-1899666F9E0A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.05.1 - V1
+Filter Reduction - 0.8</t>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="7" shapeId="0" xr:uid="{E5A81D46-C47A-4F8B-B1AC-CF962EF34B5F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.05.2- V1
+Filter Reduction - 0.8</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>PSNR</t>
   </si>
@@ -187,6 +267,36 @@
   </si>
   <si>
     <t>V1.04.7</t>
+  </si>
+  <si>
+    <t>Mix 3</t>
+  </si>
+  <si>
+    <t>V1.05.1</t>
+  </si>
+  <si>
+    <t>V1.06.1</t>
+  </si>
+  <si>
+    <t>Mix 4</t>
+  </si>
+  <si>
+    <t>Inverted T</t>
+  </si>
+  <si>
+    <t>Mix 5</t>
+  </si>
+  <si>
+    <t>Mix 6</t>
+  </si>
+  <si>
+    <t>Mix 7</t>
+  </si>
+  <si>
+    <t>Mix 8</t>
+  </si>
+  <si>
+    <t>I-Haze Performance</t>
   </si>
 </sst>
 </file>
@@ -196,7 +306,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +327,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,7 +367,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -657,18 +793,8 @@
   <threadedComment ref="Q3" dT="2021-05-18T03:13:43.18" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{0FAD6CEB-CB5F-4DFF-8D01-DEFC0CDD8613}">
     <text>Uniform distribution</text>
   </threadedComment>
-  <threadedComment ref="S3" dT="2021-05-18T12:56:43.53" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{E82EA847-54E7-4608-A448-8D64BCF97254}">
-    <text>Albedo - V1.04.1
-Transmission - V1.04.2
-Airlight - V1.04.1 - V1</text>
-  </threadedComment>
   <threadedComment ref="Q4" dT="2021-05-18T03:13:33.39" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{3F86E3B3-8FF0-4088-B742-25CD9983CE5C}">
     <text>Gaussian distribution</text>
-  </threadedComment>
-  <threadedComment ref="S4" dT="2021-05-18T12:56:52.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}">
-    <text>Albedo - V1.04.1
-Transmission - V1.04.2
-Airlight - V1.04.1 - V2</text>
   </threadedComment>
   <threadedComment ref="A27" dT="2021-04-20T10:03:24.42" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{40A82B49-95A5-4984-90D4-AB59EAD5E8C5}">
     <text>Dependencies:
@@ -678,12 +804,61 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A3" dT="2021-05-18T12:56:43.53" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{E82EA847-54E7-4608-A448-8D64BCF97254}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V1</text>
+  </threadedComment>
+  <threadedComment ref="A4" dT="2021-05-18T12:56:52.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{DBDF72CD-B7FB-4546-AEB4-02DC53AA84CC}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V2</text>
+  </threadedComment>
+  <threadedComment ref="A5" dT="2021-05-18T12:56:43.53" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{21E14CA7-7C70-4824-A24A-24B19D5AC225}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.3
+Airlight - V1.04.1 - V1</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2021-05-18T12:56:43.53" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{B423A14E-6E73-4CA1-8A5E-4AF9FB25AB6A}">
+    <text>Albedo - V1.04.1
+Transmission - V1.06.1
+Airlight - V1.04.1 - V1</text>
+  </threadedComment>
+  <threadedComment ref="A11" dT="2021-05-18T12:56:52.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{CC4DD7ED-03B2-42EC-97D0-F81EF4F06185}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.04.1 - V2
+Filter Reduction - 0.7</text>
+  </threadedComment>
+  <threadedComment ref="A12" dT="2021-05-18T12:56:52.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{0E4A7996-D293-44E9-81E2-FFF166AC288C}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.05.1 - V1
+Filter Reduction - 0.7</text>
+  </threadedComment>
+  <threadedComment ref="A13" dT="2021-05-18T12:56:52.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{72DC73A6-4878-4D44-AAEC-1899666F9E0A}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.05.1 - V1
+Filter Reduction - 0.8</text>
+  </threadedComment>
+  <threadedComment ref="A14" dT="2021-05-18T12:56:52.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{E5A81D46-C47A-4F8B-B1AC-CF962EF34B5F}">
+    <text>Albedo - V1.04.1
+Transmission - V1.04.2
+Airlight - V1.05.2- V1
+Filter Reduction - 0.8</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +873,7 @@
     <col min="23" max="24" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -725,17 +900,8 @@
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="4"/>
-      <c r="W1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -777,21 +943,8 @@
         <v>9</v>
       </c>
       <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -831,23 +984,8 @@
       <c r="Q3">
         <v>2.8829400000000001</v>
       </c>
-      <c r="S3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3">
-        <v>15.36356</v>
-      </c>
-      <c r="U3">
-        <v>0.83669000000000004</v>
-      </c>
-      <c r="W3">
-        <v>21.71951</v>
-      </c>
-      <c r="X3">
-        <v>0.96267000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -887,23 +1025,8 @@
       <c r="Q4">
         <v>4.0149999999999998E-2</v>
       </c>
-      <c r="S4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T4">
-        <v>15.54205</v>
-      </c>
-      <c r="U4">
-        <v>0.83874000000000004</v>
-      </c>
-      <c r="W4" s="3">
-        <v>22.3033</v>
-      </c>
-      <c r="X4">
-        <v>0.96426000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -941,7 +1064,7 @@
         <v>1.468E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -979,7 +1102,7 @@
         <v>1.436E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1017,7 +1140,7 @@
         <v>1.728E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1049,7 +1172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1065,8 +1188,20 @@
       <c r="I9">
         <v>0.95730000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9">
+        <v>1.363E-2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9">
+        <v>1.6289999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1092,7 +1227,7 @@
         <v>0.96704999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1118,7 +1253,7 @@
         <v>0.93915999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +1279,7 @@
         <v>0.93645</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1158,7 +1293,7 @@
         <v>0.81723999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1171,8 +1306,20 @@
       <c r="D14">
         <v>0.77834000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14">
+        <v>25.70628</v>
+      </c>
+      <c r="H14">
+        <v>1.329E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.88024000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1186,59 +1333,281 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="W1:X1"/>
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="11" priority="12" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="12" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="10" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="8" priority="9" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="9" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="6" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W2">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E4D2B0-246F-48C3-B870-33165E2ABBB9}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>15.36356</v>
+      </c>
+      <c r="C3">
+        <v>0.83669000000000004</v>
+      </c>
+      <c r="H3">
+        <v>21.71951</v>
+      </c>
+      <c r="I3">
+        <v>0.96267000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>15.54205</v>
+      </c>
+      <c r="C4">
+        <v>0.83874000000000004</v>
+      </c>
+      <c r="H4" s="3">
+        <v>22.3033</v>
+      </c>
+      <c r="I4">
+        <v>0.96426000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>15.170680000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.83174999999999999</v>
+      </c>
+      <c r="H5">
+        <v>21.379529999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.95659000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>15.06462</v>
+      </c>
+      <c r="C6">
+        <v>0.82930999999999999</v>
+      </c>
+      <c r="H6">
+        <v>21.289100000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.95581000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>14.95074</v>
+      </c>
+      <c r="C11">
+        <v>0.82809999999999995</v>
+      </c>
+      <c r="H11">
+        <v>20.077909999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.96001000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>14.58703</v>
+      </c>
+      <c r="C12">
+        <v>0.83023000000000002</v>
+      </c>
+      <c r="H12">
+        <v>19.243189999999998</v>
+      </c>
+      <c r="I12">
+        <v>0.94542999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>14.87238</v>
+      </c>
+      <c r="C13">
+        <v>0.83857000000000004</v>
+      </c>
+      <c r="E13">
+        <v>16.02392</v>
+      </c>
+      <c r="F13">
+        <v>0.87753000000000003</v>
+      </c>
+      <c r="H13">
+        <v>20.222660000000001</v>
+      </c>
+      <c r="I13">
+        <v>0.96033000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>15.06216</v>
+      </c>
+      <c r="C14">
+        <v>0.83582999999999996</v>
+      </c>
+      <c r="E14">
+        <v>15.812469999999999</v>
+      </c>
+      <c r="F14">
+        <v>0.86987000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Latest checkpoint of project.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -5,22 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\delgallegon\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDC431C-30BC-4B9E-A3A6-F22DE1A1FB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D02395-2E36-49AE-8ECF-5FBE1A849FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40050" yWindow="2070" windowWidth="24315" windowHeight="16995" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41340" yWindow="2460" windowWidth="33060" windowHeight="15435" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="Actual" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -77,6 +86,13 @@
     <author>tc={E5A81D46-C47A-4F8B-B1AC-CF962EF34B5F}</author>
     <author>tc={1977C059-DF85-4730-8DF2-9DDE1A872EB9}</author>
     <author>tc={4094402C-F5C5-47DB-BB10-76538A3FD858}</author>
+    <author>tc={1631D402-746A-4827-BF4C-839F3BA272C6}</author>
+    <author>tc={907B7804-9C5A-4E10-B69A-D3A98603E98C}</author>
+    <author>tc={FCC4E973-4106-4AC1-A598-C8AB62A595D0}</author>
+    <author>tc={93EBB620-A219-4A52-BC3E-044462FB7776}</author>
+    <author>tc={BA14E670-3446-4794-8F7A-737043F69BF5}</author>
+    <author>tc={D81608AE-052B-4752-BBC5-25B914B72E85}</author>
+    <author>tc={2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}</author>
   </authors>
   <commentList>
     <comment ref="A3" authorId="0" shapeId="0" xr:uid="{E82EA847-54E7-4608-A448-8D64BCF97254}">
@@ -185,12 +201,174 @@
 Filter Reduction - 0.8</t>
       </text>
     </comment>
+    <comment ref="A17" authorId="10" shapeId="0" xr:uid="{1631D402-746A-4827-BF4C-839F3BA272C6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.07.1
+Airlight - V1.05.1- V1
+Filter Reduction - 0.8</t>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="11" shapeId="0" xr:uid="{907B7804-9C5A-4E10-B69A-D3A98603E98C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.07.2
+Airlight - V1.05.1- V1
+Filter Reduction - 0.8</t>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="12" shapeId="0" xr:uid="{FCC4E973-4106-4AC1-A598-C8AB62A595D0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.07.3
+Airlight - V1.05.1- V1
+Filter Reduction - 0.8</t>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="13" shapeId="0" xr:uid="{93EBB620-A219-4A52-BC3E-044462FB7776}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.07.1
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="14" shapeId="0" xr:uid="{BA14E670-3446-4794-8F7A-737043F69BF5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.07.2
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="15" shapeId="0" xr:uid="{D81608AE-052B-4752-BBC5-25B914B72E85}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.07.3
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="16" shapeId="0" xr:uid="{2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.06.4
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Neil Patrick  A. Del Gallego</author>
+  </authors>
+  <commentList>
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{75B324E0-4548-4529-BAB7-B3E2D92548E8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Best performance. They tried training NYU-depth and measured performance against i-Haze.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{46A1CEC9-A4B5-4783-918D-40173DA716D8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Domain Adaptation for Image Dehazing
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{93004584-1BDD-4568-B7AD-29E5716B6F68}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Learning to Dehaze From Realistic Scene with
+A Fast Physics-based Dehazing Network
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
   <si>
     <t>PSNR</t>
   </si>
@@ -331,16 +509,146 @@
   </si>
   <si>
     <t>Mix 10</t>
+  </si>
+  <si>
+    <t>V1.06.3</t>
+  </si>
+  <si>
+    <t>V1.06.4</t>
+  </si>
+  <si>
+    <t>V1.06.5</t>
+  </si>
+  <si>
+    <t>DCP</t>
+  </si>
+  <si>
+    <t>AOD-Net</t>
+  </si>
+  <si>
+    <t>Cycle-Dehaze</t>
+  </si>
+  <si>
+    <t>FFA-Net</t>
+  </si>
+  <si>
+    <t>GridDehazeNet</t>
+  </si>
+  <si>
+    <t>EDPN</t>
+  </si>
+  <si>
+    <t>AVC-DCP</t>
+  </si>
+  <si>
+    <t>iCycleGAN</t>
+  </si>
+  <si>
+    <t>PCFAN</t>
+  </si>
+  <si>
+    <t>15.00 &lt; X &lt; 17.00</t>
+  </si>
+  <si>
+    <t>0.4 &lt; X 0. 41</t>
+  </si>
+  <si>
+    <t>0.39 &lt; X &lt; 0.40</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ours</t>
+  </si>
+  <si>
+    <t>DeepPrior</t>
+  </si>
+  <si>
+    <t>DA-Dehaze</t>
+  </si>
+  <si>
+    <t>Physics-Dehaze</t>
+  </si>
+  <si>
+    <t>Model-Based/optimization approach</t>
+  </si>
+  <si>
+    <t>Unsupervised/Unpaired</t>
+  </si>
+  <si>
+    <t>Supervised/Paired</t>
+  </si>
+  <si>
+    <t>Training Data</t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>Mix 11</t>
+  </si>
+  <si>
+    <t>Mix 12</t>
+  </si>
+  <si>
+    <t>V1.07.1</t>
+  </si>
+  <si>
+    <t>V1.07.2</t>
+  </si>
+  <si>
+    <t>V1.07.3</t>
+  </si>
+  <si>
+    <t>NYU Indoor</t>
+  </si>
+  <si>
+    <t>Mix 13</t>
+  </si>
+  <si>
+    <t>I-HAZE + O-HAZE</t>
+  </si>
+  <si>
+    <t>RESIDE ITS + RESIDE OTS</t>
+  </si>
+  <si>
+    <t>I-HAZE</t>
+  </si>
+  <si>
+    <t>RESIDE (All)</t>
+  </si>
+  <si>
+    <t>3D Movies</t>
+  </si>
+  <si>
+    <t>Urban Virtual Environment</t>
+  </si>
+  <si>
+    <t>Average (related work)</t>
+  </si>
+  <si>
+    <t>Mix 14</t>
+  </si>
+  <si>
+    <t>Mix 15</t>
+  </si>
+  <si>
+    <t>Mix 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mix 17 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +669,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -389,20 +723,439 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="65">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -997,6 +1750,48 @@
 Airlight - V1.05.1- V1
 Filter Reduction - 0.8</text>
   </threadedComment>
+  <threadedComment ref="A17" dT="2021-06-15T02:34:01.02" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{1631D402-746A-4827-BF4C-839F3BA272C6}">
+    <text>Albedo - V1.04.1
+Transmission - V1.07.1
+Airlight - V1.05.1- V1
+Filter Reduction - 0.8</text>
+  </threadedComment>
+  <threadedComment ref="A18" dT="2021-06-15T02:34:01.02" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{907B7804-9C5A-4E10-B69A-D3A98603E98C}">
+    <text>Albedo - V1.04.1
+Transmission - V1.07.2
+Airlight - V1.05.1- V1
+Filter Reduction - 0.8</text>
+  </threadedComment>
+  <threadedComment ref="A19" dT="2021-06-15T02:34:01.02" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{FCC4E973-4106-4AC1-A598-C8AB62A595D0}">
+    <text>Albedo - V1.04.1
+Transmission - V1.07.3
+Airlight - V1.05.1- V1
+Filter Reduction - 0.8</text>
+  </threadedComment>
+  <threadedComment ref="A20" dT="2021-06-15T13:14:50.19" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{93EBB620-A219-4A52-BC3E-044462FB7776}">
+    <text>Albedo - V1.04.1
+Transmission - V1.07.1
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A21" dT="2021-06-15T13:59:59.08" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{BA14E670-3446-4794-8F7A-737043F69BF5}">
+    <text>Albedo - V1.04.1
+Transmission - V1.07.2
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A22" dT="2021-06-15T14:00:03.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{D81608AE-052B-4752-BBC5-25B914B72E85}">
+    <text>Albedo - V1.04.1
+Transmission - V1.07.3
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A23" dT="2021-06-15T14:14:23.51" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}">
+    <text>Albedo - V1.04.1
+Transmission - V1.06.4
+Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1004,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,27 +1816,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="9"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="5"/>
+      <c r="O1" s="9"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
@@ -1107,13 +1902,13 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>11.878299999999999</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>0.19220000000000001</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <v>0.61419999999999997</v>
       </c>
       <c r="K3" t="s">
@@ -1148,13 +1943,13 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>22.260269999999998</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>5.9899999999999997E-3</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="5">
         <v>0.79791999999999996</v>
       </c>
       <c r="K4" t="s">
@@ -1189,13 +1984,13 @@
       <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>20.749400000000001</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>8.5100000000000002E-3</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>0.82787999999999995</v>
       </c>
       <c r="K5" t="s">
@@ -1227,13 +2022,13 @@
       <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="6">
         <v>21.47146</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="6">
         <v>7.2199999999999999E-3</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="6">
         <v>0.84968999999999995</v>
       </c>
       <c r="K6" t="s">
@@ -1265,13 +2060,13 @@
       <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="6">
         <v>25.76465</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="6">
         <v>2.6900000000000001E-3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="6">
         <v>0.91974</v>
       </c>
       <c r="K7" t="s">
@@ -1303,13 +2098,13 @@
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="6">
         <v>33.608440000000002</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="6">
         <v>4.4999999999999999E-4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="6">
         <v>0.97160000000000002</v>
       </c>
       <c r="K8" t="s">
@@ -1326,13 +2121,13 @@
       <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="6">
         <v>29.921849999999999</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="6">
         <v>1.0399999999999999E-3</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="6">
         <v>0.95730000000000004</v>
       </c>
       <c r="K9" t="s">
@@ -1364,13 +2159,13 @@
       <c r="F10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="6">
         <v>32.728729999999999</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="6">
         <v>5.5000000000000003E-4</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="6">
         <v>0.96704999999999997</v>
       </c>
     </row>
@@ -1390,13 +2185,13 @@
       <c r="F11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="6">
         <v>29.98086</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="6">
         <v>1.0200000000000001E-3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="6">
         <v>0.93915999999999999</v>
       </c>
     </row>
@@ -1416,13 +2211,13 @@
       <c r="F12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="6">
         <v>29.826049999999999</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="6">
         <v>1.06E-3</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="6">
         <v>0.93645</v>
       </c>
     </row>
@@ -1439,6 +2234,9 @@
       <c r="D13">
         <v>0.81723999999999997</v>
       </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1456,13 +2254,13 @@
       <c r="F14" t="s">
         <v>35</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
         <v>25.70628</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>1.329E-2</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <v>0.88024000000000002</v>
       </c>
     </row>
@@ -1479,24 +2277,124 @@
       <c r="D15">
         <v>0.752</v>
       </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>36</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="5">
         <v>20.87011</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <v>2.2630000000000001E-2</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="5">
         <v>0.87870000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="5">
+        <v>23.779900000000001</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1.9210000000000001E-2</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0.85977999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="5">
+        <v>24.08257</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1.6990000000000002E-2</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0.90881000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="5">
+        <v>24.216670000000001</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1.8710000000000001E-2</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0.90439999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25">
+        <v>22.329409999999999</v>
+      </c>
+      <c r="H25">
+        <v>2.581E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.80874999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26">
+        <v>23.66535</v>
+      </c>
+      <c r="H26">
+        <v>1.9890000000000001E-2</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.84340000000000004</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27">
+        <v>22.58784</v>
+      </c>
+      <c r="H27">
+        <v>2.2710000000000001E-2</v>
+      </c>
+      <c r="I27">
+        <v>0.84702</v>
       </c>
     </row>
   </sheetData>
@@ -1508,28 +2406,37 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="23" priority="12" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="48" priority="15" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="22" priority="11" percent="1" bottom="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="21" priority="10" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="20" priority="9" percent="1" bottom="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="19" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="47" priority="14" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I19 I21:I1048576">
+    <cfRule type="top10" dxfId="46" priority="13" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H19 H21:H1048576">
+    <cfRule type="top10" dxfId="45" priority="12" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G19 G21:G1048576">
+    <cfRule type="top10" dxfId="44" priority="11" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="18" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="43" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="17" priority="6" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="9" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="16" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="41" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19:G31">
+    <cfRule type="top10" dxfId="40" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:H32">
+    <cfRule type="top10" dxfId="39" priority="2" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19:I32">
+    <cfRule type="top10" dxfId="38" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1539,10 +2446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E4D2B0-246F-48C3-B870-33165E2ABBB9}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F23" sqref="B23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,22 +2466,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1801,6 +2708,137 @@
       </c>
       <c r="I16">
         <v>0.95584999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17">
+        <v>15.003579999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.84104999999999996</v>
+      </c>
+      <c r="E17">
+        <v>16.212589999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.88575999999999999</v>
+      </c>
+      <c r="H17">
+        <v>21.07751</v>
+      </c>
+      <c r="I17">
+        <v>0.95701999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18">
+        <v>15.06118</v>
+      </c>
+      <c r="C18">
+        <v>0.84123999999999999</v>
+      </c>
+      <c r="E18">
+        <v>16.1281</v>
+      </c>
+      <c r="F18">
+        <v>0.88378000000000001</v>
+      </c>
+      <c r="H18">
+        <v>21.08567</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.95660000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19">
+        <v>15.018269999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.84130000000000005</v>
+      </c>
+      <c r="E19">
+        <v>16.219280000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.88595000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20">
+        <v>14.519769999999999</v>
+      </c>
+      <c r="C20">
+        <v>0.82887999999999995</v>
+      </c>
+      <c r="E20">
+        <v>15.407299999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.87216000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="3">
+        <v>14.2448</v>
+      </c>
+      <c r="C21">
+        <v>0.82067000000000001</v>
+      </c>
+      <c r="E21" s="3">
+        <v>14.220700000000001</v>
+      </c>
+      <c r="F21">
+        <v>0.84714999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22">
+        <v>14.334070000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.82484999999999997</v>
+      </c>
+      <c r="E22">
+        <v>15.11833</v>
+      </c>
+      <c r="F22">
+        <v>0.86584000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23">
+        <v>14.561640000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.83301999999999998</v>
+      </c>
+      <c r="E23">
+        <v>15.308960000000001</v>
+      </c>
+      <c r="F23">
+        <v>0.87485999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -1810,55 +2848,580 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="K1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="13" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="12" priority="13" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B20">
-    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C20">
-    <cfRule type="top10" dxfId="8" priority="9" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E20">
-    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11:F19">
-    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="18" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22 B11:B18">
+    <cfRule type="top10" dxfId="34" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H19">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="11" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I19">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K15">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:L15">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B19 B21:B32">
+    <cfRule type="top10" dxfId="27" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E19 E21:E1048576">
+    <cfRule type="top10" dxfId="26" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F19 F21:F1048576">
+    <cfRule type="top10" dxfId="25" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C19 C21:C1048576">
+    <cfRule type="top10" dxfId="24" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="6" width="15" customWidth="1"/>
+    <col min="8" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="5">
+        <v>13.48476</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.80076000000000003</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>13.25198</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5">
+        <v>15.690049999999999</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.90192000000000005</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="5">
+        <v>24.71</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.89170000000000005</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="5">
+        <v>14.45778</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.79003000000000001</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5">
+        <v>14.733599999999999</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.86065999999999998</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5">
+        <v>20.638760000000001</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.94225000000000003</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="10">
+        <v>20.130600000000001</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.77390000000000003</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="10">
+        <v>16.80341</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.83260999999999996</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
+        <v>11.688040000000001</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.81701999999999997</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="5">
+        <v>18.2179</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.85409999999999997</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5">
+        <v>15.921799999999999</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.74519999999999997</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5">
+        <v>22.065799999999999</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.91469999999999996</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="5">
+        <v>13.980880000000001</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.80913000000000002</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5">
+        <v>13.07117</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.83233999999999997</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5">
+        <v>20.32086</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.93916999999999995</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="5">
+        <v>12.759320000000001</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.78044000000000002</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5">
+        <v>12.753729999999999</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.82584000000000002</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
+        <v>20.321269999999998</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.94330999999999998</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="5">
+        <v>16.487590000000001</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.81867999999999996</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
+        <v>15.15972</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.86604000000000003</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5">
+        <v>20.150410000000001</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.91915999999999998</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5">
+        <v>24.01</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="5">
+        <v>27.76</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.9284</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="10">
+        <v>30.33</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0.94730000000000003</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="5">
+        <v>14.561640000000001</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.83301999999999998</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5">
+        <v>15.308960000000001</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.87485999999999997</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
+        <v>21.335280000000001</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.95531999999999995</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="5">
+        <f>AVERAGE(B3,B6:B11)</f>
+        <v>15.645547142857144</v>
+      </c>
+      <c r="C16" s="5">
+        <f>AVERAGE(C3,C6:C11)</f>
+        <v>0.8038628571428571</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
+        <f t="shared" ref="D16:I16" si="0">AVERAGE(E3,E6:E11)</f>
+        <v>14.527915714285715</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.8314557142857143</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
+        <f>AVERAGE(H3,H5:H11)</f>
+        <v>19.448148749999998</v>
+      </c>
+      <c r="I16" s="5">
+        <f>AVERAGE(I3,I5:I11)</f>
+        <v>0.90865375000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="top10" dxfId="23" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="top10" dxfId="22" priority="12" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="top10" dxfId="21" priority="11" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="top10" dxfId="20" priority="10" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="top10" dxfId="19" priority="9" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="top10" dxfId="18" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:H15 H21:H1048576 H1:H12">
+    <cfRule type="top10" dxfId="17" priority="62" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15 B2:B4 B6:B13">
+    <cfRule type="top10" dxfId="16" priority="73" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C4 C15 C21:C1048576 C6:C13">
+    <cfRule type="top10" dxfId="15" priority="80" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E4 E15 E21:E1048576 E6:E13">
+    <cfRule type="top10" dxfId="14" priority="86" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F4 F15 F21:F1048576 F6:F13">
+    <cfRule type="top10" dxfId="13" priority="92" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21:I1048576 I1:I15">
+    <cfRule type="top10" dxfId="12" priority="96" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixed and optimization
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D02395-2E36-49AE-8ECF-5FBE1A849FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDF29B0-641A-408C-894F-BB2AB2DB9C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41340" yWindow="2460" windowWidth="33060" windowHeight="15435" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,6 +93,7 @@
     <author>tc={BA14E670-3446-4794-8F7A-737043F69BF5}</author>
     <author>tc={D81608AE-052B-4752-BBC5-25B914B72E85}</author>
     <author>tc={2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}</author>
+    <author>tc={0565FFCA-9B79-4E45-A917-937AF9B4A186}</author>
   </authors>
   <commentList>
     <comment ref="A3" authorId="0" shapeId="0" xr:uid="{E82EA847-54E7-4608-A448-8D64BCF97254}">
@@ -234,7 +235,7 @@
 Filter Reduction - 0.8</t>
       </text>
     </comment>
-    <comment ref="A20" authorId="13" shapeId="0" xr:uid="{93EBB620-A219-4A52-BC3E-044462FB7776}">
+    <comment ref="A24" authorId="13" shapeId="0" xr:uid="{93EBB620-A219-4A52-BC3E-044462FB7776}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -245,7 +246,7 @@
 Filter Reduction -N/A - DIRECT</t>
       </text>
     </comment>
-    <comment ref="A21" authorId="14" shapeId="0" xr:uid="{BA14E670-3446-4794-8F7A-737043F69BF5}">
+    <comment ref="A25" authorId="14" shapeId="0" xr:uid="{BA14E670-3446-4794-8F7A-737043F69BF5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -256,7 +257,7 @@
 Filter Reduction -N/A - DIRECT</t>
       </text>
     </comment>
-    <comment ref="A22" authorId="15" shapeId="0" xr:uid="{D81608AE-052B-4752-BBC5-25B914B72E85}">
+    <comment ref="A26" authorId="15" shapeId="0" xr:uid="{D81608AE-052B-4752-BBC5-25B914B72E85}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -267,7 +268,7 @@
 Filter Reduction -N/A - DIRECT</t>
       </text>
     </comment>
-    <comment ref="A23" authorId="16" shapeId="0" xr:uid="{2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}">
+    <comment ref="A27" authorId="16" shapeId="0" xr:uid="{2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -275,6 +276,17 @@
     Albedo - V1.04.1
 Transmission - V1.06.4
 Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="17" shapeId="0" xr:uid="{0565FFCA-9B79-4E45-A917-937AF9B4A186}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission - V1.08.1
+Airlight - V1.06.1- V1
 Filter Reduction -N/A - DIRECT</t>
       </text>
     </comment>
@@ -368,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>PSNR</t>
   </si>
@@ -638,6 +650,27 @@
   </si>
   <si>
     <t xml:space="preserve">Mix 17 </t>
+  </si>
+  <si>
+    <t>V1.07.4</t>
+  </si>
+  <si>
+    <t>DIRECT</t>
+  </si>
+  <si>
+    <t>Mix 18</t>
+  </si>
+  <si>
+    <t>Mix 19</t>
+  </si>
+  <si>
+    <t>Mix 20</t>
+  </si>
+  <si>
+    <t>V1.08.1</t>
+  </si>
+  <si>
+    <t>Atmospheric Map Generator</t>
   </si>
 </sst>
 </file>
@@ -737,235 +770,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="43">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1768,28 +1581,34 @@
 Airlight - V1.05.1- V1
 Filter Reduction - 0.8</text>
   </threadedComment>
-  <threadedComment ref="A20" dT="2021-06-15T13:14:50.19" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{93EBB620-A219-4A52-BC3E-044462FB7776}">
+  <threadedComment ref="A24" dT="2021-06-15T13:14:50.19" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{93EBB620-A219-4A52-BC3E-044462FB7776}">
     <text>Albedo - V1.04.1
 Transmission - V1.07.1
 Airlight - V1.05.1- V1
 Filter Reduction -N/A - DIRECT</text>
   </threadedComment>
-  <threadedComment ref="A21" dT="2021-06-15T13:59:59.08" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{BA14E670-3446-4794-8F7A-737043F69BF5}">
+  <threadedComment ref="A25" dT="2021-06-15T13:59:59.08" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{BA14E670-3446-4794-8F7A-737043F69BF5}">
     <text>Albedo - V1.04.1
 Transmission - V1.07.2
 Airlight - V1.05.1- V1
 Filter Reduction -N/A - DIRECT</text>
   </threadedComment>
-  <threadedComment ref="A22" dT="2021-06-15T14:00:03.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{D81608AE-052B-4752-BBC5-25B914B72E85}">
+  <threadedComment ref="A26" dT="2021-06-15T14:00:03.33" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{D81608AE-052B-4752-BBC5-25B914B72E85}">
     <text>Albedo - V1.04.1
 Transmission - V1.07.3
 Airlight - V1.05.1- V1
 Filter Reduction -N/A - DIRECT</text>
   </threadedComment>
-  <threadedComment ref="A23" dT="2021-06-15T14:14:23.51" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}">
+  <threadedComment ref="A27" dT="2021-06-15T14:14:23.51" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}">
     <text>Albedo - V1.04.1
 Transmission - V1.06.4
 Airlight - V1.05.1- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A28" dT="2021-06-18T10:11:52.04" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{0565FFCA-9B79-4E45-A917-937AF9B4A186}">
+    <text>Albedo - V1.04.1
+Transmission - V1.08.1
+Airlight - V1.06.1- V1
 Filter Reduction -N/A - DIRECT</text>
   </threadedComment>
 </ThreadedComments>
@@ -1797,10 +1616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,35 +1634,41 @@
     <col min="23" max="24" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="9"/>
+      <c r="O1" s="10"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1885,8 +1710,20 @@
         <v>9</v>
       </c>
       <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1926,8 +1763,11 @@
       <c r="Q3">
         <v>2.8829400000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1968,7 +1808,7 @@
         <v>4.0149999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2006,7 +1846,7 @@
         <v>1.468E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2044,7 +1884,7 @@
         <v>1.436E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2082,7 +1922,7 @@
         <v>1.728E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2114,7 +1954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2143,7 +1983,7 @@
         <v>1.6289999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2168,8 +2008,20 @@
       <c r="I10" s="6">
         <v>0.96704999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="3">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10">
+        <v>1.059E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2195,7 +2047,7 @@
         <v>0.93915999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2221,7 +2073,7 @@
         <v>0.93645</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2238,7 +2090,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2264,7 +2116,7 @@
         <v>0.88024000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2133,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -2397,46 +2249,93 @@
         <v>0.84702</v>
       </c>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28">
+        <v>22.715630000000001</v>
+      </c>
+      <c r="H28">
+        <v>2.2780000000000002E-2</v>
+      </c>
+      <c r="I28">
+        <v>0.88112999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29">
+        <v>22.226849999999999</v>
+      </c>
+      <c r="H29">
+        <v>9.4199999999999996E-3</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.8821</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="S1:V1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="48" priority="15" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="47" priority="14" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="41" priority="20" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="46" priority="13" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="40" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="45" priority="12" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="39" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="44" priority="11" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="38" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="43" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="16" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="42" priority="9" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="15" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="41" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="14" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="40" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="39" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="38" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2446,10 +2345,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E4D2B0-246F-48C3-B870-33165E2ABBB9}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="B23:F23"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,22 +2365,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="I1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2772,73 +2671,117 @@
       <c r="F19">
         <v>0.88595000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20">
-        <v>14.519769999999999</v>
-      </c>
-      <c r="C20">
-        <v>0.82887999999999995</v>
-      </c>
-      <c r="E20">
-        <v>15.407299999999999</v>
-      </c>
-      <c r="F20">
-        <v>0.87216000000000005</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="3">
-        <v>14.2448</v>
-      </c>
-      <c r="C21">
-        <v>0.82067000000000001</v>
-      </c>
-      <c r="E21" s="3">
-        <v>14.220700000000001</v>
-      </c>
-      <c r="F21">
-        <v>0.84714999999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22">
-        <v>14.334070000000001</v>
-      </c>
-      <c r="C22">
-        <v>0.82484999999999997</v>
-      </c>
-      <c r="E22">
-        <v>15.11833</v>
-      </c>
-      <c r="F22">
-        <v>0.86584000000000005</v>
+      <c r="H19">
+        <v>21.000109999999999</v>
+      </c>
+      <c r="I19">
+        <v>0.95657000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24">
+        <v>14.519769999999999</v>
+      </c>
+      <c r="C24">
+        <v>0.82887999999999995</v>
+      </c>
+      <c r="E24">
+        <v>15.407299999999999</v>
+      </c>
+      <c r="F24">
+        <v>0.87216000000000005</v>
+      </c>
+      <c r="H24">
+        <v>20.320869999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.95033999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="3">
+        <v>14.2448</v>
+      </c>
+      <c r="C25">
+        <v>0.82067000000000001</v>
+      </c>
+      <c r="E25" s="3">
+        <v>14.220700000000001</v>
+      </c>
+      <c r="F25">
+        <v>0.84714999999999996</v>
+      </c>
+      <c r="H25">
+        <v>19.64358</v>
+      </c>
+      <c r="I25">
+        <v>0.93786000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26">
+        <v>14.334070000000001</v>
+      </c>
+      <c r="C26">
+        <v>0.82484999999999997</v>
+      </c>
+      <c r="E26">
+        <v>15.522019999999999</v>
+      </c>
+      <c r="F26">
+        <v>0.87358000000000002</v>
+      </c>
+      <c r="H26">
+        <v>18.918559999999999</v>
+      </c>
+      <c r="I26">
+        <v>0.94703000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>89</v>
       </c>
-      <c r="B23">
+      <c r="B27">
         <v>14.561640000000001</v>
       </c>
-      <c r="C23">
+      <c r="C27">
         <v>0.83301999999999998</v>
       </c>
-      <c r="E23">
+      <c r="E27">
         <v>15.308960000000001</v>
       </c>
-      <c r="F23">
+      <c r="F27">
         <v>0.87485999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2850,46 +2793,46 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="37" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="36" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="35" priority="18" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22 B11:B18">
-    <cfRule type="top10" dxfId="34" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="18" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26 B11:B18">
+    <cfRule type="top10" dxfId="28" priority="15" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="top10" dxfId="27" priority="9" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="top10" dxfId="26" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11:K15">
+    <cfRule type="top10" dxfId="25" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11:L15">
+    <cfRule type="top10" dxfId="24" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H19">
-    <cfRule type="top10" dxfId="33" priority="11" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="98" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I19">
-    <cfRule type="top10" dxfId="32" priority="10" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="top10" dxfId="31" priority="9" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2">
-    <cfRule type="top10" dxfId="30" priority="8" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11:K15">
-    <cfRule type="top10" dxfId="29" priority="7" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L11:L15">
-    <cfRule type="top10" dxfId="28" priority="6" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B19 B21:B32">
-    <cfRule type="top10" dxfId="27" priority="5" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E19 E21:E1048576">
-    <cfRule type="top10" dxfId="26" priority="3" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F19 F21:F1048576">
-    <cfRule type="top10" dxfId="25" priority="2" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C19 C21:C1048576">
-    <cfRule type="top10" dxfId="24" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="100" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B19 B29:B32 B25:B27">
+    <cfRule type="top10" dxfId="21" priority="116" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E19 E29:E1048576 E25:E27">
+    <cfRule type="top10" dxfId="20" priority="120" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F19 F29:F1048576 F25:F27">
+    <cfRule type="top10" dxfId="19" priority="124" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C19 C29:C1048576 C25:C27">
+    <cfRule type="top10" dxfId="18" priority="128" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2900,8 +2843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="B15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3080,14 +3023,14 @@
       <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>20.130600000000001</v>
       </c>
       <c r="C7" s="5">
         <v>0.77390000000000003</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>16.80341</v>
       </c>
       <c r="F7" s="5">
@@ -3114,7 +3057,7 @@
       <c r="B8" s="5">
         <v>18.2179</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>0.85409999999999997</v>
       </c>
       <c r="D8" s="5"/>
@@ -3307,7 +3250,7 @@
       <c r="F14" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>30.33</v>
       </c>
       <c r="I14" s="5">
@@ -3325,23 +3268,23 @@
         <v>63</v>
       </c>
       <c r="B15" s="5">
-        <v>14.561640000000001</v>
+        <v>14.519769999999999</v>
       </c>
       <c r="C15" s="5">
-        <v>0.83301999999999998</v>
+        <v>0.82887999999999995</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5">
-        <v>15.308960000000001</v>
-      </c>
-      <c r="F15" s="10">
-        <v>0.87485999999999997</v>
+        <v>15.407299999999999</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0.87216000000000005</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
         <v>21.335280000000001</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="9">
         <v>0.95531999999999995</v>
       </c>
       <c r="J15" s="8" t="s">
@@ -3365,7 +3308,7 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5">
-        <f t="shared" ref="D16:I16" si="0">AVERAGE(E3,E6:E11)</f>
+        <f t="shared" ref="E16:F16" si="0">AVERAGE(E3,E6:E11)</f>
         <v>14.527915714285715</v>
       </c>
       <c r="F16" s="5">
@@ -3385,40 +3328,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="23" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="22" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="21" priority="11" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="11" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="20" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="19" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="18" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H15 H21:H1048576 H1:H12">
-    <cfRule type="top10" dxfId="17" priority="62" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="62" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 B2:B4 B6:B13">
-    <cfRule type="top10" dxfId="16" priority="73" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="73" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C4 C15 C21:C1048576 C6:C13">
-    <cfRule type="top10" dxfId="15" priority="80" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="80" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E4 E15 E21:E1048576 E6:E13">
-    <cfRule type="top10" dxfId="14" priority="86" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="86" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F4 F15 F21:F1048576 F6:F13">
-    <cfRule type="top10" dxfId="13" priority="92" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="92" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:I1048576 I1:I15">
-    <cfRule type="top10" dxfId="12" priority="96" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="96" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Checkpoint for airlight gen map.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDF29B0-641A-408C-894F-BB2AB2DB9C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70920893-A683-4FAE-808E-3CCB00FEA554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -778,7 +778,577 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1619,7 +2189,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,6 +2201,7 @@
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" customWidth="1"/>
     <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" customWidth="1"/>
     <col min="23" max="24" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1765,6 +2336,15 @@
       </c>
       <c r="S3" t="s">
         <v>15</v>
+      </c>
+      <c r="T3">
+        <v>20.669039999999999</v>
+      </c>
+      <c r="U3">
+        <v>2.998E-2</v>
+      </c>
+      <c r="V3">
+        <v>0.79024000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -2287,54 +2867,63 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="42" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="38" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="41" priority="20" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="40" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="39" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="38" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="37" priority="16" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="36" priority="15" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="35" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="34" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="33" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="32" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
+    <cfRule type="top10" dxfId="22" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:T1048576">
+    <cfRule type="top10" dxfId="21" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U1048576">
+    <cfRule type="top10" dxfId="20" priority="2" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:V1048576">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2793,46 +3382,46 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="31" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="99" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="30" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="98" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="29" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="97" priority="18" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26 B11:B18">
-    <cfRule type="top10" dxfId="28" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="96" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="top10" dxfId="27" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="95" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="top10" dxfId="26" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="94" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K15">
-    <cfRule type="top10" dxfId="25" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="93" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:L15">
-    <cfRule type="top10" dxfId="24" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="92" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H19">
-    <cfRule type="top10" dxfId="23" priority="98" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="91" priority="98" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I19">
-    <cfRule type="top10" dxfId="22" priority="100" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="90" priority="100" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B19 B29:B32 B25:B27">
-    <cfRule type="top10" dxfId="21" priority="116" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="89" priority="116" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E19 E29:E1048576 E25:E27">
-    <cfRule type="top10" dxfId="20" priority="120" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="88" priority="120" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F19 F29:F1048576 F25:F27">
-    <cfRule type="top10" dxfId="19" priority="124" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="87" priority="124" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C19 C29:C1048576 C25:C27">
-    <cfRule type="top10" dxfId="18" priority="128" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="86" priority="128" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3328,40 +3917,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="17" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="85" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="16" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="84" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="15" priority="11" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="83" priority="11" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="14" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="82" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="13" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="81" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="12" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="80" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H15 H21:H1048576 H1:H12">
-    <cfRule type="top10" dxfId="11" priority="62" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="79" priority="62" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 B2:B4 B6:B13">
-    <cfRule type="top10" dxfId="10" priority="73" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="78" priority="73" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C4 C15 C21:C1048576 C6:C13">
-    <cfRule type="top10" dxfId="9" priority="80" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="77" priority="80" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E4 E15 E21:E1048576 E6:E13">
-    <cfRule type="top10" dxfId="8" priority="86" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="76" priority="86" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F4 F15 F21:F1048576 F6:F13">
-    <cfRule type="top10" dxfId="7" priority="92" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="75" priority="92" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:I1048576 I1:I15">
-    <cfRule type="top10" dxfId="6" priority="96" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="74" priority="96" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to make code compatible with CCS server as well.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70920893-A683-4FAE-808E-3CCB00FEA554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66864A80-336E-4E89-8878-2CAB366FB8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41475" yWindow="1200" windowWidth="31140" windowHeight="18765" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,6 +94,11 @@
     <author>tc={D81608AE-052B-4752-BBC5-25B914B72E85}</author>
     <author>tc={2226094B-B7F4-41F1-BC4D-7F5CD120A7F9}</author>
     <author>tc={0565FFCA-9B79-4E45-A917-937AF9B4A186}</author>
+    <author>tc={A9A7CD2B-5913-4CEC-AE6E-248336989EBD}</author>
+    <author>tc={5C7C14C7-91F1-4A87-8314-79E41E5DC914}</author>
+    <author>tc={655DBA17-7BE4-40D2-AD9B-06B528D8B78F}</author>
+    <author>tc={797832C7-B45D-4A83-A3D7-8C968C4EACD4}</author>
+    <author>tc={A9549F78-4440-4381-B2CB-3CC21B8E821E}</author>
   </authors>
   <commentList>
     <comment ref="A3" authorId="0" shapeId="0" xr:uid="{E82EA847-54E7-4608-A448-8D64BCF97254}">
@@ -285,8 +290,63 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Albedo - V1.04.1
-Transmission - V1.08.1
-Airlight - V1.06.1- V1
+Transmission -Dehazer  V2.02.1
+Airlight - Dehazer V2.02.1- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="18" shapeId="0" xr:uid="{A9A7CD2B-5913-4CEC-AE6E-248336989EBD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission -Dehazer  V2.03.2
+Airlight - Dehazer V2.03.2- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="19" shapeId="0" xr:uid="{5C7C14C7-91F1-4A87-8314-79E41E5DC914}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission -Dehazer  V2.03.3
+Airlight - Dehazer V2.03.3- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="20" shapeId="0" xr:uid="{655DBA17-7BE4-40D2-AD9B-06B528D8B78F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission -Dehazer  V2.02.3
+Airlight - Dehazer V2.02.3- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="21" shapeId="0" xr:uid="{797832C7-B45D-4A83-A3D7-8C968C4EACD4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission -Dehazer  V2.02.4
+Airlight - Dehazer V2.02.4- V1
+Filter Reduction -N/A - DIRECT</t>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="22" shapeId="0" xr:uid="{A9549F78-4440-4381-B2CB-3CC21B8E821E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Albedo - V1.04.1
+Transmission -Dehazer  V2.02.5
+Airlight - Dehazer V2.02.5- V1
 Filter Reduction -N/A - DIRECT</t>
       </text>
     </comment>
@@ -300,6 +360,30 @@
     <author>Neil Patrick  A. Del Gallego</author>
   </authors>
   <commentList>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{B8FEB020-08E7-48AB-9FC5-5D94EBF7E06B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Aod-net: All-in-one dehazing network</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K7" authorId="0" shapeId="0" xr:uid="{75B324E0-4548-4529-BAB7-B3E2D92548E8}">
       <text>
         <r>
@@ -321,6 +405,102 @@
           </rPr>
           <t xml:space="preserve">
 Best performance. They tried training NYU-depth and measured performance against i-Haze.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{EB12C098-206A-4BF3-AD79-D44EAB9839E5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+FFA-Net: Feature fusion attention network for single image dehazing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{8BC64385-DC3F-4DFA-B521-DB08FCB87180}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Attention-Based Multi-Scale Network for Image Dehazing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{0F558C0D-1355-42FE-B50F-F830B2AA61AC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enhanced Pix2pix Dehazing Network</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{A39CBFF1-AA98-466B-AF97-CEA2E7911F2F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pyramid channel-based feature attention network for image dehazing</t>
         </r>
       </text>
     </comment>
@@ -380,7 +560,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
   <si>
     <t>PSNR</t>
   </si>
@@ -547,9 +727,6 @@
     <t>GridDehazeNet</t>
   </si>
   <si>
-    <t>EDPN</t>
-  </si>
-  <si>
     <t>AVC-DCP</t>
   </si>
   <si>
@@ -671,6 +848,18 @@
   </si>
   <si>
     <t>Atmospheric Map Generator</t>
+  </si>
+  <si>
+    <t>Mix 21</t>
+  </si>
+  <si>
+    <t>Mix 22</t>
+  </si>
+  <si>
+    <t>Mix 23</t>
+  </si>
+  <si>
+    <t>EPDN</t>
   </si>
 </sst>
 </file>
@@ -778,547 +967,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="100">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2177,8 +1826,38 @@
   </threadedComment>
   <threadedComment ref="A28" dT="2021-06-18T10:11:52.04" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{0565FFCA-9B79-4E45-A917-937AF9B4A186}">
     <text>Albedo - V1.04.1
-Transmission - V1.08.1
-Airlight - V1.06.1- V1
+Transmission -Dehazer  V2.02.1
+Airlight - Dehazer V2.02.1- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A29" dT="2021-07-07T08:08:24.83" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{A9A7CD2B-5913-4CEC-AE6E-248336989EBD}">
+    <text>Albedo - V1.04.1
+Transmission -Dehazer  V2.03.2
+Airlight - Dehazer V2.03.2- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A30" dT="2021-07-07T08:08:40.38" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{5C7C14C7-91F1-4A87-8314-79E41E5DC914}">
+    <text>Albedo - V1.04.1
+Transmission -Dehazer  V2.03.3
+Airlight - Dehazer V2.03.3- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A31" dT="2021-07-07T08:08:53.21" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{655DBA17-7BE4-40D2-AD9B-06B528D8B78F}">
+    <text>Albedo - V1.04.1
+Transmission -Dehazer  V2.02.3
+Airlight - Dehazer V2.02.3- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A32" dT="2021-07-07T08:09:00.95" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{797832C7-B45D-4A83-A3D7-8C968C4EACD4}">
+    <text>Albedo - V1.04.1
+Transmission -Dehazer  V2.02.4
+Airlight - Dehazer V2.02.4- V1
+Filter Reduction -N/A - DIRECT</text>
+  </threadedComment>
+  <threadedComment ref="A33" dT="2021-07-07T08:09:10.31" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{A9549F78-4440-4381-B2CB-3CC21B8E821E}">
+    <text>Albedo - V1.04.1
+Transmission -Dehazer  V2.02.5
+Airlight - Dehazer V2.02.5- V1
 Filter Reduction -N/A - DIRECT</text>
   </threadedComment>
 </ThreadedComments>
@@ -2188,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +1912,7 @@
       </c>
       <c r="R1" s="2"/>
       <c r="S1" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T1" s="10"/>
       <c r="U1" s="10"/>
@@ -2786,7 +2465,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25">
         <v>22.329409999999999</v>
@@ -2800,7 +2479,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G26">
         <v>23.66535</v>
@@ -2817,7 +2496,7 @@
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G27">
         <v>22.58784</v>
@@ -2831,7 +2510,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28">
         <v>22.715630000000001</v>
@@ -2845,7 +2524,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29">
         <v>22.226849999999999</v>
@@ -2867,64 +2546,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="38" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="45" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="37" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="44" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="36" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="43" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="35" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="34" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="41" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="33" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="40" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="32" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="39" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="31" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="38" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="30" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="29" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="28" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="27" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="26" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="25" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="24" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="23" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="22" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="21" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="20" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2934,10 +2613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E4D2B0-246F-48C3-B870-33165E2ABBB9}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,7 +2879,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17">
         <v>15.003579999999999</v>
@@ -3223,7 +2902,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18">
         <v>15.06118</v>
@@ -3246,7 +2925,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19">
         <v>15.018269999999999</v>
@@ -3269,12 +2948,12 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24">
         <v>14.519769999999999</v>
@@ -3297,7 +2976,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="3">
         <v>14.2448</v>
@@ -3320,7 +2999,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26">
         <v>14.334070000000001</v>
@@ -3343,7 +3022,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27">
         <v>14.561640000000001</v>
@@ -3360,17 +3039,50 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="B28">
+        <v>13.951309999999999</v>
+      </c>
+      <c r="C28">
+        <v>0.82604999999999995</v>
+      </c>
+      <c r="E28">
+        <v>14.573869999999999</v>
+      </c>
+      <c r="F28">
+        <v>0.85013000000000005</v>
+      </c>
+      <c r="H28">
+        <v>19.027850000000001</v>
+      </c>
+      <c r="I28">
+        <v>0.93942000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3382,46 +3094,46 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="99" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="98" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="97" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="18" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26 B11:B18">
-    <cfRule type="top10" dxfId="96" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="15" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="top10" dxfId="95" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="top10" dxfId="94" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K15">
-    <cfRule type="top10" dxfId="93" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:L15">
-    <cfRule type="top10" dxfId="92" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H19">
-    <cfRule type="top10" dxfId="91" priority="98" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="98" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I19">
-    <cfRule type="top10" dxfId="90" priority="100" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="100" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B19 B29:B32 B25:B27">
-    <cfRule type="top10" dxfId="89" priority="116" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="116" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E19 E29:E1048576 E25:E27">
-    <cfRule type="top10" dxfId="88" priority="120" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="120" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F19 F29:F1048576 F25:F27">
-    <cfRule type="top10" dxfId="87" priority="124" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="124" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C19 C29:C1048576 C25:C27">
-    <cfRule type="top10" dxfId="86" priority="128" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="128" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3432,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="B15:F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,10 +3172,10 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3511,58 +3223,58 @@
         <v>0.90192000000000005</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="5">
         <v>24.71</v>
@@ -3571,10 +3283,10 @@
         <v>0.89170000000000005</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3602,10 +3314,10 @@
         <v>0.94225000000000003</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3633,15 +3345,15 @@
         <v>0.81701999999999997</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="5">
         <v>18.2179</v>
@@ -3664,10 +3376,10 @@
         <v>0.91469999999999996</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3695,10 +3407,10 @@
         <v>0.93916999999999995</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3726,15 +3438,15 @@
         <v>0.94330999999999998</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B11" s="5">
         <v>16.487590000000001</v>
@@ -3757,28 +3469,28 @@
         <v>0.91915999999999998</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
@@ -3788,27 +3500,27 @@
         <v>0.93500000000000005</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" s="5">
         <v>27.76</v>
@@ -3817,27 +3529,27 @@
         <v>0.9284</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="9">
         <v>30.33</v>
@@ -3846,15 +3558,15 @@
         <v>0.94730000000000003</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5">
         <v>14.519769999999999</v>
@@ -3877,15 +3589,15 @@
         <v>0.95531999999999995</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="5">
         <f>AVERAGE(B3,B6:B11)</f>
@@ -3917,40 +3629,40 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="85" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="84" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="83" priority="11" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="11" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="82" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="81" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="80" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H15 H21:H1048576 H1:H12">
-    <cfRule type="top10" dxfId="79" priority="62" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="62" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 B2:B4 B6:B13">
-    <cfRule type="top10" dxfId="78" priority="73" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="73" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C4 C15 C21:C1048576 C6:C13">
-    <cfRule type="top10" dxfId="77" priority="80" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="80" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E4 E15 E21:E1048576 E6:E13">
-    <cfRule type="top10" dxfId="76" priority="86" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="86" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F4 F15 F21:F1048576 F6:F13">
-    <cfRule type="top10" dxfId="75" priority="92" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="92" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:I1048576 I1:I15">
-    <cfRule type="top10" dxfId="74" priority="96" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="96" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Latest checkpoint of network
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66864A80-336E-4E89-8878-2CAB366FB8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03C0122-80F2-4CAD-B49E-8BD9C24BAB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41475" yWindow="1200" windowWidth="31140" windowHeight="18765" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38880" yWindow="1065" windowWidth="31140" windowHeight="18765" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -945,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -963,11 +963,1923 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="237">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2546,64 +4458,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="45" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="236" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="44" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="235" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="43" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="234" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="42" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="233" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="41" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="232" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="40" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="231" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="39" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="230" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="38" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="229" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="37" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="228" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="36" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="227" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="35" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="226" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="34" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="225" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="33" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="224" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="32" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="223" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="31" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="222" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="30" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="221" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="29" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="220" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="28" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="219" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="27" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="218" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="26" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="217" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2616,7 +4528,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B30" sqref="B30:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3069,6 +4981,24 @@
       <c r="A30" t="s">
         <v>93</v>
       </c>
+      <c r="B30">
+        <v>14.98892</v>
+      </c>
+      <c r="C30">
+        <v>0.83618000000000003</v>
+      </c>
+      <c r="E30">
+        <v>15.376620000000001</v>
+      </c>
+      <c r="F30">
+        <v>0.87207000000000001</v>
+      </c>
+      <c r="H30">
+        <v>21.1431</v>
+      </c>
+      <c r="I30">
+        <v>0.95669999999999999</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -3093,47 +5023,23 @@
     <mergeCell ref="K1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="25" priority="21" percent="1" rank="10"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="top10" dxfId="178" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="24" priority="19" percent="1" rank="10"/>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="top10" dxfId="177" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="23" priority="18" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="top10" dxfId="176" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26 B11:B18">
-    <cfRule type="top10" dxfId="22" priority="15" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="175" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="top10" dxfId="21" priority="9" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="top10" dxfId="174" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2">
-    <cfRule type="top10" dxfId="20" priority="8" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11:K15">
-    <cfRule type="top10" dxfId="19" priority="7" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L11:L15">
-    <cfRule type="top10" dxfId="18" priority="6" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H19">
-    <cfRule type="top10" dxfId="17" priority="98" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11:I19">
-    <cfRule type="top10" dxfId="16" priority="100" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B19 B29:B32 B25:B27">
-    <cfRule type="top10" dxfId="15" priority="116" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E19 E29:E1048576 E25:E27">
-    <cfRule type="top10" dxfId="14" priority="120" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F19 F29:F1048576 F25:F27">
-    <cfRule type="top10" dxfId="13" priority="124" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C19 C29:C1048576 C25:C27">
-    <cfRule type="top10" dxfId="12" priority="128" percent="1" rank="10"/>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="top10" dxfId="168" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3145,7 +5051,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3551,7 +5457,7 @@
       <c r="F14" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="11">
         <v>30.33</v>
       </c>
       <c r="I14" s="5">
@@ -3568,25 +5474,25 @@
       <c r="A15" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="5">
-        <v>14.519769999999999</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.82887999999999995</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5">
-        <v>15.407299999999999</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0.87216000000000005</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5">
-        <v>21.335280000000001</v>
-      </c>
-      <c r="I15" s="9">
-        <v>0.95531999999999995</v>
+      <c r="B15" s="12">
+        <v>14.98892</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.83618000000000003</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12">
+        <v>15.376620000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.87207000000000001</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12">
+        <v>21.1431</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.95669999999999999</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>68</v>
@@ -3628,41 +5534,41 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="top10" dxfId="11" priority="7" percent="1" rank="10"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="10" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="9" priority="11" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="8" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="7" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="top10" dxfId="6" priority="8" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H21:H1048576 H1:H2">
+    <cfRule type="top10" dxfId="18" priority="72" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H15 H21:H1048576 H1:H12">
-    <cfRule type="top10" dxfId="5" priority="62" percent="1" rank="10"/>
+  <conditionalFormatting sqref="B2:B4 B6:B13">
+    <cfRule type="top10" dxfId="17" priority="83" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 B2:B4 B6:B13">
-    <cfRule type="top10" dxfId="4" priority="73" percent="1" rank="10"/>
+  <conditionalFormatting sqref="C1:C4 C21:C1048576 C6:C13">
+    <cfRule type="top10" dxfId="16" priority="90" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C4 C15 C21:C1048576 C6:C13">
-    <cfRule type="top10" dxfId="3" priority="80" percent="1" rank="10"/>
+  <conditionalFormatting sqref="I21:I1048576 I1:I2">
+    <cfRule type="top10" dxfId="15" priority="106" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E4 E15 E21:E1048576 E6:E13">
-    <cfRule type="top10" dxfId="2" priority="86" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="top10" dxfId="14" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F4 F15 F21:F1048576 F6:F13">
-    <cfRule type="top10" dxfId="1" priority="92" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:I1048576 I1:I15">
-    <cfRule type="top10" dxfId="0" priority="96" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="top10" dxfId="12" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Early stopper stable implementation.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03C0122-80F2-4CAD-B49E-8BD9C24BAB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B26E595-11DC-49BC-895F-A7BE203BC279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38880" yWindow="1065" windowWidth="31140" windowHeight="18765" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
+    <sheet name="RRL Info" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -360,6 +361,54 @@
     <author>Neil Patrick  A. Del Gallego</author>
   </authors>
   <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{48B75DE8-3A04-4BBF-A2B8-8C340553ACD5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Image dehazing based on a transmission fusion strategy by automatic image matting</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{71C910E2-04E6-4A4B-A2EA-30A03538683B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Learning Deep Priors for Image Dehazing</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A6" authorId="0" shapeId="0" xr:uid="{B8FEB020-08E7-48AB-9FC5-5D94EBF7E06B}">
       <text>
         <r>
@@ -560,7 +609,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="104">
   <si>
     <t>PSNR</t>
   </si>
@@ -860,6 +909,18 @@
   </si>
   <si>
     <t>EPDN</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>EDPN</t>
+  </si>
+  <si>
+    <t>3D Movies + RESIDE OTS</t>
   </si>
 </sst>
 </file>
@@ -870,7 +931,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -918,6 +979,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -933,7 +1007,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -941,11 +1015,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -953,1893 +1104,95 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="237">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3797,38 +2150,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="K1" s="10" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="10"/>
+      <c r="L1" s="9"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="10"/>
+      <c r="O1" s="9"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4458,64 +2811,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="236" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="235" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="234" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="233" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="232" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="231" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="230" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="229" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="228" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="227" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="226" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="225" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="224" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="223" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="222" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="221" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="220" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="219" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="218" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="217" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4545,22 +2898,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="H1" s="10" t="s">
+      <c r="F1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="K1" s="10" t="s">
+      <c r="I1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="10"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -5024,22 +3377,22 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="178" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="177" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="176" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="175" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="174" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="168" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5051,144 +3404,155 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="3" width="16.5703125" customWidth="1"/>
-    <col min="5" max="6" width="15" customWidth="1"/>
-    <col min="8" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" style="8" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="9" width="17" style="20" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="7" customWidth="1"/>
     <col min="11" max="11" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="8" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="15"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="29">
         <v>13.48476</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="30">
         <v>0.80076000000000003</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5">
+      <c r="D3" s="29">
         <v>13.25198</v>
       </c>
-      <c r="F3" s="5">
+      <c r="E3" s="29">
         <v>0.85750000000000004</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5">
+      <c r="F3" s="30"/>
+      <c r="G3" s="29">
         <v>15.690049999999999</v>
       </c>
-      <c r="I3" s="5">
+      <c r="H3" s="31">
         <v>0.90192000000000005</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="18" t="s">
         <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" s="18" t="s">
         <v>66</v>
       </c>
       <c r="K4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="5">
+      <c r="F5" s="36"/>
+      <c r="G5" s="29">
         <v>24.71</v>
       </c>
-      <c r="I5" s="5">
+      <c r="H5" s="31">
         <v>0.89170000000000005</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="14"/>
+      <c r="J5" s="18" t="s">
         <v>66</v>
       </c>
       <c r="K5" t="s">
@@ -5199,27 +3563,27 @@
       <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="29">
         <v>14.45778</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="30">
         <v>0.79003000000000001</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5">
+      <c r="D6" s="29">
         <v>14.733599999999999</v>
       </c>
-      <c r="F6" s="5">
+      <c r="E6" s="29">
         <v>0.86065999999999998</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5">
+      <c r="F6" s="30"/>
+      <c r="G6" s="29">
         <v>20.638760000000001</v>
       </c>
-      <c r="I6" s="5">
+      <c r="H6" s="31">
         <v>0.94225000000000003</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K6" t="s">
@@ -5230,27 +3594,27 @@
       <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="37">
         <v>20.130600000000001</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="30">
         <v>0.77390000000000003</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="9">
+      <c r="D7" s="37">
         <v>16.80341</v>
       </c>
-      <c r="F7" s="5">
+      <c r="E7" s="29">
         <v>0.83260999999999996</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5">
+      <c r="F7" s="30"/>
+      <c r="G7" s="29">
         <v>11.688040000000001</v>
       </c>
-      <c r="I7" s="5">
+      <c r="H7" s="31">
         <v>0.81701999999999997</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="18" t="s">
         <v>67</v>
       </c>
       <c r="K7" t="s">
@@ -5261,27 +3625,27 @@
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="29">
         <v>18.2179</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="38">
         <v>0.85409999999999997</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5">
+      <c r="D8" s="29">
         <v>15.921799999999999</v>
       </c>
-      <c r="F8" s="5">
+      <c r="E8" s="29">
         <v>0.74519999999999997</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5">
+      <c r="F8" s="30"/>
+      <c r="G8" s="29">
         <v>22.065799999999999</v>
       </c>
-      <c r="I8" s="5">
+      <c r="H8" s="31">
         <v>0.91469999999999996</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="18" t="s">
         <v>67</v>
       </c>
       <c r="K8" t="s">
@@ -5292,27 +3656,27 @@
       <c r="A9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="29">
         <v>13.980880000000001</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="30">
         <v>0.80913000000000002</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5">
+      <c r="D9" s="29">
         <v>13.07117</v>
       </c>
-      <c r="F9" s="5">
+      <c r="E9" s="29">
         <v>0.83233999999999997</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5">
+      <c r="F9" s="30"/>
+      <c r="G9" s="29">
         <v>20.32086</v>
       </c>
-      <c r="I9" s="5">
+      <c r="H9" s="31">
         <v>0.93916999999999995</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K9" t="s">
@@ -5323,27 +3687,27 @@
       <c r="A10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="29">
         <v>12.759320000000001</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="30">
         <v>0.78044000000000002</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5">
+      <c r="D10" s="29">
         <v>12.753729999999999</v>
       </c>
-      <c r="F10" s="5">
+      <c r="E10" s="29">
         <v>0.82584000000000002</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5">
+      <c r="F10" s="30"/>
+      <c r="G10" s="29">
         <v>20.321269999999998</v>
       </c>
-      <c r="I10" s="5">
+      <c r="H10" s="31">
         <v>0.94330999999999998</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K10" t="s">
@@ -5354,27 +3718,27 @@
       <c r="A11" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="29">
         <v>16.487590000000001</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="30">
         <v>0.81867999999999996</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5">
+      <c r="D11" s="29">
         <v>15.15972</v>
       </c>
-      <c r="F11" s="5">
+      <c r="E11" s="29">
         <v>0.86604000000000003</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5">
+      <c r="F11" s="30"/>
+      <c r="G11" s="29">
         <v>20.150410000000001</v>
       </c>
-      <c r="I11" s="5">
+      <c r="H11" s="31">
         <v>0.91915999999999998</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="I11" s="14"/>
+      <c r="J11" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K11" t="s">
@@ -5385,27 +3749,27 @@
       <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="E12" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5">
+      <c r="F12" s="30"/>
+      <c r="G12" s="29">
         <v>24.01</v>
       </c>
-      <c r="I12" s="5">
+      <c r="H12" s="31">
         <v>0.93500000000000005</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K12" t="s">
@@ -5416,25 +3780,27 @@
       <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="5">
+      <c r="F13" s="36"/>
+      <c r="G13" s="29">
         <v>27.76</v>
       </c>
-      <c r="I13" s="5">
+      <c r="H13" s="31">
         <v>0.9284</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="I13" s="14"/>
+      <c r="J13" s="18" t="s">
         <v>67</v>
       </c>
       <c r="K13" t="s">
@@ -5445,25 +3811,27 @@
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="11">
+      <c r="F14" s="36"/>
+      <c r="G14" s="29">
         <v>30.33</v>
       </c>
-      <c r="I14" s="5">
+      <c r="H14" s="31">
         <v>0.94730000000000003</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="I14" s="14"/>
+      <c r="J14" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K14" t="s">
@@ -5474,27 +3842,27 @@
       <c r="A15" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="12">
-        <v>14.98892</v>
-      </c>
-      <c r="C15" s="12">
-        <v>0.83618000000000003</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12">
-        <v>15.376620000000001</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="B15" s="29">
+        <v>14.393179999999999</v>
+      </c>
+      <c r="C15" s="30">
+        <v>0.83142000000000005</v>
+      </c>
+      <c r="D15" s="29">
+        <v>15.48873</v>
+      </c>
+      <c r="E15" s="37">
         <v>0.87207000000000001</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12">
-        <v>21.1431</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0.95669999999999999</v>
-      </c>
-      <c r="J15" s="8" t="s">
+      <c r="F15" s="30"/>
+      <c r="G15" s="29">
+        <v>19.650929999999999</v>
+      </c>
+      <c r="H15" s="39">
+        <v>0.95106000000000002</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="18" t="s">
         <v>68</v>
       </c>
       <c r="K15" t="s">
@@ -5502,76 +3870,270 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="40">
         <f>AVERAGE(B3,B6:B11)</f>
         <v>15.645547142857144</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="41">
         <f>AVERAGE(C3,C6:C11)</f>
         <v>0.8038628571428571</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5">
-        <f t="shared" ref="E16:F16" si="0">AVERAGE(E3,E6:E11)</f>
+      <c r="D16" s="40">
+        <f t="shared" ref="D16:E16" si="0">AVERAGE(D3,D6:D11)</f>
         <v>14.527915714285715</v>
       </c>
-      <c r="F16" s="5">
+      <c r="E16" s="40">
         <f t="shared" si="0"/>
         <v>0.8314557142857143</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5">
+      <c r="F16" s="41"/>
+      <c r="G16" s="42">
+        <f>AVERAGE(G3,G5:G11)</f>
+        <v>19.448148749999998</v>
+      </c>
+      <c r="H16" s="40">
         <f>AVERAGE(H3,H5:H11)</f>
-        <v>19.448148749999998</v>
-      </c>
-      <c r="I16" s="5">
-        <f>AVERAGE(I3,I5:I11)</f>
         <v>0.90865375000000004</v>
       </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="top10" dxfId="22" priority="22" percent="1" rank="10"/>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="top10" dxfId="8" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="top10" dxfId="21" priority="21" percent="1" rank="10"/>
+  <conditionalFormatting sqref="G21:G1048576">
+    <cfRule type="top10" dxfId="7" priority="72" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="20" priority="20" percent="1" rank="10"/>
+  <conditionalFormatting sqref="C21:C1048576">
+    <cfRule type="top10" dxfId="5" priority="90" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="top10" dxfId="19" priority="19" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H21:I1048576 I2">
+    <cfRule type="top10" dxfId="4" priority="106" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H1048576 H1:H2">
-    <cfRule type="top10" dxfId="18" priority="72" percent="1" rank="10"/>
+  <conditionalFormatting sqref="D17:D1048576">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B4 B6:B13">
-    <cfRule type="top10" dxfId="17" priority="83" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E17:E1048576">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C4 C21:C1048576 C6:C13">
-    <cfRule type="top10" dxfId="16" priority="90" percent="1" rank="10"/>
+  <conditionalFormatting sqref="G17:G1048576">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:I1048576 I1:I2">
-    <cfRule type="top10" dxfId="15" priority="106" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="14" priority="4" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="12" priority="2" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="H17:I1048576 I2:I16">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90921C0C-3EF8-488C-A8AD-77E45C51350D}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="24" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C13:C14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes. Changed early stopper method so that it only saves the model when a better metric arrives.
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76FAD08-D98D-4213-A847-59DC9AB6EB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E616D4B-20D5-4DBD-96A5-FA27B1984A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
     <sheet name="RRL Info" sheetId="4" r:id="rId4"/>
+    <sheet name="Camera Specs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -609,7 +610,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="120">
   <si>
     <t>PSNR</t>
   </si>
@@ -921,15 +922,64 @@
   </si>
   <si>
     <t>3D Movies + RESIDE OTS</t>
+  </si>
+  <si>
+    <t>$\mathcal{K}_{d}$</t>
+  </si>
+  <si>
+    <t>Clipping Planes</t>
+  </si>
+  <si>
+    <t>Near</t>
+  </si>
+  <si>
+    <t>Far</t>
+  </si>
+  <si>
+    <t>$\mathcal{K}_{c}$</t>
+  </si>
+  <si>
+    <t>$\mathcal{K}_{u}$</t>
+  </si>
+  <si>
+    <t>Field of View</t>
+  </si>
+  <si>
+    <t>Direct Samples</t>
+  </si>
+  <si>
+    <t>Indirect Samples</t>
+  </si>
+  <si>
+    <t>Environment Samples</t>
+  </si>
+  <si>
+    <t>Bounces</t>
+  </si>
+  <si>
+    <t>Lightmapper Parameters</t>
+  </si>
+  <si>
+    <t>Post Processing</t>
+  </si>
+  <si>
+    <t>Post-Exposure Value</t>
+  </si>
+  <si>
+    <t>Saturation</t>
+  </si>
+  <si>
+    <t>Contrast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1026,7 +1076,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1111,11 +1161,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1183,6 +1242,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1201,14 +1290,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2011,38 +2109,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="F1" s="37" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="F1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="K1" s="37" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="K1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="37"/>
+      <c r="L1" s="53"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="37"/>
+      <c r="O1" s="53"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2759,22 +2857,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="C1" s="53"/>
+      <c r="E1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="H1" s="37" t="s">
+      <c r="F1" s="53"/>
+      <c r="H1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="K1" s="37" t="s">
+      <c r="I1" s="53"/>
+      <c r="K1" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="37"/>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3264,8 +3362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3281,19 +3379,19 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="40" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="38"/>
+      <c r="E1" s="54"/>
       <c r="F1" s="20"/>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="38"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="18"/>
       <c r="J1" s="15" t="s">
         <v>70</v>
@@ -3455,13 +3553,13 @@
       <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="39">
         <v>20.130600000000001</v>
       </c>
       <c r="C7" s="26">
         <v>0.77390000000000003</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="42">
         <v>16.80341</v>
       </c>
       <c r="E7" s="25">
@@ -3486,10 +3584,10 @@
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="42">
         <v>18.2179</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="40">
         <v>0.85409999999999997</v>
       </c>
       <c r="D8" s="25">
@@ -3647,14 +3745,14 @@
       <c r="C13" s="26">
         <v>0.82333000000000001</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="39">
         <v>17.625070000000001</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="39">
         <v>0.88229000000000002</v>
       </c>
       <c r="F13" s="32"/>
-      <c r="G13" s="48">
+      <c r="G13" s="42">
         <v>27.76</v>
       </c>
       <c r="H13" s="27">
@@ -3685,10 +3783,10 @@
         <v>61</v>
       </c>
       <c r="F14" s="32"/>
-      <c r="G14" s="45">
+      <c r="G14" s="39">
         <v>30.33</v>
       </c>
-      <c r="H14" s="50">
+      <c r="H14" s="44">
         <v>0.94730000000000003</v>
       </c>
       <c r="I14" s="13"/>
@@ -3706,20 +3804,20 @@
       <c r="B15" s="25">
         <v>14.393179999999999</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="43">
         <v>0.83142000000000005</v>
       </c>
       <c r="D15" s="25">
         <v>15.48873</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="42">
         <v>0.87207000000000001</v>
       </c>
       <c r="F15" s="26"/>
       <c r="G15" s="25">
         <v>19.650929999999999</v>
       </c>
-      <c r="H15" s="47">
+      <c r="H15" s="41">
         <v>0.95106000000000002</v>
       </c>
       <c r="I15" s="14"/>
@@ -3734,28 +3832,28 @@
       <c r="A16" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16" s="37">
         <f>AVERAGE(B3,B6:B11, B13)</f>
         <v>15.875438750000001</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="38">
         <f>AVERAGE(C3,C6:C11, C13)</f>
         <v>0.80629625000000005</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="37">
         <f>AVERAGE(D3,D6:D11, D13)</f>
         <v>14.91506</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="37">
         <f>AVERAGE(E3,E6:E11, E13)</f>
         <v>0.83781000000000005</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="43">
+      <c r="F16" s="38"/>
+      <c r="G16" s="37">
         <f>AVERAGE(G3,G6:G11, G13)</f>
         <v>19.829398749999999</v>
       </c>
-      <c r="H16" s="43">
+      <c r="H16" s="37">
         <f>AVERAGE(H3,H6:H11, H13)</f>
         <v>0.91324125</v>
       </c>
@@ -3834,10 +3932,10 @@
       <c r="B2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="57" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3848,8 +3946,8 @@
       <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -3858,8 +3956,8 @@
       <c r="B4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -3882,7 +3980,7 @@
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="57" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="33" t="s">
@@ -3896,7 +3994,7 @@
       <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="35" t="s">
         <v>78</v>
       </c>
@@ -3908,10 +4006,10 @@
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="57" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3922,8 +4020,8 @@
       <c r="B9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -3932,8 +4030,8 @@
       <c r="B10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -3942,8 +4040,8 @@
       <c r="B11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -3966,7 +4064,7 @@
       <c r="B13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="57" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="33" t="s">
@@ -3980,7 +4078,7 @@
       <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="35" t="s">
         <v>83</v>
       </c>
@@ -3997,4 +4095,163 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F9487-F4C7-4CD2-99DE-114C67825D09}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="45">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="45">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="50">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="48">
+        <v>100</v>
+      </c>
+      <c r="D5" s="52">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="59"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="60">
+        <v>1024</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="60">
+        <v>1024</v>
+      </c>
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="61">
+        <v>1024</v>
+      </c>
+      <c r="C10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="63">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="64"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes and updates on benchmarking
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E616D4B-20D5-4DBD-96A5-FA27B1984A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA39E42-1A0F-4E56-B37A-6395F63A8721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{75B324E0-4548-4529-BAB7-B3E2D92548E8}">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{75B324E0-4548-4529-BAB7-B3E2D92548E8}">
       <text>
         <r>
           <rPr>
@@ -610,7 +610,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="125">
   <si>
     <t>PSNR</t>
   </si>
@@ -970,6 +970,21 @@
   </si>
   <si>
     <t>Contrast</t>
+  </si>
+  <si>
+    <t>FFA-Synth</t>
+  </si>
+  <si>
+    <t>Ours - Default</t>
+  </si>
+  <si>
+    <t>Ours - No G_s</t>
+  </si>
+  <si>
+    <t>Ours - No G_s, No G_u</t>
+  </si>
+  <si>
+    <t>Ours - No G_u</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1091,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1170,11 +1185,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1211,10 +1237,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1273,6 +1297,20 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1293,25 +1331,260 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2109,38 +2382,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="F1" s="53" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="F1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="K1" s="53" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="K1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="53"/>
+      <c r="L1" s="57"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="53"/>
+      <c r="O1" s="57"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2840,7 +3113,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:I30"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2857,22 +3130,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="E1" s="53" t="s">
+      <c r="C1" s="57"/>
+      <c r="E1" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="H1" s="53" t="s">
+      <c r="F1" s="57"/>
+      <c r="H1" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="K1" s="53" t="s">
+      <c r="I1" s="57"/>
+      <c r="K1" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="53"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3360,10 +3633,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,526 +3644,607 @@
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="9" width="17" style="19" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="8" width="17" style="19" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="56" t="s">
+      <c r="E1" s="58"/>
+      <c r="F1" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="54"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="14"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="23">
         <v>13.48476</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="24">
         <v>0.80076000000000003</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="23">
         <v>13.25198</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="72">
         <v>0.85750000000000004</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="23">
+        <v>15.690049999999999</v>
+      </c>
       <c r="G3" s="25">
-        <v>15.690049999999999</v>
-      </c>
-      <c r="H3" s="27">
         <v>0.90192000000000005</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="17" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="26" t="s">
+        <v>61</v>
+      </c>
       <c r="G4" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="23">
+        <v>24.71</v>
+      </c>
       <c r="G5" s="25">
-        <v>24.71</v>
-      </c>
-      <c r="H5" s="27">
         <v>0.89170000000000005</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="17" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="23">
         <v>14.45778</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="24">
         <v>0.79003000000000001</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>14.733599999999999</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>0.86065999999999998</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="23">
+        <v>20.638760000000001</v>
+      </c>
       <c r="G6" s="25">
-        <v>20.638760000000001</v>
-      </c>
-      <c r="H6" s="27">
         <v>0.94225000000000003</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="17" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>20.130600000000001</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="24">
         <v>0.77390000000000003</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="40">
         <v>16.80341</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>0.83260999999999996</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="23">
+        <v>11.688040000000001</v>
+      </c>
       <c r="G7" s="25">
-        <v>11.688040000000001</v>
-      </c>
-      <c r="H7" s="27">
         <v>0.81701999999999997</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="17" t="s">
+      <c r="H7" s="13"/>
+      <c r="I7" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8" s="40">
         <v>18.2179</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="38">
         <v>0.85409999999999997</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="23">
         <v>15.921799999999999</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>0.74519999999999997</v>
       </c>
-      <c r="F8" s="26"/>
+      <c r="F8" s="23">
+        <v>22.065799999999999</v>
+      </c>
       <c r="G8" s="25">
-        <v>22.065799999999999</v>
-      </c>
-      <c r="H8" s="27">
         <v>0.91469999999999996</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="17" t="s">
+      <c r="H8" s="13"/>
+      <c r="I8" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K8" t="s">
+      <c r="J8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="23">
         <v>13.980880000000001</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>0.80913000000000002</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="23">
         <v>13.07117</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>0.83233999999999997</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="23">
+        <v>20.32086</v>
+      </c>
       <c r="G9" s="25">
-        <v>20.32086</v>
-      </c>
-      <c r="H9" s="27">
         <v>0.93916999999999995</v>
       </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="17" t="s">
+      <c r="H9" s="13"/>
+      <c r="I9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K9" t="s">
+      <c r="J9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="23">
         <v>12.759320000000001</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>0.78044000000000002</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="23">
         <v>12.753729999999999</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>0.82584000000000002</v>
       </c>
-      <c r="F10" s="26"/>
+      <c r="F10" s="23">
+        <v>20.321269999999998</v>
+      </c>
       <c r="G10" s="25">
-        <v>20.321269999999998</v>
-      </c>
-      <c r="H10" s="27">
         <v>0.94330999999999998</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="17" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K10" t="s">
+      <c r="J10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="23">
         <v>16.487590000000001</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="24">
         <v>0.81867999999999996</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="23">
         <v>15.15972</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <v>0.86604000000000003</v>
       </c>
-      <c r="F11" s="26"/>
+      <c r="F11" s="23">
+        <v>20.150410000000001</v>
+      </c>
       <c r="G11" s="25">
-        <v>20.150410000000001</v>
-      </c>
-      <c r="H11" s="27">
         <v>0.91915999999999998</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="17" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K11" t="s">
+      <c r="J11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="26"/>
+      <c r="F12" s="23">
+        <v>24.01</v>
+      </c>
       <c r="G12" s="25">
-        <v>24.01</v>
-      </c>
-      <c r="H12" s="27">
         <v>0.93500000000000005</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="17" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K12" t="s">
+      <c r="J12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="23">
         <v>17.484680000000001</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="24">
         <v>0.82333000000000001</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="37">
         <v>17.625070000000001</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="38">
         <v>0.88229000000000002</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="42">
+      <c r="F13" s="40">
         <v>27.76</v>
       </c>
-      <c r="H13" s="27">
+      <c r="G13" s="25">
         <v>0.9284</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="17" t="s">
+      <c r="H13" s="13"/>
+      <c r="I13" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K13" t="s">
+      <c r="J13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="39">
+      <c r="F14" s="37">
         <v>30.33</v>
       </c>
-      <c r="H14" s="44">
+      <c r="G14" s="42">
         <v>0.94730000000000003</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="17" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K14" t="s">
+      <c r="J14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="23">
         <v>14.393179999999999</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="41">
         <v>0.83142000000000005</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="23">
         <v>15.48873</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="41">
         <v>0.87207000000000001</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="25">
+      <c r="F15" s="23">
         <v>19.650929999999999</v>
       </c>
-      <c r="H15" s="41">
+      <c r="G15" s="39">
         <v>0.95106000000000002</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="17" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K15" t="s">
+      <c r="J15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="35">
         <f>AVERAGE(B3,B6:B11, B13)</f>
         <v>15.875438750000001</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="36">
         <f>AVERAGE(C3,C6:C11, C13)</f>
         <v>0.80629625000000005</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="35">
         <f>AVERAGE(D3,D6:D11, D13)</f>
         <v>14.91506</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="36">
         <f>AVERAGE(E3,E6:E11, E13)</f>
         <v>0.83781000000000005</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="37">
+      <c r="F16" s="35">
+        <f>AVERAGE(F3,F6:F11, F13)</f>
+        <v>19.829398749999999</v>
+      </c>
+      <c r="G16" s="35">
         <f>AVERAGE(G3,G6:G11, G13)</f>
-        <v>19.829398749999999</v>
-      </c>
-      <c r="H16" s="37">
-        <f>AVERAGE(H3,H6:H11, H13)</f>
         <v>0.91324125</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="9"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="58"/>
+      <c r="F19" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="58"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="5">
+        <v>14.02351</v>
+      </c>
+      <c r="C20" s="67">
+        <v>0.81435000000000002</v>
+      </c>
+      <c r="D20" s="5">
+        <v>15.275</v>
+      </c>
+      <c r="E20" s="67">
+        <v>0.86826000000000003</v>
+      </c>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="68"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="68"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="64"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="68"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="66">
+        <v>14.393179999999999</v>
+      </c>
+      <c r="C24" s="65">
+        <v>0.83142000000000005</v>
+      </c>
+      <c r="D24" s="69">
+        <v>15.48873</v>
+      </c>
+      <c r="E24" s="70">
+        <v>0.87207000000000001</v>
+      </c>
+      <c r="F24" s="71">
+        <v>19.650929999999999</v>
+      </c>
+      <c r="G24" s="71">
+        <v>0.95106000000000002</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="H2">
     <cfRule type="top10" dxfId="7" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:G1048576">
+  <conditionalFormatting sqref="F25:F1048576">
     <cfRule type="top10" dxfId="6" priority="72" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C1048576">
+  <conditionalFormatting sqref="C25:C1048576">
     <cfRule type="top10" dxfId="5" priority="90" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:I1048576 I2">
-    <cfRule type="top10" dxfId="4" priority="106" percent="1" rank="10"/>
+  <conditionalFormatting sqref="D25:D1048576 D17:D18">
+    <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D1048576">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E25:E1048576 E17:E18">
+    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E1048576">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F25:F1048576 F17:F18">
+    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:G1048576">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+  <conditionalFormatting sqref="G25:H1048576 G17:H18 H2:H16">
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:I1048576 I2:I16">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+  <conditionalFormatting sqref="G25:H1048576 H2">
+    <cfRule type="top10" dxfId="0" priority="107" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3915,13 +4269,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3932,10 +4286,10 @@
       <c r="B2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="61" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3946,8 +4300,8 @@
       <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -3956,8 +4310,8 @@
       <c r="B4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -3966,10 +4320,10 @@
       <c r="B5" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="34" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3980,10 +4334,10 @@
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="31" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3994,8 +4348,8 @@
       <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="35" t="s">
+      <c r="C7" s="62"/>
+      <c r="D7" s="33" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4006,10 +4360,10 @@
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="61" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4020,8 +4374,8 @@
       <c r="B9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -4030,8 +4384,8 @@
       <c r="B10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -4040,8 +4394,8 @@
       <c r="B11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -4050,10 +4404,10 @@
       <c r="B12" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="34" t="s">
         <v>81</v>
       </c>
     </row>
@@ -4064,10 +4418,10 @@
       <c r="B13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="31" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4078,8 +4432,8 @@
       <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="35" t="s">
+      <c r="C14" s="62"/>
+      <c r="D14" s="33" t="s">
         <v>83</v>
       </c>
       <c r="G14" s="8"/>
@@ -4101,7 +4455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F9487-F4C7-4CD2-99DE-114C67825D09}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -4114,20 +4468,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="47" t="s">
+      <c r="C1" s="63"/>
+      <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="44" t="s">
         <v>107</v>
       </c>
       <c r="D2" s="9"/>
@@ -4136,13 +4490,13 @@
       <c r="A3" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="47">
         <v>0.3</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="43">
         <v>1000</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="49">
         <v>60</v>
       </c>
     </row>
@@ -4150,13 +4504,13 @@
       <c r="A4" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="47">
         <v>0.3</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="43">
         <v>1000</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="49">
         <v>60</v>
       </c>
     </row>
@@ -4164,13 +4518,13 @@
       <c r="A5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="48">
         <v>0.3</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="46">
         <v>100</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="50">
         <v>60</v>
       </c>
     </row>
@@ -4181,26 +4535,26 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59" t="s">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="59"/>
+      <c r="D7" s="63"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="60">
+      <c r="B8" s="51">
         <v>1024</v>
       </c>
       <c r="C8" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="53">
         <v>1</v>
       </c>
     </row>
@@ -4208,13 +4562,13 @@
       <c r="A9" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="60">
+      <c r="B9" s="51">
         <v>1024</v>
       </c>
       <c r="C9" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="43">
         <v>25</v>
       </c>
     </row>
@@ -4222,13 +4576,13 @@
       <c r="A10" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="61">
+      <c r="B10" s="52">
         <v>1024</v>
       </c>
       <c r="C10" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="43">
         <v>25</v>
       </c>
     </row>
@@ -4236,14 +4590,14 @@
       <c r="A11" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="63">
+      <c r="B11" s="54">
         <v>2</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="64"/>
+      <c r="D11" s="55"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="65"/>
+      <c r="C13" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Checkpoint for refinement of training T and A
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA39E42-1A0F-4E56-B37A-6395F63A8721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AB6C92-DB76-4140-A2A3-EEB69265EFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1310,6 +1310,15 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1331,260 +1340,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2382,38 +2142,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="F1" s="57" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="F1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="K1" s="57" t="s">
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="K1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="57"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="57"/>
+      <c r="O1" s="66"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3130,22 +2890,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="E1" s="57" t="s">
+      <c r="C1" s="66"/>
+      <c r="E1" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="H1" s="57" t="s">
+      <c r="F1" s="66"/>
+      <c r="H1" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="57"/>
-      <c r="K1" s="57" t="s">
+      <c r="I1" s="66"/>
+      <c r="K1" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="57"/>
+      <c r="L1" s="66"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3636,7 +3396,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3652,18 +3412,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="60" t="s">
+      <c r="E1" s="67"/>
+      <c r="F1" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="58"/>
+      <c r="G1" s="67"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15" t="s">
         <v>70</v>
@@ -3709,7 +3469,7 @@
       <c r="D3" s="23">
         <v>13.25198</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="65">
         <v>0.85750000000000004</v>
       </c>
       <c r="F3" s="23">
@@ -4061,13 +3821,13 @@
         <v>62</v>
       </c>
       <c r="B15" s="23">
-        <v>14.393179999999999</v>
+        <v>14.676819999999999</v>
       </c>
       <c r="C15" s="41">
-        <v>0.83142000000000005</v>
+        <v>0.83743999999999996</v>
       </c>
       <c r="D15" s="23">
-        <v>15.48873</v>
+        <v>15.654809999999999</v>
       </c>
       <c r="E15" s="41">
         <v>0.87207000000000001</v>
@@ -4091,27 +3851,27 @@
         <v>84</v>
       </c>
       <c r="B16" s="35">
-        <f>AVERAGE(B3,B6:B11, B13)</f>
+        <f t="shared" ref="B16:G16" si="0">AVERAGE(B3,B6:B11, B13)</f>
         <v>15.875438750000001</v>
       </c>
       <c r="C16" s="36">
-        <f>AVERAGE(C3,C6:C11, C13)</f>
+        <f t="shared" si="0"/>
         <v>0.80629625000000005</v>
       </c>
       <c r="D16" s="35">
-        <f>AVERAGE(D3,D6:D11, D13)</f>
+        <f t="shared" si="0"/>
         <v>14.91506</v>
       </c>
       <c r="E16" s="36">
-        <f>AVERAGE(E3,E6:E11, E13)</f>
+        <f t="shared" si="0"/>
         <v>0.83781000000000005</v>
       </c>
       <c r="F16" s="35">
-        <f>AVERAGE(F3,F6:F11, F13)</f>
+        <f t="shared" si="0"/>
         <v>19.829398749999999</v>
       </c>
       <c r="G16" s="35">
-        <f>AVERAGE(G3,G6:G11, G13)</f>
+        <f t="shared" si="0"/>
         <v>0.91324125</v>
       </c>
       <c r="H16" s="13"/>
@@ -4129,18 +3889,18 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60" t="s">
+      <c r="C19" s="68"/>
+      <c r="D19" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="58"/>
-      <c r="F19" s="60" t="s">
+      <c r="E19" s="67"/>
+      <c r="F19" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="58"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -4149,25 +3909,30 @@
       <c r="B20" s="5">
         <v>14.02351</v>
       </c>
-      <c r="C20" s="67">
+      <c r="C20" s="60">
         <v>0.81435000000000002</v>
       </c>
       <c r="D20" s="5">
         <v>15.275</v>
       </c>
-      <c r="E20" s="67">
+      <c r="E20" s="60">
         <v>0.86826000000000003</v>
       </c>
-      <c r="G20"/>
+      <c r="F20">
+        <v>17.915420000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.94120999999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>122</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="68"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="68"/>
+      <c r="E21" s="61"/>
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4175,40 +3940,40 @@
         <v>124</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="68"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="68"/>
+      <c r="E22" s="61"/>
       <c r="G22"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="64"/>
+      <c r="C23" s="57"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="68"/>
+      <c r="E23" s="61"/>
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="B24" s="66">
-        <v>14.393179999999999</v>
-      </c>
-      <c r="C24" s="65">
-        <v>0.83142000000000005</v>
-      </c>
-      <c r="D24" s="69">
-        <v>15.48873</v>
-      </c>
-      <c r="E24" s="70">
+      <c r="B24" s="59">
+        <v>14.676819999999999</v>
+      </c>
+      <c r="C24" s="58">
+        <v>0.83743999999999996</v>
+      </c>
+      <c r="D24" s="62">
+        <v>15.654809999999999</v>
+      </c>
+      <c r="E24" s="63">
         <v>0.87207000000000001</v>
       </c>
-      <c r="F24" s="71">
+      <c r="F24" s="64">
         <v>19.650929999999999</v>
       </c>
-      <c r="G24" s="71">
+      <c r="G24" s="64">
         <v>0.95106000000000002</v>
       </c>
     </row>
@@ -4286,10 +4051,10 @@
       <c r="B2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="70" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4300,8 +4065,8 @@
       <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4310,8 +4075,8 @@
       <c r="B4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -4334,7 +4099,7 @@
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="70" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="31" t="s">
@@ -4348,7 +4113,7 @@
       <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="62"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="33" t="s">
         <v>78</v>
       </c>
@@ -4360,10 +4125,10 @@
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="70" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4374,8 +4139,8 @@
       <c r="B9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -4384,8 +4149,8 @@
       <c r="B10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -4394,8 +4159,8 @@
       <c r="B11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -4418,7 +4183,7 @@
       <c r="B13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="70" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="31" t="s">
@@ -4432,7 +4197,7 @@
       <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="62"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="33" t="s">
         <v>83</v>
       </c>
@@ -4468,10 +4233,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="63"/>
+      <c r="C1" s="72"/>
       <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
@@ -4535,14 +4300,14 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63" t="s">
+      <c r="B7" s="72"/>
+      <c r="C7" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="63"/>
+      <c r="D7" s="72"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Optimization in T and A training
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143907D2-99B6-442B-909A-2F84327F5DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6895E3B-32E2-4AF0-9C71-E38896A4CCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="125">
   <si>
     <t>PSNR</t>
   </si>
@@ -1200,7 +1200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1310,7 +1310,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2141,38 +2140,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="F1" s="65" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="F1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="K1" s="65" t="s">
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="K1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="65"/>
+      <c r="L1" s="64"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="65" t="s">
+      <c r="N1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="65"/>
+      <c r="O1" s="64"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="65" t="s">
+      <c r="S1" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2889,22 +2888,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="E1" s="65" t="s">
+      <c r="C1" s="64"/>
+      <c r="E1" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="H1" s="65" t="s">
+      <c r="F1" s="64"/>
+      <c r="H1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="65"/>
-      <c r="K1" s="65" t="s">
+      <c r="I1" s="64"/>
+      <c r="K1" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="65"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3392,10 +3391,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,18 +3410,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="68" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="68" t="s">
+      <c r="E1" s="65"/>
+      <c r="F1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15" t="s">
         <v>70</v>
@@ -3468,7 +3467,7 @@
       <c r="D3" s="23">
         <v>13.25198</v>
       </c>
-      <c r="E3" s="64">
+      <c r="E3" s="63">
         <v>0.85750000000000004</v>
       </c>
       <c r="F3" s="23">
@@ -3888,118 +3887,152 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="68" t="s">
+      <c r="C19" s="66"/>
+      <c r="D19" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="68" t="s">
+      <c r="E19" s="65"/>
+      <c r="F19" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="66"/>
+      <c r="G19" s="65"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="5">
-        <v>14.02351</v>
-      </c>
-      <c r="C20" s="60">
-        <v>0.81435000000000002</v>
-      </c>
-      <c r="D20" s="5">
-        <v>15.275</v>
-      </c>
-      <c r="E20" s="60">
-        <v>0.86826000000000003</v>
-      </c>
-      <c r="F20" s="5">
-        <v>17.915420000000001</v>
-      </c>
-      <c r="G20" s="5">
-        <v>0.94120999999999999</v>
+      <c r="A20" s="11"/>
+      <c r="B20" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B21" s="5">
-        <v>14.051920000000001</v>
-      </c>
-      <c r="C21" s="61">
-        <v>0.83204</v>
+        <v>14.02351</v>
+      </c>
+      <c r="C21" s="59">
+        <v>0.81435000000000002</v>
       </c>
       <c r="D21" s="5">
-        <v>15.15972</v>
-      </c>
-      <c r="E21" s="61">
-        <v>0.86431000000000002</v>
+        <v>15.275</v>
+      </c>
+      <c r="E21" s="59">
+        <v>0.86826000000000003</v>
       </c>
       <c r="F21" s="5">
-        <v>18.527529999999999</v>
+        <v>17.915420000000001</v>
       </c>
       <c r="G21" s="5">
-        <v>0.94394999999999996</v>
+        <v>0.94120999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" s="5">
-        <v>13.87458</v>
-      </c>
-      <c r="C22" s="61">
-        <v>0.82935000000000003</v>
+        <v>14.051920000000001</v>
+      </c>
+      <c r="C22" s="60">
+        <v>0.83204</v>
       </c>
       <c r="D22" s="5">
-        <v>15.59061</v>
-      </c>
-      <c r="E22" s="61">
-        <v>0.86753000000000002</v>
+        <v>15.15972</v>
+      </c>
+      <c r="E22" s="60">
+        <v>0.86431000000000002</v>
       </c>
       <c r="F22" s="5">
-        <v>17.965720000000001</v>
+        <v>18.527529999999999</v>
       </c>
       <c r="G22" s="5">
-        <v>0.94262000000000001</v>
+        <v>0.94394999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="5">
+        <v>13.87458</v>
+      </c>
+      <c r="C23" s="60">
+        <v>0.82935000000000003</v>
+      </c>
+      <c r="D23" s="5">
+        <v>15.59061</v>
+      </c>
+      <c r="E23" s="60">
+        <v>0.86753000000000002</v>
+      </c>
+      <c r="F23" s="5">
+        <v>17.965720000000001</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.94262000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="B24" s="5">
+        <v>12.76966</v>
+      </c>
+      <c r="C24" s="60">
+        <v>0.80222000000000004</v>
+      </c>
+      <c r="D24" s="5">
+        <v>14.243539999999999</v>
+      </c>
+      <c r="E24" s="60">
+        <v>0.84404999999999997</v>
+      </c>
+      <c r="F24" s="5">
+        <v>17.19858</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.92442000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="B24" s="59">
+      <c r="B25" s="58">
         <v>14.676819999999999</v>
       </c>
-      <c r="C24" s="58">
+      <c r="C25" s="57">
         <v>0.83743999999999996</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D25" s="61">
         <v>15.654809999999999</v>
       </c>
-      <c r="E24" s="63">
+      <c r="E25" s="62">
         <v>0.87207000000000001</v>
       </c>
-      <c r="F24" s="62">
+      <c r="F25" s="61">
         <v>19.914300000000001</v>
       </c>
-      <c r="G24" s="62">
+      <c r="G25" s="61">
         <v>0.95125000000000004</v>
       </c>
     </row>
@@ -4016,26 +4049,26 @@
   <conditionalFormatting sqref="H2">
     <cfRule type="top10" dxfId="7" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F1048576">
+  <conditionalFormatting sqref="F26:F1048576">
     <cfRule type="top10" dxfId="6" priority="72" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C1048576">
+  <conditionalFormatting sqref="C26:C1048576">
     <cfRule type="top10" dxfId="5" priority="90" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D1048576 D17:D18">
+  <conditionalFormatting sqref="D26:D1048576 D17:D18">
     <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E1048576 E17:E18">
+  <conditionalFormatting sqref="E26:E1048576 E17:E18">
     <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F1048576 F17:F18">
+  <conditionalFormatting sqref="F26:F1048576 F17:F18">
     <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G25:H1048576 G17:H18 H2:H16">
-    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H25:H1048576 G26:G1048576 G17:H18 H2:H16">
+    <cfRule type="top10" dxfId="1" priority="111" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G25:H1048576 H2">
-    <cfRule type="top10" dxfId="0" priority="107" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H25:H1048576 G26:G1048576 H2">
+    <cfRule type="top10" dxfId="0" priority="115" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4077,10 +4110,10 @@
       <c r="B2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="68" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4091,8 +4124,8 @@
       <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4101,8 +4134,8 @@
       <c r="B4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -4125,7 +4158,7 @@
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="68" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="31" t="s">
@@ -4139,7 +4172,7 @@
       <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="70"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="33" t="s">
         <v>78</v>
       </c>
@@ -4151,10 +4184,10 @@
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="68" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4165,8 +4198,8 @@
       <c r="B9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -4175,8 +4208,8 @@
       <c r="B10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -4185,8 +4218,8 @@
       <c r="B11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -4209,7 +4242,7 @@
       <c r="B13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="68" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="31" t="s">
@@ -4223,7 +4256,7 @@
       <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="70"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="33" t="s">
         <v>83</v>
       </c>
@@ -4259,10 +4292,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="71"/>
+      <c r="C1" s="70"/>
       <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
@@ -4326,14 +4359,14 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71" t="s">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="70"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Bug fixes in CycleGAN training
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\NeuralNets-GenerativeExperiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\SynthDehazing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990ACFE6-D43E-43D2-A949-2B5CCEC489A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F8D394-4EBE-458D-B8EE-BB3DCA5D1657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="198" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
     <sheet name="Actual" sheetId="3" r:id="rId3"/>
-    <sheet name="RRL Info" sheetId="4" r:id="rId4"/>
-    <sheet name="Camera Specs" sheetId="5" r:id="rId5"/>
+    <sheet name="Ablation 1" sheetId="6" r:id="rId4"/>
+    <sheet name="RRL Info" sheetId="4" r:id="rId5"/>
+    <sheet name="Camera Specs" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -610,7 +611,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="147">
   <si>
     <t>PSNR</t>
   </si>
@@ -1021,6 +1022,36 @@
   </si>
   <si>
     <t>32 x 32</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>[0.6, 1.8]</t>
+  </si>
+  <si>
+    <t>[0.7, 1.0]</t>
+  </si>
+  <si>
+    <t>[0.1, 1.8]</t>
+  </si>
+  <si>
+    <t>[0.1, 1.0]</t>
+  </si>
+  <si>
+    <t>[0.35, 0.5]</t>
+  </si>
+  <si>
+    <t>[0.3, 0.9]</t>
+  </si>
+  <si>
+    <t>[0.05, 0.9]</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1356,6 +1387,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1368,6 +1407,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1377,18 +1425,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2191,38 +2227,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="F1" s="59" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="F1" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="K1" s="59" t="s">
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="K1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="59"/>
+      <c r="L1" s="67"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="59"/>
+      <c r="O1" s="67"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="59" t="s">
+      <c r="S1" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2939,22 +2975,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="E1" s="59" t="s">
+      <c r="C1" s="67"/>
+      <c r="E1" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="H1" s="59" t="s">
+      <c r="F1" s="67"/>
+      <c r="H1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="K1" s="59" t="s">
+      <c r="I1" s="67"/>
+      <c r="K1" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="59"/>
+      <c r="L1" s="67"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3444,13 +3480,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
@@ -3461,18 +3497,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="60"/>
-      <c r="F1" s="62" t="s">
+      <c r="E1" s="68"/>
+      <c r="F1" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="60"/>
+      <c r="G1" s="68"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15" t="s">
         <v>70</v>
@@ -3938,37 +3974,37 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="69" t="s">
+      <c r="C19" s="72"/>
+      <c r="D19" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="70"/>
-      <c r="F19" s="60" t="s">
+      <c r="E19" s="72"/>
+      <c r="F19" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="60"/>
+      <c r="G19" s="68"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="67" t="s">
+      <c r="D20" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="67" t="s">
+      <c r="F20" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="60" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4097,16 +4133,16 @@
       <c r="C26" s="38">
         <v>0.83743999999999996</v>
       </c>
-      <c r="D26" s="66">
+      <c r="D26" s="59">
         <v>15.654809999999999</v>
       </c>
-      <c r="E26" s="71">
+      <c r="E26" s="62">
         <v>0.87207000000000001</v>
       </c>
-      <c r="F26" s="66">
+      <c r="F26" s="59">
         <v>19.914300000000001</v>
       </c>
-      <c r="G26" s="66">
+      <c r="G26" s="59">
         <v>0.95125000000000004</v>
       </c>
     </row>
@@ -4114,22 +4150,22 @@
       <c r="A27" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="72">
+      <c r="B27" s="63">
         <v>15.875438750000001</v>
       </c>
-      <c r="C27" s="73">
+      <c r="C27" s="64">
         <v>0.80629625000000005</v>
       </c>
-      <c r="D27" s="72">
+      <c r="D27" s="63">
         <v>14.91506</v>
       </c>
-      <c r="E27" s="73">
+      <c r="E27" s="64">
         <v>0.83781000000000005</v>
       </c>
-      <c r="F27" s="72">
+      <c r="F27" s="63">
         <v>19.829398749999999</v>
       </c>
-      <c r="G27" s="72">
+      <c r="G27" s="63">
         <v>0.91324125</v>
       </c>
     </row>
@@ -4147,25 +4183,25 @@
     <cfRule type="top10" dxfId="7" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F1048576">
-    <cfRule type="top10" dxfId="6" priority="72" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="116" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C1048576">
-    <cfRule type="top10" dxfId="5" priority="90" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="119" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D1048576 D17:D18">
-    <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
+  <conditionalFormatting sqref="D17:D18 D28:D1048576">
+    <cfRule type="top10" dxfId="4" priority="122" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E1048576 E17:E18">
-    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E17:E18 E28:E1048576">
+    <cfRule type="top10" dxfId="3" priority="126" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F1048576 F17:F18">
-    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F17:F18 F28:F1048576">
+    <cfRule type="top10" dxfId="2" priority="130" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26:H1048576 G28:G1048576 G17:H18 H2:H16">
-    <cfRule type="top10" dxfId="1" priority="111" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H26:H1048576 G17:H18 H2:H16 G28:G1048576">
+    <cfRule type="top10" dxfId="1" priority="134" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26:H1048576 G28:G1048576 H2">
-    <cfRule type="top10" dxfId="0" priority="115" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H26:H1048576 H2 G28:G1048576">
+    <cfRule type="top10" dxfId="0" priority="142" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4174,6 +4210,194 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3513DC-2654-45B1-823E-7102A41B0B3D}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="19" customWidth="1"/>
+    <col min="3" max="8" width="18.7109375" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="71"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="66">
+        <v>14.84685</v>
+      </c>
+      <c r="D4" s="66">
+        <v>0.83896000000000004</v>
+      </c>
+      <c r="E4" s="13">
+        <v>16.093779999999999</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.88080999999999998</v>
+      </c>
+      <c r="G4" s="66">
+        <v>20.314550000000001</v>
+      </c>
+      <c r="H4" s="66">
+        <v>0.95567999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="13">
+        <v>14.66441</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.8387</v>
+      </c>
+      <c r="E6" s="13">
+        <v>16.181640000000002</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.88209000000000004</v>
+      </c>
+      <c r="G6" s="13">
+        <v>20.25264</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.95398000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90921C0C-3EF8-488C-A8AD-77E45C51350D}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -4207,10 +4431,10 @@
       <c r="B2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="74" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4221,8 +4445,8 @@
       <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4231,8 +4455,8 @@
       <c r="B4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -4255,7 +4479,7 @@
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="74" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="31" t="s">
@@ -4269,7 +4493,7 @@
       <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="64"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="33" t="s">
         <v>78</v>
       </c>
@@ -4281,10 +4505,10 @@
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="74" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4295,8 +4519,8 @@
       <c r="B9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -4305,8 +4529,8 @@
       <c r="B10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -4315,8 +4539,8 @@
       <c r="B11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -4339,7 +4563,7 @@
       <c r="B13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="74" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="31" t="s">
@@ -4353,7 +4577,7 @@
       <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="33" t="s">
         <v>83</v>
       </c>
@@ -4372,7 +4596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F9487-F4C7-4CD2-99DE-114C67825D09}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -4389,10 +4613,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="65"/>
+      <c r="C1" s="76"/>
       <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
@@ -4456,14 +4680,14 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65" t="s">
+      <c r="B7" s="76"/>
+      <c r="C7" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="65"/>
+      <c r="D7" s="76"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Added new RRL for benchmarking
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\SynthDehazing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040AEC46-9254-45BF-B489-CDC0B935C92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CE6DF4-D303-46C0-8642-D457205F977C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="1425" windowWidth="34320" windowHeight="18645" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,6 +607,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{EC797CBB-6EFF-4872-A54A-E01E77B17F80}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neil Patrick  A. Del Gallego:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+physics-based generative adversarial models for image restoration and beyond
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -630,7 +655,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="172">
   <si>
     <t>PSNR</t>
   </si>
@@ -1128,6 +1153,24 @@
   </si>
   <si>
     <t>\mathcal{K}_{c}</t>
+  </si>
+  <si>
+    <t>PhysicsGAN</t>
+  </si>
+  <si>
+    <t>Supervised, Single-Image</t>
+  </si>
+  <si>
+    <t>Supervised, Single Image</t>
+  </si>
+  <si>
+    <t>Input image as reference</t>
+  </si>
+  <si>
+    <t>YOLY-Dehaze</t>
+  </si>
+  <si>
+    <t>SGID-PFF</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1238,6 +1281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1351,7 +1400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1423,7 +1472,6 @@
     <xf numFmtId="165" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1450,7 +1498,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1469,6 +1516,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1499,18 +1565,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2321,38 +2390,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="F1" s="73" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="F1" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="K1" s="73" t="s">
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="K1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="73"/>
+      <c r="L1" s="80"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="73" t="s">
+      <c r="N1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="73"/>
+      <c r="O1" s="80"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="73" t="s">
+      <c r="S1" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3069,22 +3138,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="E1" s="73" t="s">
+      <c r="C1" s="80"/>
+      <c r="E1" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="H1" s="73" t="s">
+      <c r="F1" s="80"/>
+      <c r="H1" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="73"/>
-      <c r="K1" s="73" t="s">
+      <c r="I1" s="80"/>
+      <c r="K1" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="73"/>
+      <c r="L1" s="80"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3572,10 +3641,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,18 +3660,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="76" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="76" t="s">
+      <c r="E1" s="81"/>
+      <c r="F1" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="74"/>
+      <c r="G1" s="81"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15" t="s">
         <v>69</v>
@@ -3645,10 +3714,10 @@
       <c r="C3" s="24">
         <v>0.80076000000000003</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="91">
         <v>13.25198</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="92">
         <v>0.85750000000000004</v>
       </c>
       <c r="F3" s="23">
@@ -3675,10 +3744,10 @@
       <c r="C4" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="93" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="94" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="26" t="s">
@@ -3705,10 +3774,10 @@
       <c r="C5" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="96" t="s">
         <v>60</v>
       </c>
       <c r="F5" s="23">
@@ -3735,10 +3804,10 @@
       <c r="C6" s="24">
         <v>0.79003000000000001</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="91">
         <v>14.733599999999999</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="97">
         <v>0.86065999999999998</v>
       </c>
       <c r="F6" s="23">
@@ -3765,10 +3834,10 @@
       <c r="C7" s="24">
         <v>0.77390000000000003</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="90">
         <v>16.80341</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="97">
         <v>0.83260999999999996</v>
       </c>
       <c r="F7" s="23">
@@ -3795,10 +3864,10 @@
       <c r="C8" s="38">
         <v>0.85409999999999997</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="91">
         <v>15.921799999999999</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="97">
         <v>0.74519999999999997</v>
       </c>
       <c r="F8" s="23">
@@ -3825,10 +3894,10 @@
       <c r="C9" s="24">
         <v>0.80913000000000002</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="91">
         <v>13.07117</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="97">
         <v>0.83233999999999997</v>
       </c>
       <c r="F9" s="23">
@@ -3855,10 +3924,10 @@
       <c r="C10" s="24">
         <v>0.78044000000000002</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="91">
         <v>12.753729999999999</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="97">
         <v>0.82584000000000002</v>
       </c>
       <c r="F10" s="23">
@@ -3885,10 +3954,10 @@
       <c r="C11" s="24">
         <v>0.81867999999999996</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="91">
         <v>15.15972</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="97">
         <v>0.86604000000000003</v>
       </c>
       <c r="F11" s="23">
@@ -3915,10 +3984,10 @@
       <c r="C12" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="97" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="23">
@@ -3948,7 +4017,7 @@
       <c r="D13" s="37">
         <v>17.625070000000001</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="97">
         <v>0.88229000000000002</v>
       </c>
       <c r="F13" s="40">
@@ -3975,16 +4044,16 @@
       <c r="C14" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="96" t="s">
         <v>60</v>
       </c>
       <c r="F14" s="37">
         <v>30.33</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="41">
         <v>0.94730000000000003</v>
       </c>
       <c r="H14" s="13"/>
@@ -3997,288 +4066,344 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="23">
+        <v>17.29</v>
+      </c>
+      <c r="C15" s="24">
+        <v>0.82862000000000002</v>
+      </c>
+      <c r="D15" s="91">
+        <v>16.479649999999999</v>
+      </c>
+      <c r="E15" s="97">
+        <v>0.87983</v>
+      </c>
+      <c r="F15" s="77"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="23">
+        <v>15.60083</v>
+      </c>
+      <c r="C17" s="24">
+        <v>0.79781999999999997</v>
+      </c>
+      <c r="D17" s="91">
+        <v>16.34646</v>
+      </c>
+      <c r="E17" s="78">
+        <v>0.88778000000000001</v>
+      </c>
+      <c r="F17" s="77"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="23">
-        <v>14.84685</v>
-      </c>
-      <c r="C15" s="41">
-        <v>0.83896000000000004</v>
-      </c>
-      <c r="D15" s="23">
-        <v>16.093779999999999</v>
-      </c>
-      <c r="E15" s="41">
-        <v>0.88080999999999998</v>
-      </c>
-      <c r="F15" s="23">
+      <c r="B18" s="5">
+        <v>14.94026</v>
+      </c>
+      <c r="C18" s="76">
+        <v>0.83992</v>
+      </c>
+      <c r="D18" s="98">
+        <v>16.16921</v>
+      </c>
+      <c r="E18" s="56">
+        <v>0.88885000000000003</v>
+      </c>
+      <c r="F18" s="23">
         <v>20.314550000000001</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G18" s="39">
         <v>0.95567999999999997</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="H18" s="14"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="35">
-        <f t="shared" ref="B16:G16" si="0">AVERAGE(B3,B6:B11, B13)</f>
+      <c r="B19" s="35">
+        <f t="shared" ref="B19:G19" si="0">AVERAGE(B3,B6:B11, B13)</f>
         <v>15.875438750000001</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C19" s="36">
         <f t="shared" si="0"/>
         <v>0.80629625000000005</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D19" s="99">
         <f t="shared" si="0"/>
         <v>14.91506</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E19" s="100">
         <f t="shared" si="0"/>
         <v>0.83781000000000005</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F19" s="35">
         <f t="shared" si="0"/>
         <v>19.829398749999999</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G19" s="35">
         <f t="shared" si="0"/>
         <v>0.91324125</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="H19" s="13"/>
+      <c r="I19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="B17" s="5">
-        <v>14.94026</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B20" s="5">
+        <v>16.07985</v>
+      </c>
+      <c r="C20" s="5">
         <v>0.83992</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D20" s="5">
         <v>16.16921</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E20" s="5">
         <v>0.88100000000000001</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="77" t="s">
+      <c r="F20" s="5"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="77" t="s">
+      <c r="C22" s="85"/>
+      <c r="D22" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="78"/>
-      <c r="F19" s="74" t="s">
+      <c r="E22" s="85"/>
+      <c r="F22" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="74"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="56" t="s">
+      <c r="G22" s="81"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C23" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D23" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E23" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F23" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="56" t="s">
+      <c r="G23" s="54" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B24" s="13">
         <v>14.02351</v>
       </c>
-      <c r="C21" s="53">
+      <c r="C24" s="52">
         <v>0.81435000000000002</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D24" s="13">
         <v>15.275</v>
       </c>
-      <c r="E21" s="53">
+      <c r="E24" s="52">
         <v>0.86826000000000003</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F24" s="75">
         <v>17.915420000000001</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G24" s="13">
         <v>0.94120999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B25" s="13">
         <v>14.051920000000001</v>
       </c>
-      <c r="C22" s="53">
+      <c r="C25" s="52">
         <v>0.83204</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D25" s="13">
         <v>15.15972</v>
       </c>
-      <c r="E22" s="53">
+      <c r="E25" s="52">
         <v>0.86431000000000002</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F25" s="13">
         <v>18.527529999999999</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G25" s="13">
         <v>0.94394999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B26" s="13">
         <v>13.87458</v>
       </c>
-      <c r="C23" s="53">
+      <c r="C26" s="52">
         <v>0.82935000000000003</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D26" s="13">
         <v>15.59061</v>
       </c>
-      <c r="E23" s="53">
+      <c r="E26" s="52">
         <v>0.86753000000000002</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F26" s="13">
         <v>17.965720000000001</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G26" s="13">
         <v>0.94262000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B27" s="13">
         <v>12.76966</v>
       </c>
-      <c r="C24" s="53">
+      <c r="C27" s="52">
         <v>0.80222000000000004</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D27" s="13">
         <v>14.243539999999999</v>
       </c>
-      <c r="E24" s="53">
+      <c r="E27" s="52">
         <v>0.84404999999999997</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F27" s="13">
         <v>17.19858</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G27" s="13">
         <v>0.92442000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B28" s="13">
         <v>12.74478</v>
       </c>
-      <c r="C25" s="53">
+      <c r="C28" s="52">
         <v>0.79569000000000001</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D28" s="13">
         <v>14.030749999999999</v>
       </c>
-      <c r="E25" s="53">
+      <c r="E28" s="52">
         <v>0.82940000000000003</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F28" s="13">
         <v>15.864240000000001</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G28" s="13">
         <v>0.91015000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="39">
+      <c r="B29" s="39">
         <v>14.676819999999999</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C29" s="38">
         <v>0.83743999999999996</v>
       </c>
-      <c r="D26" s="55">
+      <c r="D29" s="53">
         <v>15.654809999999999</v>
       </c>
-      <c r="E26" s="58">
+      <c r="E29" s="56">
         <v>0.87207000000000001</v>
       </c>
-      <c r="F26" s="55">
+      <c r="F29" s="53">
         <v>19.914300000000001</v>
       </c>
-      <c r="G26" s="55">
+      <c r="G29" s="53">
         <v>0.95125000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="59">
+      <c r="B30" s="57">
         <v>15.875438750000001</v>
       </c>
-      <c r="C27" s="60">
+      <c r="C30" s="58">
         <v>0.80629625000000005</v>
       </c>
-      <c r="D27" s="59">
+      <c r="D30" s="57">
         <v>14.91506</v>
       </c>
-      <c r="E27" s="60">
+      <c r="E30" s="58">
         <v>0.83781000000000005</v>
       </c>
-      <c r="F27" s="59">
+      <c r="F30" s="57">
         <v>19.829398749999999</v>
       </c>
-      <c r="G27" s="59">
+      <c r="G30" s="57">
         <v>0.91324125</v>
       </c>
     </row>
@@ -4287,34 +4412,34 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="7" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F1048576">
-    <cfRule type="top10" dxfId="6" priority="116" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F31:F1048576">
+    <cfRule type="top10" dxfId="6" priority="118" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C1048576">
-    <cfRule type="top10" dxfId="5" priority="119" percent="1" rank="10"/>
+  <conditionalFormatting sqref="C31:C1048576">
+    <cfRule type="top10" dxfId="5" priority="121" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D18 D28:D1048576">
-    <cfRule type="top10" dxfId="4" priority="122" percent="1" rank="10"/>
+  <conditionalFormatting sqref="D20:D21 D31:D1048576">
+    <cfRule type="top10" dxfId="4" priority="124" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E18 E28:E1048576">
-    <cfRule type="top10" dxfId="3" priority="126" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E20:E21 E31:E1048576">
+    <cfRule type="top10" dxfId="3" priority="128" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F18 F28:F1048576">
-    <cfRule type="top10" dxfId="2" priority="130" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F20:F21 F31:F1048576">
+    <cfRule type="top10" dxfId="2" priority="132" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26:H1048576 G17:H18 H2:H16 G28:G1048576">
-    <cfRule type="top10" dxfId="1" priority="134" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H29:H1048576 G20:H21 H2:H19 G31:G1048576">
+    <cfRule type="top10" dxfId="1" priority="136" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26:H1048576 H2 G28:G1048576">
-    <cfRule type="top10" dxfId="0" priority="142" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H29:H1048576 H2 G31:G1048576">
+    <cfRule type="top10" dxfId="0" priority="144" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4324,10 +4449,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90921C0C-3EF8-488C-A8AD-77E45C51350D}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4356,10 +4481,10 @@
       <c r="B2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="86" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4370,8 +4495,8 @@
       <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
@@ -4380,8 +4505,8 @@
       <c r="B4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -4404,7 +4529,7 @@
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="86" t="s">
         <v>66</v>
       </c>
       <c r="D6" s="31" t="s">
@@ -4418,7 +4543,7 @@
       <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="80"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="33" t="s">
         <v>77</v>
       </c>
@@ -4430,10 +4555,10 @@
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="86" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4444,8 +4569,8 @@
       <c r="B9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -4454,8 +4579,8 @@
       <c r="B10" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -4464,8 +4589,8 @@
       <c r="B11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -4481,36 +4606,56 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="79" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="79" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B15" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C15" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D15" s="31" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="33" t="s">
+      <c r="C16" s="87"/>
+      <c r="D16" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="C6:C7"/>
@@ -4525,7 +4670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F9487-F4C7-4CD2-99DE-114C67825D09}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
@@ -4538,20 +4683,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="88"/>
+      <c r="D1" s="44" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>105</v>
       </c>
       <c r="D2" s="9"/>
@@ -4560,13 +4705,13 @@
       <c r="A3" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="85">
+      <c r="B3" s="73">
         <v>0.3</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="42">
         <v>1000</v>
       </c>
-      <c r="D3" s="83">
+      <c r="D3" s="71">
         <v>60</v>
       </c>
     </row>
@@ -4574,13 +4719,13 @@
       <c r="A4" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="85">
+      <c r="B4" s="73">
         <v>0.3</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="42">
         <v>1000</v>
       </c>
-      <c r="D4" s="83">
+      <c r="D4" s="71">
         <v>60</v>
       </c>
     </row>
@@ -4588,13 +4733,13 @@
       <c r="A5" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="86">
+      <c r="B5" s="74">
         <v>0.3</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>100</v>
       </c>
-      <c r="D5" s="84">
+      <c r="D5" s="72">
         <v>60</v>
       </c>
     </row>
@@ -4605,26 +4750,26 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81" t="s">
+      <c r="B7" s="88"/>
+      <c r="C7" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="81"/>
+      <c r="D7" s="88"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="46">
         <v>1024</v>
       </c>
       <c r="C8" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="49">
+      <c r="D8" s="48">
         <v>1</v>
       </c>
     </row>
@@ -4632,13 +4777,13 @@
       <c r="A9" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="46">
         <v>1024</v>
       </c>
       <c r="C9" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="42">
         <v>25</v>
       </c>
     </row>
@@ -4646,13 +4791,13 @@
       <c r="A10" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="47">
         <v>1024</v>
       </c>
       <c r="C10" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="42">
         <v>25</v>
       </c>
     </row>
@@ -4660,14 +4805,14 @@
       <c r="A11" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B11" s="49">
         <v>2</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="51"/>
+      <c r="D11" s="50"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="52"/>
+      <c r="C13" s="51"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
@@ -4676,10 +4821,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="44" t="s">
         <v>126</v>
       </c>
     </row>
@@ -4741,7 +4886,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4764,22 +4909,22 @@
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="77" t="s">
+      <c r="C2" s="89"/>
+      <c r="D2" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77" t="s">
+      <c r="G2" s="84"/>
+      <c r="H2" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="77"/>
+      <c r="I2" s="84"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -4791,22 +4936,22 @@
       <c r="C3" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="54" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4820,22 +4965,22 @@
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="69">
+      <c r="D4" s="67">
         <v>14.84685</v>
       </c>
-      <c r="E4" s="69">
+      <c r="E4" s="67">
         <v>0.83896000000000004</v>
       </c>
-      <c r="F4" s="64">
+      <c r="F4" s="62">
         <v>16.093779999999999</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="62">
         <v>0.88080999999999998</v>
       </c>
-      <c r="H4" s="69">
+      <c r="H4" s="67">
         <v>20.314550000000001</v>
       </c>
-      <c r="I4" s="69">
+      <c r="I4" s="67">
         <v>0.95567999999999997</v>
       </c>
       <c r="J4" s="14"/>
@@ -4850,22 +4995,22 @@
       <c r="C5" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="68">
+      <c r="D5" s="66">
         <v>14.874219999999999</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="66">
         <v>0.83862999999999999</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="66">
         <v>16.381509999999999</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="66">
         <v>0.88307000000000002</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="66">
         <v>20.566669999999998</v>
       </c>
-      <c r="I5" s="68">
+      <c r="I5" s="66">
         <v>0.95433999999999997</v>
       </c>
     </row>
@@ -4873,7 +5018,7 @@
       <c r="B6" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="59" t="s">
         <v>135</v>
       </c>
       <c r="D6" s="13">
@@ -4896,7 +5041,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="61">
+      <c r="A7" s="59">
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -4925,13 +5070,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="61">
+      <c r="A8" s="59">
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="61" t="s">
         <v>140</v>
       </c>
       <c r="D8" s="13">
@@ -4954,42 +5099,42 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="61">
+      <c r="A9" s="59">
         <v>10</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="60">
         <v>14.916359999999999</v>
       </c>
-      <c r="E9" s="62">
+      <c r="E9" s="60">
         <v>0.83982999999999997</v>
       </c>
-      <c r="F9" s="62">
+      <c r="F9" s="60">
         <v>16.407520000000002</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G9" s="60">
         <v>0.88507000000000002</v>
       </c>
-      <c r="H9" s="62">
+      <c r="H9" s="60">
         <v>20.710329999999999</v>
       </c>
-      <c r="I9" s="62">
+      <c r="I9" s="60">
         <v>0.95567000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="61">
+      <c r="A10" s="59">
         <v>11</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="59" t="s">
         <v>135</v>
       </c>
       <c r="D10" s="13">
@@ -5012,7 +5157,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="61">
+      <c r="A11" s="59">
         <v>12</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -5041,14 +5186,14 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="77" t="s">
+      <c r="C13" s="89"/>
+      <c r="D13" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="77"/>
+      <c r="E13" s="84"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
@@ -5060,10 +5205,10 @@
       <c r="C14" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="54" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5071,27 +5216,27 @@
       <c r="A15" s="19">
         <v>6</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="69">
+      <c r="D15" s="67">
         <v>14.84685</v>
       </c>
-      <c r="E15" s="69">
+      <c r="E15" s="67">
         <v>0.83896000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="61">
+      <c r="A16" s="59">
         <v>8</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="64" t="s">
         <v>137</v>
       </c>
       <c r="D16" s="13">
@@ -5102,13 +5247,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="61">
+      <c r="A17" s="59">
         <v>9</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="65" t="s">
         <v>140</v>
       </c>
       <c r="D17" s="13">
@@ -5119,31 +5264,31 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="61">
+      <c r="A18" s="59">
         <v>10</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="72">
+      <c r="D18" s="70">
         <v>14.916359999999999</v>
       </c>
-      <c r="E18" s="72">
+      <c r="E18" s="70">
         <v>0.83982999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="77" t="s">
+      <c r="C20" s="89"/>
+      <c r="D20" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="77"/>
+      <c r="E20" s="84"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
@@ -5152,32 +5297,32 @@
       <c r="C21" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="56" t="s">
+      <c r="E21" s="54" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D22" s="62">
         <v>16.093779999999999</v>
       </c>
-      <c r="E22" s="64">
+      <c r="E22" s="62">
         <v>0.88080999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="64" t="s">
         <v>137</v>
       </c>
       <c r="D23" s="13">
@@ -5188,10 +5333,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="65" t="s">
         <v>140</v>
       </c>
       <c r="D24" s="13">
@@ -5202,28 +5347,28 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="72">
+      <c r="D25" s="70">
         <v>16.407520000000002</v>
       </c>
-      <c r="E25" s="72">
+      <c r="E25" s="70">
         <v>0.88507000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="82" t="s">
+      <c r="B27" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="C27" s="82"/>
-      <c r="D27" s="77" t="s">
+      <c r="C27" s="89"/>
+      <c r="D27" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="77"/>
+      <c r="E27" s="84"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -5232,32 +5377,32 @@
       <c r="C28" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="54" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="69">
+      <c r="D29" s="67">
         <v>20.314550000000001</v>
       </c>
-      <c r="E29" s="69">
+      <c r="E29" s="67">
         <v>0.95567999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="64" t="s">
         <v>137</v>
       </c>
       <c r="D30" s="13">
@@ -5268,10 +5413,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="67" t="s">
+      <c r="C31" s="65" t="s">
         <v>140</v>
       </c>
       <c r="D31" s="13">
@@ -5282,16 +5427,16 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="70" t="s">
+      <c r="B32" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="C32" s="71" t="s">
+      <c r="C32" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="72">
+      <c r="D32" s="70">
         <v>20.710329999999999</v>
       </c>
-      <c r="E32" s="72">
+      <c r="E32" s="70">
         <v>0.95567000000000002</v>
       </c>
     </row>
@@ -5332,8 +5477,8 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -5356,10 +5501,10 @@
       <c r="A5" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="66">
+      <c r="C5" s="64">
         <v>4</v>
       </c>
       <c r="D5" t="s">
@@ -5373,7 +5518,7 @@
       <c r="A6" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="64" t="s">
         <v>148</v>
       </c>
       <c r="C6" s="19">
@@ -5390,10 +5535,10 @@
       <c r="A7" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="61">
+      <c r="C7" s="59">
         <v>4</v>
       </c>
       <c r="D7" t="s">
@@ -5407,10 +5552,10 @@
       <c r="A8" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="66">
+      <c r="C8" s="64">
         <v>4</v>
       </c>
       <c r="D8" t="s">
@@ -5424,10 +5569,10 @@
       <c r="A9" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="65">
         <v>6</v>
       </c>
       <c r="D9" t="s">
@@ -5441,10 +5586,10 @@
       <c r="A10" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="65">
         <v>6</v>
       </c>
       <c r="D10" t="s">
@@ -5458,10 +5603,10 @@
       <c r="A11" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="67">
+      <c r="C11" s="65">
         <v>6</v>
       </c>
       <c r="D11" t="s">
@@ -5475,10 +5620,10 @@
       <c r="A12" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="67">
+      <c r="C12" s="65">
         <v>6</v>
       </c>
       <c r="D12" t="s">

</xml_diff>

<commit_message>
Checkpoint for dehazing ablation study
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\SynthDehazing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CC7FB9-8A8A-41E6-89CB-7DCEA77737E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9442AA8-C97C-4BFC-9140-B6F60513E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -655,7 +655,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="188">
   <si>
     <t>PSNR</t>
   </si>
@@ -1008,15 +1008,6 @@
     <t>Ours - Default</t>
   </si>
   <si>
-    <t>Ours - No G_s</t>
-  </si>
-  <si>
-    <t>Ours - No G_s, No G_u</t>
-  </si>
-  <si>
-    <t>Ours - No G_u</t>
-  </si>
-  <si>
     <t>Ours - LR Synth</t>
   </si>
   <si>
@@ -1161,9 +1152,6 @@
     <t>Supervised, Single-Image</t>
   </si>
   <si>
-    <t>Supervised, Single Image</t>
-  </si>
-  <si>
     <t>Input image as reference</t>
   </si>
   <si>
@@ -1180,6 +1168,57 @@
   </si>
   <si>
     <t>B3 (L_lpips)</t>
+  </si>
+  <si>
+    <t>NYU Indoor + Make3D Outdoor</t>
+  </si>
+  <si>
+    <t>Unsupervised, Single Image</t>
+  </si>
+  <si>
+    <t>RESIDE ITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + RESIDE OTS</t>
+  </si>
+  <si>
+    <t>Model-Based</t>
+  </si>
+  <si>
+    <t>or optimization approach</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>$[0.7, 1.0]$</t>
+  </si>
+  <si>
+    <t>$[0.6, 1.8]$</t>
+  </si>
+  <si>
+    <t>$[0.1, 1.0]$</t>
+  </si>
+  <si>
+    <t>$[0.1, 1.8]$</t>
+  </si>
+  <si>
+    <t>$[0.35, 0.5]$</t>
+  </si>
+  <si>
+    <t>$[0.3, 0.9]$</t>
+  </si>
+  <si>
+    <t>$[0.05, 0.9]$</t>
+  </si>
+  <si>
+    <t>Ours - No $G_s$</t>
+  </si>
+  <si>
+    <t>Ours - No $G_u$</t>
+  </si>
+  <si>
+    <t>Ours - No $G_s$, No $G_u$</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1405,11 +1444,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1463,12 +1511,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1513,7 +1555,6 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1564,6 +1605,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1582,10 +1662,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1594,16 +1677,194 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="52">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2409,38 +2670,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="F1" s="94" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="F1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="K1" s="94" t="s">
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="K1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="94"/>
+      <c r="L1" s="118"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="94" t="s">
+      <c r="N1" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="94"/>
+      <c r="O1" s="118"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="94" t="s">
+      <c r="S1" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
+      <c r="V1" s="118"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3070,64 +3331,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="33" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="51" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="32" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="50" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="31" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="49" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="30" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="48" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="29" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="47" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="28" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="46" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="27" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="45" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="26" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="44" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="25" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="43" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="24" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="23" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="41" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="22" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="40" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="21" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="39" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="20" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="38" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="19" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="37" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="18" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="17" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="16" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="15" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="14" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3157,22 +3418,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="E1" s="94" t="s">
+      <c r="C1" s="118"/>
+      <c r="E1" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="94"/>
-      <c r="H1" s="94" t="s">
+      <c r="F1" s="118"/>
+      <c r="H1" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="94"/>
-      <c r="K1" s="94" t="s">
+      <c r="I1" s="118"/>
+      <c r="K1" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="94"/>
+      <c r="L1" s="118"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3636,22 +3897,22 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="13" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="12" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="9" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="8" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3662,8 +3923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:G18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3679,18 +3940,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="97" t="s">
+      <c r="C1" s="120"/>
+      <c r="D1" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="95"/>
-      <c r="F1" s="97" t="s">
+      <c r="E1" s="119"/>
+      <c r="F1" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="95"/>
+      <c r="G1" s="119"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15" t="s">
         <v>69</v>
@@ -3733,10 +3994,10 @@
       <c r="C3" s="24">
         <v>0.80076000000000003</v>
       </c>
-      <c r="D3" s="77">
+      <c r="D3" s="74">
         <v>13.25198</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E3" s="75">
         <v>0.85750000000000004</v>
       </c>
       <c r="F3" s="23">
@@ -3761,12 +4022,12 @@
         <v>58</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="77" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="26" t="s">
@@ -3793,10 +4054,10 @@
       <c r="C5" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="79" t="s">
         <v>60</v>
       </c>
       <c r="F5" s="23">
@@ -3823,10 +4084,10 @@
       <c r="C6" s="24">
         <v>0.79003000000000001</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="74">
         <v>14.733599999999999</v>
       </c>
-      <c r="E6" s="83">
+      <c r="E6" s="80">
         <v>0.86065999999999998</v>
       </c>
       <c r="F6" s="23">
@@ -3847,16 +4108,16 @@
       <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="35">
         <v>20.130600000000001</v>
       </c>
       <c r="C7" s="24">
         <v>0.77390000000000003</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="73">
         <v>16.80341</v>
       </c>
-      <c r="E7" s="83">
+      <c r="E7" s="80">
         <v>0.83260999999999996</v>
       </c>
       <c r="F7" s="23">
@@ -3877,16 +4138,16 @@
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="38">
         <v>18.2179</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="36">
         <v>0.85409999999999997</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="74">
         <v>15.921799999999999</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="80">
         <v>0.74519999999999997</v>
       </c>
       <c r="F8" s="23">
@@ -3913,10 +4174,10 @@
       <c r="C9" s="24">
         <v>0.80913000000000002</v>
       </c>
-      <c r="D9" s="77">
+      <c r="D9" s="74">
         <v>13.07117</v>
       </c>
-      <c r="E9" s="83">
+      <c r="E9" s="80">
         <v>0.83233999999999997</v>
       </c>
       <c r="F9" s="23">
@@ -3943,10 +4204,10 @@
       <c r="C10" s="24">
         <v>0.78044000000000002</v>
       </c>
-      <c r="D10" s="77">
+      <c r="D10" s="74">
         <v>12.753729999999999</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="80">
         <v>0.82584000000000002</v>
       </c>
       <c r="F10" s="23">
@@ -3973,10 +4234,10 @@
       <c r="C11" s="24">
         <v>0.81867999999999996</v>
       </c>
-      <c r="D11" s="77">
+      <c r="D11" s="74">
         <v>15.15972</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="80">
         <v>0.86604000000000003</v>
       </c>
       <c r="F11" s="23">
@@ -4003,10 +4264,10 @@
       <c r="C12" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="83" t="s">
+      <c r="E12" s="80" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="23">
@@ -4033,10 +4294,10 @@
       <c r="C13" s="24">
         <v>0.82333000000000001</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="35">
         <v>17.625070000000001</v>
       </c>
-      <c r="E13" s="83">
+      <c r="E13" s="80">
         <v>0.88229000000000002</v>
       </c>
       <c r="F13" s="23">
@@ -4063,13 +4324,13 @@
       <c r="C14" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="D14" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="35">
         <v>30.33</v>
       </c>
       <c r="G14" s="25">
@@ -4085,7 +4346,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B15" s="23">
         <v>17.29</v>
@@ -4093,10 +4354,10 @@
       <c r="C15" s="24">
         <v>0.82862000000000002</v>
       </c>
-      <c r="D15" s="77">
+      <c r="D15" s="74">
         <v>16.479649999999999</v>
       </c>
-      <c r="E15" s="83">
+      <c r="E15" s="80">
         <v>0.87983</v>
       </c>
       <c r="F15" s="23">
@@ -4107,12 +4368,12 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B16" s="23">
         <v>15.980639999999999</v>
@@ -4120,10 +4381,10 @@
       <c r="C16" s="24">
         <v>0.81313999999999997</v>
       </c>
-      <c r="D16" s="77">
+      <c r="D16" s="74">
         <v>15.48396</v>
       </c>
-      <c r="E16" s="83">
+      <c r="E16" s="80">
         <v>0.85555000000000003</v>
       </c>
       <c r="F16" s="23">
@@ -4137,7 +4398,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B17" s="23">
         <v>15.60083</v>
@@ -4145,41 +4406,41 @@
       <c r="C17" s="24">
         <v>0.79781999999999997</v>
       </c>
-      <c r="D17" s="77">
+      <c r="D17" s="74">
         <v>16.34646</v>
       </c>
-      <c r="E17" s="74">
+      <c r="E17" s="71">
         <v>0.88778000000000001</v>
       </c>
-      <c r="F17" s="76">
+      <c r="F17" s="73">
         <v>29.243469999999999</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="37">
         <v>0.96103000000000005</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="87">
+      <c r="B18" s="84">
         <v>16.07985</v>
       </c>
-      <c r="C18" s="88">
+      <c r="C18" s="85">
         <v>0.83992</v>
       </c>
-      <c r="D18" s="89">
+      <c r="D18" s="86">
         <v>16.16921</v>
       </c>
-      <c r="E18" s="90">
+      <c r="E18" s="87">
         <v>0.88885000000000003</v>
       </c>
-      <c r="F18" s="91">
+      <c r="F18" s="88">
         <v>20.49427</v>
       </c>
-      <c r="G18" s="92">
+      <c r="G18" s="89">
         <v>0.95567999999999997</v>
       </c>
       <c r="H18" s="14"/>
@@ -4189,27 +4450,27 @@
       <c r="A19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="35">
+      <c r="B19" s="33">
         <f>AVERAGE(B3,B6:B11, B13:B17)</f>
         <v>15.988634545454545</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="34">
         <f>AVERAGE(C3,C6:C11, C13:C17)</f>
         <v>0.8081772727272728</v>
       </c>
-      <c r="D19" s="84">
+      <c r="D19" s="81">
         <f>AVERAGE(D3,D6:D11, D13:D17)</f>
         <v>15.239140909090908</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="34">
         <f t="shared" ref="E19" si="0">AVERAGE(E3,E6:E11, E13:E17)</f>
         <v>0.84778545454545451</v>
       </c>
-      <c r="F19" s="35">
+      <c r="F19" s="33">
         <f>AVERAGE(F3,F5:F12, F13:F17)</f>
         <v>22.100981428571426</v>
       </c>
-      <c r="G19" s="35">
+      <c r="G19" s="33">
         <f>AVERAGE(G3,G5:G12, G13:G17)</f>
         <v>0.9222164285714286</v>
       </c>
@@ -4222,8 +4483,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
-        <v>161</v>
+      <c r="A20" s="56" t="s">
+        <v>158</v>
       </c>
       <c r="B20" s="5">
         <v>16.07985</v>
@@ -4251,37 +4512,37 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="99"/>
-      <c r="D22" s="98" t="s">
+      <c r="C22" s="123"/>
+      <c r="D22" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="99"/>
-      <c r="F22" s="95" t="s">
+      <c r="E22" s="123"/>
+      <c r="F22" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="95"/>
+      <c r="G22" s="119"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="53" t="s">
+      <c r="F23" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="53" t="s">
+      <c r="G23" s="51" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4292,16 +4553,16 @@
       <c r="B24" s="13">
         <v>14.02351</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C24" s="49">
         <v>0.81435000000000002</v>
       </c>
       <c r="D24" s="13">
         <v>15.275</v>
       </c>
-      <c r="E24" s="51">
+      <c r="E24" s="49">
         <v>0.86826000000000003</v>
       </c>
-      <c r="F24" s="85">
+      <c r="F24" s="82">
         <v>17.915420000000001</v>
       </c>
       <c r="G24" s="13">
@@ -4310,21 +4571,21 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="B25" s="13">
         <v>14.051920000000001</v>
       </c>
-      <c r="C25" s="51">
+      <c r="C25" s="49">
         <v>0.83204</v>
       </c>
       <c r="D25" s="13">
         <v>15.15972</v>
       </c>
-      <c r="E25" s="51">
+      <c r="E25" s="49">
         <v>0.86431000000000002</v>
       </c>
-      <c r="F25" s="85">
+      <c r="F25" s="82">
         <v>18.527529999999999</v>
       </c>
       <c r="G25" s="13">
@@ -4333,18 +4594,18 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>119</v>
+        <v>186</v>
       </c>
       <c r="B26" s="13">
         <v>13.87458</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="49">
         <v>0.82935000000000003</v>
       </c>
       <c r="D26" s="13">
         <v>15.59061</v>
       </c>
-      <c r="E26" s="51">
+      <c r="E26" s="49">
         <v>0.86753000000000002</v>
       </c>
       <c r="F26" s="13">
@@ -4356,18 +4617,18 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="B27" s="13">
         <v>12.76966</v>
       </c>
-      <c r="C27" s="51">
+      <c r="C27" s="49">
         <v>0.80222000000000004</v>
       </c>
       <c r="D27" s="13">
         <v>14.243539999999999</v>
       </c>
-      <c r="E27" s="51">
+      <c r="E27" s="49">
         <v>0.84404999999999997</v>
       </c>
       <c r="F27" s="13">
@@ -4379,18 +4640,18 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B28" s="13">
         <v>12.74478</v>
       </c>
-      <c r="C28" s="51">
+      <c r="C28" s="49">
         <v>0.79569000000000001</v>
       </c>
       <c r="D28" s="13">
         <v>14.030749999999999</v>
       </c>
-      <c r="E28" s="51">
+      <c r="E28" s="49">
         <v>0.82940000000000003</v>
       </c>
       <c r="F28" s="13">
@@ -4404,22 +4665,22 @@
       <c r="A29" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="39">
-        <v>14.94026</v>
-      </c>
-      <c r="C29" s="38">
+      <c r="B29" s="37">
+        <v>16.07985</v>
+      </c>
+      <c r="C29" s="36">
         <v>0.83992</v>
       </c>
-      <c r="D29" s="52">
+      <c r="D29" s="50">
         <v>16.16921</v>
       </c>
-      <c r="E29" s="55">
+      <c r="E29" s="53">
         <v>0.88885000000000003</v>
       </c>
-      <c r="F29" s="52">
+      <c r="F29" s="50">
         <v>20.49427</v>
       </c>
-      <c r="G29" s="52">
+      <c r="G29" s="50">
         <v>0.95567999999999997</v>
       </c>
     </row>
@@ -4427,23 +4688,23 @@
       <c r="A30" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="56">
-        <v>15.989433999999999</v>
-      </c>
-      <c r="C30" s="57">
-        <v>0.80768099999999998</v>
-      </c>
-      <c r="D30" s="56">
-        <v>15.214659000000001</v>
-      </c>
-      <c r="E30" s="57">
-        <v>0.84700900000000012</v>
-      </c>
-      <c r="F30" s="56">
-        <v>22.244054999999999</v>
-      </c>
-      <c r="G30" s="56">
-        <v>0.92008000000000012</v>
+      <c r="B30" s="54">
+        <v>15.988634545454545</v>
+      </c>
+      <c r="C30" s="55">
+        <v>0.8081772727272728</v>
+      </c>
+      <c r="D30" s="54">
+        <v>15.239140909090908</v>
+      </c>
+      <c r="E30" s="55">
+        <v>0.84778545454545451</v>
+      </c>
+      <c r="F30" s="54">
+        <v>22.100981428571426</v>
+      </c>
+      <c r="G30" s="54">
+        <v>0.9222164285714286</v>
       </c>
     </row>
   </sheetData>
@@ -4457,28 +4718,28 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="7" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:F1048576">
-    <cfRule type="top10" dxfId="6" priority="118" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="118" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C1048576">
-    <cfRule type="top10" dxfId="5" priority="121" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="23" priority="121" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D21 D31:D1048576">
-    <cfRule type="top10" dxfId="4" priority="124" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="22" priority="124" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E21 E31:E1048576">
-    <cfRule type="top10" dxfId="3" priority="128" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="128" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F21 F31:F1048576">
-    <cfRule type="top10" dxfId="2" priority="132" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="132" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H1048576 G20:H21 H2:H19 G31:G1048576">
-    <cfRule type="top10" dxfId="1" priority="136" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="136" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H1048576 H2 G31:G1048576">
-    <cfRule type="top10" dxfId="0" priority="144" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="144" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4488,218 +4749,256 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90921C0C-3EF8-488C-A8AD-77E45C51350D}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="24" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="97" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="E1" s="98"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
+        <f>ROW(A2) - 1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="100" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="100" t="s">
+      <c r="C2" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="126" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
+        <f t="shared" ref="A3:A17" si="0">ROW(A3) - 1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="C3" s="101" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="126"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="96" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="D4" s="126"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C7" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D7" s="72" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="33" t="s">
+      <c r="C8" s="125"/>
+      <c r="D8" s="31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="100" t="s">
+      <c r="C9" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="100" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="D9" s="99" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="126"/>
+      <c r="D10" s="101" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="126"/>
+      <c r="D11" s="99"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>11</v>
-      </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="126"/>
+      <c r="D12" s="99"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="125"/>
+      <c r="D13" s="100"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C14" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D14" s="32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="75" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="75" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="100" t="s">
+      <c r="C16" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D16" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>13</v>
-      </c>
-      <c r="B16" s="10" t="s">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="33" t="s">
+      <c r="C17" s="125"/>
+      <c r="D17" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="8"/>
+      <c r="G17" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C2:C4"/>
+  <mergeCells count="4">
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4722,63 +5021,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="127" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="43" t="s">
-        <v>162</v>
+      <c r="C1" s="127"/>
+      <c r="D1" s="41" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="40" t="s">
         <v>105</v>
       </c>
       <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="72">
+        <v>162</v>
+      </c>
+      <c r="B3" s="69">
         <v>0.3</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="39">
         <v>1000</v>
       </c>
-      <c r="D3" s="70">
+      <c r="D3" s="67">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" s="72">
+        <v>160</v>
+      </c>
+      <c r="B4" s="69">
         <v>0.3</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="39">
         <v>1000</v>
       </c>
-      <c r="D4" s="70">
+      <c r="D4" s="67">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="73">
+        <v>161</v>
+      </c>
+      <c r="B5" s="70">
         <v>0.3</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="42">
         <v>100</v>
       </c>
-      <c r="D5" s="71">
+      <c r="D5" s="68">
         <v>60</v>
       </c>
     </row>
@@ -4789,26 +5088,26 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="127" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="102" t="s">
+      <c r="B7" s="127"/>
+      <c r="C7" s="127" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="102"/>
+      <c r="D7" s="127"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="43">
         <v>1024</v>
       </c>
       <c r="C8" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="45">
         <v>1</v>
       </c>
     </row>
@@ -4816,13 +5115,13 @@
       <c r="A9" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="43">
         <v>1024</v>
       </c>
       <c r="C9" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="39">
         <v>25</v>
       </c>
     </row>
@@ -4830,13 +5129,13 @@
       <c r="A10" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="44">
         <v>1024</v>
       </c>
       <c r="C10" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="39">
         <v>25</v>
       </c>
     </row>
@@ -4844,14 +5143,14 @@
       <c r="A11" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="46">
         <v>2</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="49"/>
+      <c r="D11" s="47"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="50"/>
+      <c r="C13" s="48"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
@@ -4860,52 +5159,52 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>126</v>
+      <c r="B15" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C19" s="9"/>
     </row>
@@ -4922,10 +5221,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3513DC-2654-45B1-823E-7102A41B0B3D}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4934,10 +5233,11 @@
     <col min="2" max="2" width="12.85546875" style="19" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="19" customWidth="1"/>
     <col min="4" max="9" width="18.7109375" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="19"/>
+    <col min="10" max="10" width="16.85546875" style="19" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -4947,118 +5247,118 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="98" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="128"/>
+      <c r="D2" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98" t="s">
+      <c r="E2" s="122"/>
+      <c r="F2" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98" t="s">
+      <c r="G2" s="122"/>
+      <c r="H2" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="98"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="122"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="51" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>6</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="66">
-        <v>14.84685</v>
-      </c>
-      <c r="E4" s="66">
-        <v>0.83896000000000004</v>
-      </c>
-      <c r="F4" s="61">
-        <v>16.093779999999999</v>
-      </c>
-      <c r="G4" s="61">
-        <v>0.88080999999999998</v>
-      </c>
-      <c r="H4" s="66">
-        <v>20.314550000000001</v>
-      </c>
-      <c r="I4" s="66">
+        <v>132</v>
+      </c>
+      <c r="D4" s="63">
+        <v>16.07985</v>
+      </c>
+      <c r="E4" s="63">
+        <v>0.83992</v>
+      </c>
+      <c r="F4" s="58">
+        <v>16.16921</v>
+      </c>
+      <c r="G4" s="58">
+        <v>0.88885000000000003</v>
+      </c>
+      <c r="H4" s="63">
+        <v>20.49427</v>
+      </c>
+      <c r="I4" s="63">
         <v>0.95567999999999997</v>
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>7</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="65">
+        <v>134</v>
+      </c>
+      <c r="D5" s="62">
         <v>14.874219999999999</v>
       </c>
-      <c r="E5" s="65">
+      <c r="E5" s="62">
         <v>0.83862999999999999</v>
       </c>
-      <c r="F5" s="65">
+      <c r="F5" s="62">
         <v>16.381509999999999</v>
       </c>
-      <c r="G5" s="65">
+      <c r="G5" s="62">
         <v>0.88307000000000002</v>
       </c>
-      <c r="H5" s="65">
+      <c r="H5" s="62">
         <v>20.566669999999998</v>
       </c>
-      <c r="I5" s="65">
+      <c r="I5" s="62">
         <v>0.95433999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="58" t="s">
         <v>135</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>132</v>
       </c>
       <c r="D6" s="13">
         <v>14.66441</v>
@@ -5079,15 +5379,15 @@
         <v>0.95398000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="58">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="56">
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" s="13">
         <v>14.184150000000001</v>
@@ -5108,15 +5408,15 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="58">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="56">
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" s="60" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>137</v>
       </c>
       <c r="D8" s="13">
         <v>14.59496</v>
@@ -5137,44 +5437,44 @@
         <v>0.95042000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="58">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="56">
         <v>10</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D9" s="59">
+        <v>136</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="103">
         <v>14.916359999999999</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="103">
         <v>0.83982999999999997</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="103">
         <v>16.407520000000002</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="103">
         <v>0.88507000000000002</v>
       </c>
-      <c r="H9" s="59">
+      <c r="H9" s="103">
         <v>20.710329999999999</v>
       </c>
-      <c r="I9" s="59">
+      <c r="I9" s="103">
         <v>0.95567000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="58">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="56">
         <v>11</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="58" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>132</v>
       </c>
       <c r="D10" s="13">
         <v>14.809279999999999</v>
@@ -5195,15 +5495,15 @@
         <v>0.95442000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="58">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="56">
         <v>12</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D11" s="13">
         <v>14.78022</v>
@@ -5224,225 +5524,251 @@
         <v>0.95211000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="103" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" s="103"/>
-      <c r="D13" s="98" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="128"/>
+      <c r="D13" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="98"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="122"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="51" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>6</v>
       </c>
-      <c r="B15" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="66">
-        <v>14.84685</v>
-      </c>
-      <c r="E15" s="66">
-        <v>0.83896000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="58">
+      <c r="B15" s="131" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" s="131" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="117">
+        <v>16.07985</v>
+      </c>
+      <c r="E15" s="117">
+        <v>0.83992</v>
+      </c>
+      <c r="G15" s="84">
+        <v>16.07985</v>
+      </c>
+      <c r="H15" s="85">
+        <v>0.83992</v>
+      </c>
+      <c r="I15" s="86">
+        <v>16.16921</v>
+      </c>
+      <c r="J15" s="87">
+        <v>0.88885000000000003</v>
+      </c>
+      <c r="K15" s="88">
+        <v>20.49427</v>
+      </c>
+      <c r="L15" s="89">
+        <v>0.95567999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="56">
         <v>8</v>
       </c>
-      <c r="B16" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="63" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" s="13">
+      <c r="B16" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" s="62">
         <v>14.184150000000001</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="62">
         <v>0.82316</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="58">
+      <c r="A17" s="56">
         <v>9</v>
       </c>
-      <c r="B17" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>140</v>
-      </c>
-      <c r="D17" s="13">
+      <c r="B17" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17" s="62">
         <v>14.59496</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="62">
         <v>0.83475999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="58">
+      <c r="A18" s="56">
         <v>10</v>
       </c>
-      <c r="B18" s="67" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="68" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="69">
+      <c r="B18" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="129">
         <v>14.916359999999999</v>
       </c>
-      <c r="E18" s="69">
+      <c r="E18" s="129">
         <v>0.83982999999999997</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+    </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="103" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="103"/>
-      <c r="D20" s="98" t="s">
+      <c r="B20" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="128"/>
+      <c r="D20" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="98"/>
+      <c r="E20" s="122"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D21" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="51" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="C22" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="61">
-        <v>16.093779999999999</v>
-      </c>
-      <c r="E22" s="61">
-        <v>0.88080999999999998</v>
+      <c r="B22" s="131" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="131" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="58">
+        <v>16.16921</v>
+      </c>
+      <c r="E22" s="117">
+        <v>0.88885000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="13">
+      <c r="B23" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" s="62">
         <v>14.79847</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="62">
         <v>0.84397999999999995</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="13">
+      <c r="B24" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" s="62">
         <v>15.852830000000001</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="62">
         <v>0.87751999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="67" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="68" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="69">
+      <c r="B25" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" s="130">
         <v>16.407520000000002</v>
       </c>
-      <c r="E25" s="69">
+      <c r="E25" s="129">
         <v>0.88507000000000002</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+    </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="103" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="103"/>
-      <c r="D27" s="98" t="s">
+      <c r="B27" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="128"/>
+      <c r="D27" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="98"/>
+      <c r="E27" s="122"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="53" t="s">
+      <c r="E28" s="51" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="D29" s="66">
-        <v>20.314550000000001</v>
-      </c>
-      <c r="E29" s="66">
+      <c r="B29" s="131" t="s">
+        <v>178</v>
+      </c>
+      <c r="C29" s="131" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="63">
+        <v>20.49427</v>
+      </c>
+      <c r="E29" s="117">
         <v>0.95567999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="63" t="s">
-        <v>137</v>
+      <c r="B30" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>181</v>
       </c>
       <c r="D30" s="13">
         <v>19.391069999999999</v>
@@ -5452,11 +5778,11 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="64" t="s">
-        <v>140</v>
+      <c r="B31" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>183</v>
       </c>
       <c r="D31" s="13">
         <v>20.0871</v>
@@ -5466,271 +5792,755 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="67" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="68" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="69">
+      <c r="B32" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="D32" s="66">
         <v>20.710329999999999</v>
       </c>
-      <c r="E32" s="69">
+      <c r="E32" s="112">
         <v>0.95567000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="103" t="s">
-        <v>133</v>
-      </c>
-      <c r="C35" s="103"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="98" t="s">
+      <c r="B35" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="128"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="98"/>
-      <c r="G35" s="98" t="s">
+      <c r="F35" s="122"/>
+      <c r="G35" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="98"/>
-      <c r="I35" s="98" t="s">
+      <c r="H35" s="122"/>
+      <c r="I35" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="98"/>
+      <c r="J35" s="122"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="F36" s="53" t="s">
+      <c r="F36" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="G36" s="53" t="s">
+      <c r="G36" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="H36" s="53" t="s">
+      <c r="H36" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="I36" s="53" t="s">
+      <c r="I36" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="J36" s="53" t="s">
+      <c r="J36" s="51" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="107">
+      <c r="A37" s="105">
         <v>13</v>
       </c>
-      <c r="B37" s="105">
+      <c r="B37" s="106">
         <v>10</v>
       </c>
-      <c r="C37" s="105">
+      <c r="C37" s="106">
         <v>5</v>
       </c>
-      <c r="D37" s="105">
+      <c r="D37" s="106">
         <v>0</v>
       </c>
-      <c r="E37" s="87">
+      <c r="E37" s="107">
         <v>16.07985</v>
       </c>
-      <c r="F37" s="88">
+      <c r="F37" s="104">
         <v>0.83992</v>
       </c>
-      <c r="G37" s="89">
+      <c r="G37" s="88">
         <v>16.16921</v>
       </c>
-      <c r="H37" s="90">
+      <c r="H37" s="104">
         <v>0.88885000000000003</v>
       </c>
-      <c r="I37" s="91">
+      <c r="I37" s="88">
         <v>20.49427</v>
       </c>
-      <c r="J37" s="92">
+      <c r="J37" s="104">
         <v>0.95567999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="107">
+      <c r="A38" s="105">
         <v>14</v>
       </c>
-      <c r="B38" s="104">
+      <c r="B38" s="106">
         <v>5</v>
       </c>
-      <c r="C38" s="104">
+      <c r="C38" s="106">
         <v>10</v>
       </c>
-      <c r="D38" s="105">
+      <c r="D38" s="106">
         <v>0</v>
       </c>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
+      <c r="E38" s="108">
+        <v>13.8056</v>
+      </c>
+      <c r="F38" s="25">
+        <v>0.80891999999999997</v>
+      </c>
+      <c r="G38" s="25">
+        <v>15.778639999999999</v>
+      </c>
+      <c r="H38" s="25">
+        <v>0.87277000000000005</v>
+      </c>
+      <c r="I38" s="108">
+        <v>20.120709999999999</v>
+      </c>
+      <c r="J38" s="108">
+        <v>0.94513999999999998</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="107">
+      <c r="A39" s="105">
         <v>15</v>
       </c>
-      <c r="B39" s="104">
+      <c r="B39" s="106">
         <v>10</v>
       </c>
-      <c r="C39" s="104">
+      <c r="C39" s="106">
         <v>10</v>
       </c>
-      <c r="D39" s="105">
+      <c r="D39" s="106">
         <v>0</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="E39" s="108">
+        <v>14.84554</v>
+      </c>
+      <c r="F39" s="108">
+        <v>0.83860000000000001</v>
+      </c>
+      <c r="G39" s="108">
+        <v>14.254630000000001</v>
+      </c>
+      <c r="H39" s="108">
+        <v>0.82321</v>
+      </c>
+      <c r="I39" s="108">
+        <v>20.50639</v>
+      </c>
+      <c r="J39" s="108">
+        <v>0.95504</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="107">
+      <c r="A40" s="105">
         <v>16</v>
       </c>
-      <c r="B40" s="105">
+      <c r="B40" s="106">
         <v>10</v>
       </c>
-      <c r="C40" s="105">
+      <c r="C40" s="106">
         <v>0</v>
       </c>
-      <c r="D40" s="105">
+      <c r="D40" s="106">
         <v>0</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="E40" s="108">
+        <v>14.88763</v>
+      </c>
+      <c r="F40" s="108">
+        <v>0.83892999999999995</v>
+      </c>
+      <c r="G40" s="109">
+        <v>16.411840000000002</v>
+      </c>
+      <c r="H40" s="108">
+        <v>0.88512999999999997</v>
+      </c>
+      <c r="I40" s="109">
+        <v>20.724270000000001</v>
+      </c>
+      <c r="J40" s="108">
+        <v>0.95513999999999999</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="107">
+      <c r="A41" s="94">
         <v>17</v>
       </c>
-      <c r="B41" s="105">
+      <c r="B41" s="92">
         <v>0</v>
       </c>
-      <c r="C41" s="106">
+      <c r="C41" s="93">
         <v>10</v>
       </c>
-      <c r="D41" s="105">
+      <c r="D41" s="92">
         <v>0</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
+      <c r="E41" s="103">
+        <v>8.17394</v>
+      </c>
+      <c r="F41" s="103">
+        <v>0.47650999999999999</v>
+      </c>
+      <c r="G41" s="103">
+        <v>8.3447999999999993</v>
+      </c>
+      <c r="H41" s="103">
+        <v>0.58896000000000004</v>
+      </c>
+      <c r="I41" s="13">
+        <v>10.76324</v>
+      </c>
+      <c r="J41" s="13">
+        <v>0.64602999999999999</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="107">
+      <c r="A42" s="94">
         <v>18</v>
       </c>
-      <c r="B42" s="105">
+      <c r="B42" s="92">
         <v>10</v>
       </c>
-      <c r="C42" s="105">
+      <c r="C42" s="92">
         <v>5</v>
       </c>
-      <c r="D42" s="104">
+      <c r="D42" s="91">
         <v>1</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="E42" s="13">
+        <v>14.95445</v>
+      </c>
+      <c r="F42" s="13">
+        <v>0.84072999999999998</v>
+      </c>
+      <c r="G42" s="13">
+        <v>16.049250000000001</v>
+      </c>
+      <c r="H42" s="13">
+        <v>0.87604000000000004</v>
+      </c>
       <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="107">
+      <c r="A43" s="94">
         <v>19</v>
       </c>
-      <c r="B43" s="104">
+      <c r="B43" s="91">
         <v>5</v>
       </c>
-      <c r="C43" s="104">
+      <c r="C43" s="91">
         <v>10</v>
       </c>
-      <c r="D43" s="104">
+      <c r="D43" s="91">
         <v>1</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="E43" s="13">
+        <v>14.400690000000001</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0.82279000000000002</v>
+      </c>
+      <c r="G43" s="13">
+        <v>15.01248</v>
+      </c>
+      <c r="H43" s="13">
+        <v>0.84702999999999995</v>
+      </c>
       <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="108">
+      <c r="A44" s="95">
         <v>20</v>
       </c>
-      <c r="B44" s="104">
+      <c r="B44" s="91">
         <v>10</v>
       </c>
-      <c r="C44" s="104">
+      <c r="C44" s="91">
         <v>10</v>
       </c>
-      <c r="D44" s="104">
+      <c r="D44" s="91">
         <v>1</v>
       </c>
+      <c r="E44" s="13">
+        <v>14.77398</v>
+      </c>
+      <c r="F44" s="13">
+        <v>0.83750999999999998</v>
+      </c>
+      <c r="G44" s="13">
+        <v>15.38954</v>
+      </c>
+      <c r="H44" s="13">
+        <v>0.86206000000000005</v>
+      </c>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="108">
+      <c r="A45" s="95">
         <v>21</v>
       </c>
-      <c r="B45" s="105">
+      <c r="B45" s="92">
         <v>10</v>
       </c>
-      <c r="C45" s="105">
+      <c r="C45" s="92">
         <v>0</v>
       </c>
-      <c r="D45" s="104">
+      <c r="D45" s="91">
         <v>1</v>
       </c>
+      <c r="E45" s="13">
+        <v>14.836040000000001</v>
+      </c>
+      <c r="F45" s="13">
+        <v>0.83808000000000005</v>
+      </c>
+      <c r="G45" s="13">
+        <v>16.027190000000001</v>
+      </c>
+      <c r="H45" s="13">
+        <v>0.87643000000000004</v>
+      </c>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="108">
+      <c r="A46" s="95">
         <v>22</v>
       </c>
-      <c r="B46" s="105">
+      <c r="B46" s="92">
         <v>0</v>
       </c>
-      <c r="C46" s="106">
+      <c r="C46" s="93">
         <v>10</v>
       </c>
-      <c r="D46" s="104">
+      <c r="D46" s="91">
         <v>1</v>
       </c>
+      <c r="E46" s="13">
+        <v>14.85346</v>
+      </c>
+      <c r="F46" s="13">
+        <v>0.83828000000000003</v>
+      </c>
+      <c r="G46" s="13">
+        <v>16.27073</v>
+      </c>
+      <c r="H46" s="13">
+        <v>0.88234999999999997</v>
+      </c>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="128"/>
+      <c r="D50" s="122" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="122"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="102" t="s">
+        <v>177</v>
+      </c>
+      <c r="D51" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="115">
+        <v>10</v>
+      </c>
+      <c r="C52" s="115">
+        <v>5</v>
+      </c>
+      <c r="D52" s="114">
+        <v>16.07985</v>
+      </c>
+      <c r="E52" s="114">
+        <v>0.83992</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="106">
+        <v>5</v>
+      </c>
+      <c r="C53" s="106">
+        <v>10</v>
+      </c>
+      <c r="D53" s="108">
+        <v>13.8056</v>
+      </c>
+      <c r="E53" s="25">
+        <v>0.80891999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="106">
+        <v>10</v>
+      </c>
+      <c r="C54" s="106">
+        <v>10</v>
+      </c>
+      <c r="D54" s="108">
+        <v>14.84554</v>
+      </c>
+      <c r="E54" s="108">
+        <v>0.83860000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="106">
+        <v>10</v>
+      </c>
+      <c r="C55" s="106">
+        <v>0</v>
+      </c>
+      <c r="D55" s="108">
+        <v>14.88763</v>
+      </c>
+      <c r="E55" s="108">
+        <v>0.83892999999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="110">
+        <v>0</v>
+      </c>
+      <c r="C56" s="111">
+        <v>10</v>
+      </c>
+      <c r="D56" s="112">
+        <v>8.17394</v>
+      </c>
+      <c r="E56" s="112">
+        <v>0.47650999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="92"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="128"/>
+      <c r="D58" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" s="122"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="102" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="115">
+        <v>10</v>
+      </c>
+      <c r="C60" s="115">
+        <v>5</v>
+      </c>
+      <c r="D60" s="116">
+        <v>16.16921</v>
+      </c>
+      <c r="E60" s="114">
+        <v>0.88885000000000003</v>
+      </c>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="106">
+        <v>5</v>
+      </c>
+      <c r="C61" s="106">
+        <v>10</v>
+      </c>
+      <c r="D61" s="25">
+        <v>15.778639999999999</v>
+      </c>
+      <c r="E61" s="25">
+        <v>0.87277000000000005</v>
+      </c>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="106">
+        <v>10</v>
+      </c>
+      <c r="C62" s="106">
+        <v>10</v>
+      </c>
+      <c r="D62" s="108">
+        <v>14.254630000000001</v>
+      </c>
+      <c r="E62" s="108">
+        <v>0.82321</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="106">
+        <v>10</v>
+      </c>
+      <c r="C63" s="106">
+        <v>0</v>
+      </c>
+      <c r="D63" s="109">
+        <v>16.411840000000002</v>
+      </c>
+      <c r="E63" s="108">
+        <v>0.88512999999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="110">
+        <v>0</v>
+      </c>
+      <c r="C64" s="111">
+        <v>10</v>
+      </c>
+      <c r="D64" s="112">
+        <v>8.3447999999999993</v>
+      </c>
+      <c r="E64" s="112">
+        <v>0.58896000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="128"/>
+      <c r="D66" s="122" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" s="122"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" s="102" t="s">
+        <v>177</v>
+      </c>
+      <c r="D67" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="115">
+        <v>10</v>
+      </c>
+      <c r="C68" s="115">
+        <v>5</v>
+      </c>
+      <c r="D68" s="116">
+        <v>20.49427</v>
+      </c>
+      <c r="E68" s="114">
+        <v>0.95567999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="106">
+        <v>5</v>
+      </c>
+      <c r="C69" s="106">
+        <v>10</v>
+      </c>
+      <c r="D69" s="108">
+        <v>20.120709999999999</v>
+      </c>
+      <c r="E69" s="108">
+        <v>0.94513999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="106">
+        <v>10</v>
+      </c>
+      <c r="C70" s="106">
+        <v>10</v>
+      </c>
+      <c r="D70" s="108">
+        <v>20.50639</v>
+      </c>
+      <c r="E70" s="108">
+        <v>0.95504</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="106">
+        <v>10</v>
+      </c>
+      <c r="C71" s="106">
+        <v>0</v>
+      </c>
+      <c r="D71" s="109">
+        <v>20.724270000000001</v>
+      </c>
+      <c r="E71" s="108">
+        <v>0.95513999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="110">
+        <v>0</v>
+      </c>
+      <c r="C72" s="111">
+        <v>10</v>
+      </c>
+      <c r="D72" s="113">
+        <v>10.76324</v>
+      </c>
+      <c r="E72" s="113">
+        <v>0.64602999999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
+  <mergeCells count="20">
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B58:C58"/>
   </mergeCells>
+  <conditionalFormatting sqref="E41:E46">
+    <cfRule type="top10" dxfId="17" priority="19" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41:F46">
+    <cfRule type="top10" dxfId="16" priority="18" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41:G46">
+    <cfRule type="top10" dxfId="15" priority="17" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41:H46">
+    <cfRule type="top10" dxfId="14" priority="16" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41:I46">
+    <cfRule type="top10" dxfId="13" priority="15" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:J46">
+    <cfRule type="top10" dxfId="12" priority="14" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F57:F61">
+    <cfRule type="top10" dxfId="11" priority="10" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G57:G61">
+    <cfRule type="top10" dxfId="10" priority="9" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57:H61">
+    <cfRule type="top10" dxfId="9" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I57:I61">
+    <cfRule type="top10" dxfId="8" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="top10" dxfId="7" priority="151" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="top10" dxfId="6" priority="152" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D11">
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E11">
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F11">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G11">
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H11">
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I11">
+    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5741,7 +6551,7 @@
   <dimension ref="A3:E12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5755,160 +6565,160 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="E4" t="s">
         <v>144</v>
-      </c>
-      <c r="D4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="60">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="E5" t="s">
         <v>148</v>
-      </c>
-      <c r="C5" s="63">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6" s="63" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>145</v>
       </c>
       <c r="C6" s="19">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="56">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="58">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>151</v>
-      </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="63" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="63">
+        <v>151</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="60">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="64">
+        <v>152</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="61">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="64">
+        <v>154</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="61">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="64">
+        <v>155</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="61">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="64" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="64">
+      <c r="B12" s="61" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="61">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkpoint for manuscript revisions
</commit_message>
<xml_diff>
--- a/Model Performances.xlsx
+++ b/Model Performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\SynthDehazing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9442AA8-C97C-4BFC-9140-B6F60513E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF079A70-5C70-4E41-ADF9-1C12FAF235F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41430" yWindow="1485" windowWidth="34320" windowHeight="18645" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,6 +639,51 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={DAFD5C01-8488-4F38-A1CF-748DF34F16ED}</author>
+    <author>tc={92387C7C-B96A-40FF-AA8E-D98252008EBA}</author>
+    <author>tc={B59F46EF-F3E8-48A7-9A2B-7F43A1A8F270}</author>
+    <author>tc={E07435FA-1C6E-407E-B7B9-44BFB5DA10D9}</author>
+  </authors>
+  <commentList>
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{DAFD5C01-8488-4F38-A1CF-748DF34F16ED}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    V1.16.XX.T - 32x32</t>
+      </text>
+    </comment>
+    <comment ref="A75" authorId="1" shapeId="0" xr:uid="{92387C7C-B96A-40FF-AA8E-D98252008EBA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    V1.21.XX.T / V1.16.6.A - For GTA-Synth</t>
+      </text>
+    </comment>
+    <comment ref="A83" authorId="2" shapeId="0" xr:uid="{B59F46EF-F3E8-48A7-9A2B-7F43A1A8F270}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    V1.22.XX.T / V1.16.6.A - For GTA-Synth. With style stransfer, unlit enabled.</t>
+      </text>
+    </comment>
+    <comment ref="A92" authorId="3" shapeId="0" xr:uid="{E07435FA-1C6E-407E-B7B9-44BFB5DA10D9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    V1.16.17.T - 64x64 / V1.16.6.A</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={E9B111FA-E07A-40E3-A1B3-535FD6847041}</author>
   </authors>
   <commentList>
@@ -655,7 +700,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="194">
   <si>
     <t>PSNR</t>
   </si>
@@ -1131,9 +1176,6 @@
     <t>0.4 &lt; X &lt; 0. 41</t>
   </si>
   <si>
-    <t>V1.16.6</t>
-  </si>
-  <si>
     <t>Frustrum</t>
   </si>
   <si>
@@ -1219,6 +1261,27 @@
   </si>
   <si>
     <t>Ours - No $G_s$, No $G_u$</t>
+  </si>
+  <si>
+    <t>V1.16.18.T / V1.16.7.A</t>
+  </si>
+  <si>
+    <t>V1.16.6.T/V1.16.6.A</t>
+  </si>
+  <si>
+    <t>V1.16.6.T/V1.16.7 A</t>
+  </si>
+  <si>
+    <t>DLSU-SYNSIDE (Ours)</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>GTA-MVS (With $G_s$, $G_u$)</t>
+  </si>
+  <si>
+    <t>GTA-MVS (Without $G_s$, $G_u$)</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1644,6 +1707,18 @@
     <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1677,14 +1752,193 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2642,6 +2896,23 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A36" dT="2022-03-29T02:45:53.48" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{DAFD5C01-8488-4F38-A1CF-748DF34F16ED}">
+    <text>V1.16.XX.T - 32x32</text>
+  </threadedComment>
+  <threadedComment ref="A75" dT="2022-03-27T13:30:41.48" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{92387C7C-B96A-40FF-AA8E-D98252008EBA}">
+    <text>V1.21.XX.T / V1.16.6.A - For GTA-Synth</text>
+  </threadedComment>
+  <threadedComment ref="A83" dT="2022-03-27T13:30:41.48" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{B59F46EF-F3E8-48A7-9A2B-7F43A1A8F270}">
+    <text>V1.22.XX.T / V1.16.6.A - For GTA-Synth. With style stransfer, unlit enabled.</text>
+  </threadedComment>
+  <threadedComment ref="A92" dT="2022-03-29T02:45:53.48" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{E07435FA-1C6E-407E-B7B9-44BFB5DA10D9}">
+    <text>V1.16.17.T - 64x64 / V1.16.6.A</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A5" dT="2021-09-20T12:49:56.45" personId="{59384D5B-2A0D-4F76-A279-2B1ACCEC3898}" id="{E9B111FA-E07A-40E3-A1B3-535FD6847041}">
     <text>V1.14.4 on CCS Jupyter</text>
   </threadedComment>
@@ -2670,38 +2941,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="F1" s="118" t="s">
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="F1" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="K1" s="118" t="s">
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="K1" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="118"/>
+      <c r="L1" s="124"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="118" t="s">
+      <c r="N1" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="118"/>
+      <c r="O1" s="124"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="2"/>
-      <c r="S1" s="118" t="s">
+      <c r="S1" s="124" t="s">
         <v>94</v>
       </c>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118"/>
-      <c r="V1" s="118"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3331,64 +3602,64 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L3:L15">
-    <cfRule type="top10" dxfId="51" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="69" priority="24" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="top10" dxfId="50" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="68" priority="23" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I19 I21:I1048576">
-    <cfRule type="top10" dxfId="49" priority="22" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="67" priority="22" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H19 H21:H1048576">
-    <cfRule type="top10" dxfId="48" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="21" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G19 G21:G1048576">
-    <cfRule type="top10" dxfId="47" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="65" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="46" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="64" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="45" priority="18" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="63" priority="18" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="44" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="62" priority="17" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G31">
-    <cfRule type="top10" dxfId="43" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="61" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="top10" dxfId="42" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="60" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I32">
-    <cfRule type="top10" dxfId="41" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="59" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1">
-    <cfRule type="top10" dxfId="40" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="58" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="top10" dxfId="39" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="57" priority="8" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="top10" dxfId="38" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="56" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="top10" dxfId="37" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="55" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2">
-    <cfRule type="top10" dxfId="36" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="54" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="top10" dxfId="35" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="53" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="top10" dxfId="34" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="52" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="top10" dxfId="33" priority="2" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="51" priority="2" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="top10" dxfId="32" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="50" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3418,22 +3689,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="118"/>
-      <c r="E1" s="118" t="s">
+      <c r="C1" s="124"/>
+      <c r="E1" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="118"/>
-      <c r="H1" s="118" t="s">
+      <c r="F1" s="124"/>
+      <c r="H1" s="124" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="118"/>
-      <c r="K1" s="118" t="s">
+      <c r="I1" s="124"/>
+      <c r="K1" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="118"/>
+      <c r="L1" s="124"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3897,22 +4168,22 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="top10" dxfId="31" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="49" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="30" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="48" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="29" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="47" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="28" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="46" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="27" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="45" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="26" priority="1" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="44" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3921,10 +4192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655BD48-B478-4809-9D5B-43D478C11851}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3940,18 +4211,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="121" t="s">
+      <c r="C1" s="126"/>
+      <c r="D1" s="127" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="119"/>
-      <c r="F1" s="121" t="s">
+      <c r="E1" s="125"/>
+      <c r="F1" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="119"/>
+      <c r="G1" s="125"/>
       <c r="H1" s="18"/>
       <c r="I1" s="15" t="s">
         <v>69</v>
@@ -4346,7 +4617,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" s="23">
         <v>17.29</v>
@@ -4368,12 +4639,12 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" s="23">
         <v>15.980639999999999</v>
@@ -4398,7 +4669,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" s="23">
         <v>15.60083</v>
@@ -4484,7 +4755,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="B20" s="5">
         <v>16.07985</v>
@@ -4502,208 +4773,238 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="A21" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="13">
+        <v>15.079890000000001</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.84041999999999994</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="122" t="s">
+      <c r="A22" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="13">
+        <v>15.07785</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.84108000000000005</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="123"/>
-      <c r="D22" s="122" t="s">
+      <c r="C24" s="129"/>
+      <c r="D24" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="123"/>
-      <c r="F22" s="119" t="s">
+      <c r="E24" s="129"/>
+      <c r="F24" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="119"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="51" t="s">
+      <c r="G24" s="125"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C25" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D25" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E25" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="51" t="s">
+      <c r="F25" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="51" t="s">
+      <c r="G25" s="51" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="13">
-        <v>14.02351</v>
-      </c>
-      <c r="C24" s="49">
-        <v>0.81435000000000002</v>
-      </c>
-      <c r="D24" s="13">
-        <v>15.275</v>
-      </c>
-      <c r="E24" s="49">
-        <v>0.86826000000000003</v>
-      </c>
-      <c r="F24" s="82">
-        <v>17.915420000000001</v>
-      </c>
-      <c r="G24" s="13">
-        <v>0.94120999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="B25" s="13">
-        <v>14.051920000000001</v>
-      </c>
-      <c r="C25" s="49">
-        <v>0.83204</v>
-      </c>
-      <c r="D25" s="13">
-        <v>15.15972</v>
-      </c>
-      <c r="E25" s="49">
-        <v>0.86431000000000002</v>
-      </c>
-      <c r="F25" s="82">
-        <v>18.527529999999999</v>
-      </c>
-      <c r="G25" s="13">
-        <v>0.94394999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="B26" s="13">
-        <v>13.87458</v>
+        <v>14.02351</v>
       </c>
       <c r="C26" s="49">
-        <v>0.82935000000000003</v>
+        <v>0.81435000000000002</v>
       </c>
       <c r="D26" s="13">
-        <v>15.59061</v>
+        <v>15.275</v>
       </c>
       <c r="E26" s="49">
-        <v>0.86753000000000002</v>
-      </c>
-      <c r="F26" s="13">
-        <v>17.965720000000001</v>
+        <v>0.86826000000000003</v>
+      </c>
+      <c r="F26" s="82">
+        <v>17.915420000000001</v>
       </c>
       <c r="G26" s="13">
-        <v>0.94262000000000001</v>
+        <v>0.94120999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B27" s="13">
-        <v>12.76966</v>
+        <v>14.051920000000001</v>
       </c>
       <c r="C27" s="49">
-        <v>0.80222000000000004</v>
+        <v>0.83204</v>
       </c>
       <c r="D27" s="13">
-        <v>14.243539999999999</v>
+        <v>15.15972</v>
       </c>
       <c r="E27" s="49">
-        <v>0.84404999999999997</v>
-      </c>
-      <c r="F27" s="13">
-        <v>17.19858</v>
+        <v>0.86431000000000002</v>
+      </c>
+      <c r="F27" s="82">
+        <v>18.527529999999999</v>
       </c>
       <c r="G27" s="13">
-        <v>0.92442000000000002</v>
+        <v>0.94394999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="13">
+        <v>13.87458</v>
+      </c>
+      <c r="C28" s="49">
+        <v>0.82935000000000003</v>
+      </c>
+      <c r="D28" s="13">
+        <v>15.59061</v>
+      </c>
+      <c r="E28" s="49">
+        <v>0.86753000000000002</v>
+      </c>
+      <c r="F28" s="13">
+        <v>17.965720000000001</v>
+      </c>
+      <c r="G28" s="13">
+        <v>0.94262000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" s="13">
+        <v>12.76966</v>
+      </c>
+      <c r="C29" s="49">
+        <v>0.80222000000000004</v>
+      </c>
+      <c r="D29" s="13">
+        <v>14.243539999999999</v>
+      </c>
+      <c r="E29" s="49">
+        <v>0.84404999999999997</v>
+      </c>
+      <c r="F29" s="13">
+        <v>17.19858</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0.92442000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B30" s="13">
         <v>12.74478</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C30" s="49">
         <v>0.79569000000000001</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D30" s="13">
         <v>14.030749999999999</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E30" s="49">
         <v>0.82940000000000003</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F30" s="13">
         <v>15.864240000000001</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G30" s="13">
         <v>0.91015000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B31" s="37">
         <v>16.07985</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C31" s="36">
         <v>0.83992</v>
       </c>
-      <c r="D29" s="50">
+      <c r="D31" s="50">
         <v>16.16921</v>
       </c>
-      <c r="E29" s="53">
+      <c r="E31" s="53">
         <v>0.88885000000000003</v>
       </c>
-      <c r="F29" s="50">
+      <c r="F31" s="50">
         <v>20.49427</v>
       </c>
-      <c r="G29" s="50">
+      <c r="G31" s="50">
         <v>0.95567999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="54">
+      <c r="B32" s="54">
         <v>15.988634545454545</v>
       </c>
-      <c r="C30" s="55">
+      <c r="C32" s="55">
         <v>0.8081772727272728</v>
       </c>
-      <c r="D30" s="54">
+      <c r="D32" s="54">
         <v>15.239140909090908</v>
       </c>
-      <c r="E30" s="55">
+      <c r="E32" s="55">
         <v>0.84778545454545451</v>
       </c>
-      <c r="F30" s="54">
+      <c r="F32" s="54">
         <v>22.100981428571426</v>
       </c>
-      <c r="G30" s="54">
+      <c r="G32" s="54">
         <v>0.9222164285714286</v>
       </c>
     </row>
@@ -4712,34 +5013,34 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H2">
-    <cfRule type="top10" dxfId="25" priority="21" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="43" priority="21" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:F1048576">
-    <cfRule type="top10" dxfId="24" priority="118" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F33:F1048576">
+    <cfRule type="top10" dxfId="42" priority="118" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C1048576">
-    <cfRule type="top10" dxfId="23" priority="121" percent="1" rank="10"/>
+  <conditionalFormatting sqref="C33:C1048576">
+    <cfRule type="top10" dxfId="41" priority="121" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20:D21 D31:D1048576">
-    <cfRule type="top10" dxfId="22" priority="124" percent="1" rank="10"/>
+  <conditionalFormatting sqref="D33:D1048576 D20:D23">
+    <cfRule type="top10" dxfId="40" priority="124" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E21 E31:E1048576">
-    <cfRule type="top10" dxfId="21" priority="128" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E33:E1048576 E20:E23">
+    <cfRule type="top10" dxfId="39" priority="128" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F21 F31:F1048576">
-    <cfRule type="top10" dxfId="20" priority="132" percent="1" rank="10"/>
+  <conditionalFormatting sqref="F33:F1048576 F20:F23">
+    <cfRule type="top10" dxfId="38" priority="132" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:H1048576 G20:H21 H2:H19 G31:G1048576">
-    <cfRule type="top10" dxfId="19" priority="136" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H31:H1048576 G20:H23 H2:H19 G33:G1048576">
+    <cfRule type="top10" dxfId="37" priority="136" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29:H1048576 H2 G31:G1048576">
-    <cfRule type="top10" dxfId="18" priority="144" percent="1" rank="10"/>
+  <conditionalFormatting sqref="H31:H1048576 H2 G33:G1048576">
+    <cfRule type="top10" dxfId="36" priority="144" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4751,7 +5052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90921C0C-3EF8-488C-A8AD-77E45C51350D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -4785,9 +5086,9 @@
         <v>50</v>
       </c>
       <c r="C2" s="101" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="126" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="132" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4800,9 +5101,9 @@
         <v>55</v>
       </c>
       <c r="C3" s="101" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="126"/>
+        <v>175</v>
+      </c>
+      <c r="D3" s="132"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
@@ -4813,7 +5114,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="101"/>
-      <c r="D4" s="126"/>
+      <c r="D4" s="132"/>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
@@ -4836,13 +5137,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4853,7 +5154,7 @@
       <c r="B7" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="126" t="s">
+      <c r="C7" s="132" t="s">
         <v>66</v>
       </c>
       <c r="D7" s="72" t="s">
@@ -4868,7 +5169,7 @@
       <c r="B8" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="125"/>
+      <c r="C8" s="131"/>
       <c r="D8" s="31" t="s">
         <v>77</v>
       </c>
@@ -4881,11 +5182,11 @@
       <c r="B9" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="126" t="s">
+      <c r="C9" s="132" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="99" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4896,9 +5197,9 @@
       <c r="B10" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="126"/>
+      <c r="C10" s="132"/>
       <c r="D10" s="101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4909,7 +5210,7 @@
       <c r="B11" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="126"/>
+      <c r="C11" s="132"/>
       <c r="D11" s="99"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -4920,7 +5221,7 @@
       <c r="B12" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="126"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="99"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -4929,9 +5230,9 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C13" s="125"/>
+        <v>166</v>
+      </c>
+      <c r="C13" s="131"/>
       <c r="D13" s="100"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4955,13 +5256,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4972,7 +5273,7 @@
       <c r="B16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="124" t="s">
+      <c r="C16" s="130" t="s">
         <v>67</v>
       </c>
       <c r="D16" s="32" t="s">
@@ -4987,7 +5288,7 @@
       <c r="B17" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="125"/>
+      <c r="C17" s="131"/>
       <c r="D17" s="32" t="s">
         <v>82</v>
       </c>
@@ -5021,12 +5322,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="133" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="127"/>
+      <c r="C1" s="133"/>
       <c r="D1" s="41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5041,7 +5342,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="69">
         <v>0.3</v>
@@ -5055,7 +5356,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="69">
         <v>0.3</v>
@@ -5069,7 +5370,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="70">
         <v>0.3</v>
@@ -5088,14 +5389,14 @@
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="127" t="s">
+      <c r="A7" s="133" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="127"/>
-      <c r="C7" s="127" t="s">
+      <c r="B7" s="133"/>
+      <c r="C7" s="133" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="127"/>
+      <c r="D7" s="133"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -5220,11 +5521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3513DC-2654-45B1-823E-7102A41B0B3D}">
-  <dimension ref="A1:L72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3513DC-2654-45B1-823E-7102A41B0B3D}">
+  <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:L15"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M79" sqref="M79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5234,7 +5535,10 @@
     <col min="3" max="3" width="13.5703125" style="19" customWidth="1"/>
     <col min="4" max="9" width="18.7109375" style="19" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" style="19" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="19"/>
+    <col min="11" max="12" width="9.140625" style="19"/>
+    <col min="13" max="13" width="21.140625" style="19" customWidth="1"/>
+    <col min="14" max="19" width="14.140625" style="19" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5248,22 +5552,22 @@
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="122" t="s">
+      <c r="C2" s="134"/>
+      <c r="D2" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122" t="s">
+      <c r="E2" s="128"/>
+      <c r="F2" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122" t="s">
+      <c r="G2" s="128"/>
+      <c r="H2" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="122"/>
+      <c r="I2" s="128"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -5525,14 +5829,14 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="128"/>
-      <c r="D13" s="122" t="s">
+      <c r="C13" s="134"/>
+      <c r="D13" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="122"/>
+      <c r="E13" s="128"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
@@ -5555,11 +5859,11 @@
       <c r="A15" s="19">
         <v>6</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="121" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="121" t="s">
         <v>178</v>
-      </c>
-      <c r="C15" s="131" t="s">
-        <v>179</v>
       </c>
       <c r="D15" s="117">
         <v>16.07985</v>
@@ -5591,10 +5895,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="60" t="s">
         <v>180</v>
-      </c>
-      <c r="C16" s="60" t="s">
-        <v>181</v>
       </c>
       <c r="D16" s="62">
         <v>14.184150000000001</v>
@@ -5608,10 +5912,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="61" t="s">
         <v>182</v>
-      </c>
-      <c r="C17" s="61" t="s">
-        <v>183</v>
       </c>
       <c r="D17" s="62">
         <v>14.59496</v>
@@ -5625,15 +5929,15 @@
         <v>10</v>
       </c>
       <c r="B18" s="64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="D18" s="129">
+        <v>183</v>
+      </c>
+      <c r="D18" s="119">
         <v>14.916359999999999</v>
       </c>
-      <c r="E18" s="129">
+      <c r="E18" s="119">
         <v>0.83982999999999997</v>
       </c>
     </row>
@@ -5642,14 +5946,14 @@
       <c r="E19" s="56"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="128" t="s">
+      <c r="B20" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="128"/>
-      <c r="D20" s="122" t="s">
+      <c r="C20" s="134"/>
+      <c r="D20" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="122"/>
+      <c r="E20" s="128"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
@@ -5666,11 +5970,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="131" t="s">
+      <c r="B22" s="121" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="121" t="s">
         <v>178</v>
-      </c>
-      <c r="C22" s="131" t="s">
-        <v>179</v>
       </c>
       <c r="D22" s="58">
         <v>16.16921</v>
@@ -5681,10 +5985,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="60" t="s">
         <v>180</v>
-      </c>
-      <c r="C23" s="60" t="s">
-        <v>181</v>
       </c>
       <c r="D23" s="62">
         <v>14.79847</v>
@@ -5695,10 +5999,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="61" t="s">
         <v>182</v>
-      </c>
-      <c r="C24" s="61" t="s">
-        <v>183</v>
       </c>
       <c r="D24" s="62">
         <v>15.852830000000001</v>
@@ -5709,15 +6013,15 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C25" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="D25" s="130">
+        <v>183</v>
+      </c>
+      <c r="D25" s="120">
         <v>16.407520000000002</v>
       </c>
-      <c r="E25" s="129">
+      <c r="E25" s="119">
         <v>0.88507000000000002</v>
       </c>
     </row>
@@ -5726,14 +6030,14 @@
       <c r="E26" s="56"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="128" t="s">
+      <c r="B27" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C27" s="128"/>
-      <c r="D27" s="122" t="s">
+      <c r="C27" s="134"/>
+      <c r="D27" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="122"/>
+      <c r="E27" s="128"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -5750,11 +6054,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="131" t="s">
+      <c r="B29" s="121" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="121" t="s">
         <v>178</v>
-      </c>
-      <c r="C29" s="131" t="s">
-        <v>179</v>
       </c>
       <c r="D29" s="63">
         <v>20.49427</v>
@@ -5765,10 +6069,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="60" t="s">
         <v>180</v>
-      </c>
-      <c r="C30" s="60" t="s">
-        <v>181</v>
       </c>
       <c r="D30" s="13">
         <v>19.391069999999999</v>
@@ -5779,10 +6083,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="C31" s="61" t="s">
         <v>182</v>
-      </c>
-      <c r="C31" s="61" t="s">
-        <v>183</v>
       </c>
       <c r="D31" s="13">
         <v>20.0871</v>
@@ -5793,10 +6097,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C32" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D32" s="66">
         <v>20.710329999999999</v>
@@ -5806,36 +6110,36 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="128" t="s">
+      <c r="B35" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="128"/>
+      <c r="C35" s="134"/>
       <c r="D35" s="90"/>
-      <c r="E35" s="122" t="s">
+      <c r="E35" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="122"/>
-      <c r="G35" s="122" t="s">
+      <c r="F35" s="128"/>
+      <c r="G35" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="122"/>
-      <c r="I35" s="122" t="s">
+      <c r="H35" s="128"/>
+      <c r="I35" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="122"/>
+      <c r="J35" s="128"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>139</v>
       </c>
       <c r="B36" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="D36" s="18" t="s">
         <v>169</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>170</v>
       </c>
       <c r="E36" s="51" t="s">
         <v>0</v>
@@ -6041,8 +6345,12 @@
       <c r="H42" s="13">
         <v>0.87604000000000004</v>
       </c>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
+      <c r="I42" s="13">
+        <v>20.649899999999999</v>
+      </c>
+      <c r="J42" s="13">
+        <v>0.95572000000000001</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="94">
@@ -6069,8 +6377,12 @@
       <c r="H43" s="13">
         <v>0.84702999999999995</v>
       </c>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
+      <c r="I43" s="13">
+        <v>19.71547</v>
+      </c>
+      <c r="J43" s="13">
+        <v>0.93979000000000001</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="95">
@@ -6097,8 +6409,12 @@
       <c r="H44" s="13">
         <v>0.86206000000000005</v>
       </c>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
+      <c r="I44" s="13">
+        <v>20.411180000000002</v>
+      </c>
+      <c r="J44" s="13">
+        <v>0.95338999999999996</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="95">
@@ -6125,8 +6441,12 @@
       <c r="H45" s="13">
         <v>0.87643000000000004</v>
       </c>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
+      <c r="I45" s="13">
+        <v>20.474989999999998</v>
+      </c>
+      <c r="J45" s="13">
+        <v>0.95396000000000003</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="95">
@@ -6153,25 +6473,29 @@
       <c r="H46" s="13">
         <v>0.88234999999999997</v>
       </c>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
+      <c r="I46" s="13">
+        <v>20.589639999999999</v>
+      </c>
+      <c r="J46" s="13">
+        <v>0.95399</v>
+      </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="128" t="s">
+      <c r="B50" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="128"/>
-      <c r="D50" s="122" t="s">
+      <c r="C50" s="134"/>
+      <c r="D50" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="122"/>
+      <c r="E50" s="128"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="102" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C51" s="102" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D51" s="51" t="s">
         <v>0</v>
@@ -6261,14 +6585,14 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="128" t="s">
+      <c r="B58" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="128"/>
-      <c r="D58" s="122" t="s">
+      <c r="C58" s="134"/>
+      <c r="D58" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="122"/>
+      <c r="E58" s="128"/>
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
@@ -6276,10 +6600,10 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="102" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C59" s="102" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D59" s="51" t="s">
         <v>0</v>
@@ -6370,22 +6694,22 @@
         <v>0.58896000000000004</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="128" t="s">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B66" s="134" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="128"/>
-      <c r="D66" s="122" t="s">
+      <c r="C66" s="134"/>
+      <c r="D66" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="122"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="128"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B67" s="102" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C67" s="102" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D67" s="51" t="s">
         <v>0</v>
@@ -6394,7 +6718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B68" s="115">
         <v>10</v>
       </c>
@@ -6408,7 +6732,7 @@
         <v>0.95567999999999997</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B69" s="106">
         <v>5</v>
       </c>
@@ -6422,7 +6746,7 @@
         <v>0.94513999999999998</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B70" s="106">
         <v>10</v>
       </c>
@@ -6436,7 +6760,7 @@
         <v>0.95504</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B71" s="106">
         <v>10</v>
       </c>
@@ -6450,7 +6774,7 @@
         <v>0.95513999999999999</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B72" s="110">
         <v>0</v>
       </c>
@@ -6464,8 +6788,791 @@
         <v>0.64602999999999999</v>
       </c>
     </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M73" s="9"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B74" s="134" t="s">
+        <v>130</v>
+      </c>
+      <c r="C74" s="134"/>
+      <c r="D74" s="118"/>
+      <c r="E74" s="128" t="s">
+        <v>29</v>
+      </c>
+      <c r="F74" s="128"/>
+      <c r="G74" s="128" t="s">
+        <v>43</v>
+      </c>
+      <c r="H74" s="128"/>
+      <c r="I74" s="128" t="s">
+        <v>30</v>
+      </c>
+      <c r="J74" s="128"/>
+      <c r="M74" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="N74" s="128" t="s">
+        <v>29</v>
+      </c>
+      <c r="O74" s="128"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E75" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F75" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G75" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="H75" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I75" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="J75" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M75" s="135" t="s">
+        <v>190</v>
+      </c>
+      <c r="N75" s="136">
+        <v>16.07985</v>
+      </c>
+      <c r="O75" s="50">
+        <v>0.83992</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A76" s="105">
+        <v>13</v>
+      </c>
+      <c r="B76" s="106">
+        <v>10</v>
+      </c>
+      <c r="C76" s="106">
+        <v>5</v>
+      </c>
+      <c r="D76" s="106">
+        <v>0</v>
+      </c>
+      <c r="E76" s="19">
+        <v>13.2196</v>
+      </c>
+      <c r="F76" s="25">
+        <v>0.78095999999999999</v>
+      </c>
+      <c r="G76" s="25">
+        <v>13.66483</v>
+      </c>
+      <c r="H76" s="25">
+        <v>0.80647999999999997</v>
+      </c>
+      <c r="I76" s="19">
+        <v>17.382850000000001</v>
+      </c>
+      <c r="J76" s="19">
+        <v>0.89870000000000005</v>
+      </c>
+      <c r="M76" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="N76" s="13">
+        <v>13.2196</v>
+      </c>
+      <c r="O76" s="13">
+        <v>0.78095999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" s="105">
+        <v>14</v>
+      </c>
+      <c r="B77" s="106">
+        <v>5</v>
+      </c>
+      <c r="C77" s="106">
+        <v>10</v>
+      </c>
+      <c r="D77" s="106">
+        <v>0</v>
+      </c>
+      <c r="E77" s="108">
+        <v>12.811349999999999</v>
+      </c>
+      <c r="F77" s="25">
+        <v>0.76766000000000001</v>
+      </c>
+      <c r="G77" s="25">
+        <v>13.14568</v>
+      </c>
+      <c r="H77" s="25">
+        <v>0.79279999999999995</v>
+      </c>
+      <c r="I77" s="108">
+        <v>17.2515</v>
+      </c>
+      <c r="J77" s="108">
+        <v>0.89229999999999998</v>
+      </c>
+      <c r="M77" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="N77" s="113">
+        <v>13.45574</v>
+      </c>
+      <c r="O77" s="113">
+        <v>0.79208999999999996</v>
+      </c>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" s="105">
+        <v>15</v>
+      </c>
+      <c r="B78" s="106">
+        <v>10</v>
+      </c>
+      <c r="C78" s="106">
+        <v>10</v>
+      </c>
+      <c r="D78" s="106">
+        <v>0</v>
+      </c>
+      <c r="E78" s="108"/>
+      <c r="F78" s="108"/>
+      <c r="G78" s="108"/>
+      <c r="H78" s="108"/>
+      <c r="I78" s="108"/>
+      <c r="J78" s="108"/>
+      <c r="M78" s="11"/>
+      <c r="N78" s="11"/>
+      <c r="O78" s="11"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" s="105">
+        <v>16</v>
+      </c>
+      <c r="B79" s="106">
+        <v>10</v>
+      </c>
+      <c r="C79" s="106">
+        <v>0</v>
+      </c>
+      <c r="D79" s="106">
+        <v>0</v>
+      </c>
+      <c r="E79" s="108"/>
+      <c r="F79" s="108"/>
+      <c r="G79" s="109"/>
+      <c r="H79" s="108"/>
+      <c r="I79" s="109"/>
+      <c r="J79" s="108"/>
+      <c r="M79" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="N79" s="128" t="s">
+        <v>43</v>
+      </c>
+      <c r="O79" s="128"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" s="94">
+        <v>17</v>
+      </c>
+      <c r="B80" s="92">
+        <v>0</v>
+      </c>
+      <c r="C80" s="93">
+        <v>10</v>
+      </c>
+      <c r="D80" s="92">
+        <v>0</v>
+      </c>
+      <c r="E80" s="103"/>
+      <c r="F80" s="103"/>
+      <c r="G80" s="103"/>
+      <c r="H80" s="103"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="M80" s="135" t="s">
+        <v>190</v>
+      </c>
+      <c r="N80" s="136">
+        <v>16.16921</v>
+      </c>
+      <c r="O80" s="50">
+        <v>0.88885000000000003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M81" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="N81" s="13">
+        <v>13.66483</v>
+      </c>
+      <c r="O81" s="13">
+        <v>0.80647999999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B82" s="134" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" s="134"/>
+      <c r="D82" s="123"/>
+      <c r="E82" s="128" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" s="128"/>
+      <c r="G82" s="128" t="s">
+        <v>43</v>
+      </c>
+      <c r="H82" s="128"/>
+      <c r="I82" s="128" t="s">
+        <v>30</v>
+      </c>
+      <c r="J82" s="128"/>
+      <c r="M82" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="N82" s="113">
+        <v>13.85941</v>
+      </c>
+      <c r="O82" s="113">
+        <v>0.81513999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F83" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G83" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="H83" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I83" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="J83" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="M83" s="9"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="105">
+        <v>13</v>
+      </c>
+      <c r="B84" s="106">
+        <v>10</v>
+      </c>
+      <c r="C84" s="106">
+        <v>5</v>
+      </c>
+      <c r="D84" s="106">
+        <v>0</v>
+      </c>
+      <c r="E84" s="13">
+        <v>13.45574</v>
+      </c>
+      <c r="F84" s="13">
+        <v>0.79208999999999996</v>
+      </c>
+      <c r="G84" s="13">
+        <v>13.85941</v>
+      </c>
+      <c r="H84" s="25">
+        <v>0.81513999999999998</v>
+      </c>
+      <c r="M84" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="N84" s="128" t="s">
+        <v>30</v>
+      </c>
+      <c r="O84" s="128"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="105">
+        <v>14</v>
+      </c>
+      <c r="B85" s="106">
+        <v>5</v>
+      </c>
+      <c r="C85" s="106">
+        <v>10</v>
+      </c>
+      <c r="D85" s="106">
+        <v>0</v>
+      </c>
+      <c r="E85" s="108"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="25"/>
+      <c r="H85" s="25"/>
+      <c r="I85" s="108"/>
+      <c r="J85" s="108"/>
+      <c r="M85" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="N85" s="50">
+        <v>20.49427</v>
+      </c>
+      <c r="O85" s="50">
+        <v>0.95567999999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" s="105">
+        <v>15</v>
+      </c>
+      <c r="B86" s="106">
+        <v>10</v>
+      </c>
+      <c r="C86" s="106">
+        <v>10</v>
+      </c>
+      <c r="D86" s="106">
+        <v>0</v>
+      </c>
+      <c r="E86" s="108"/>
+      <c r="F86" s="108"/>
+      <c r="G86" s="108"/>
+      <c r="H86" s="108"/>
+      <c r="I86" s="108"/>
+      <c r="J86" s="108"/>
+      <c r="M86" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="N86" s="13">
+        <v>17.382850000000001</v>
+      </c>
+      <c r="O86" s="13">
+        <v>0.89870000000000005</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" s="105">
+        <v>16</v>
+      </c>
+      <c r="B87" s="106">
+        <v>10</v>
+      </c>
+      <c r="C87" s="106">
+        <v>0</v>
+      </c>
+      <c r="D87" s="106">
+        <v>0</v>
+      </c>
+      <c r="E87" s="108"/>
+      <c r="F87" s="108"/>
+      <c r="G87" s="109"/>
+      <c r="H87" s="108"/>
+      <c r="I87" s="109"/>
+      <c r="J87" s="108"/>
+      <c r="M87" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="N87" s="113">
+        <v>17.78434</v>
+      </c>
+      <c r="O87" s="113">
+        <v>0.90647</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" s="94">
+        <v>17</v>
+      </c>
+      <c r="B88" s="92">
+        <v>0</v>
+      </c>
+      <c r="C88" s="93">
+        <v>10</v>
+      </c>
+      <c r="D88" s="92">
+        <v>0</v>
+      </c>
+      <c r="E88" s="103"/>
+      <c r="F88" s="103"/>
+      <c r="G88" s="103"/>
+      <c r="H88" s="103"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B91" s="134" t="s">
+        <v>130</v>
+      </c>
+      <c r="C91" s="134"/>
+      <c r="D91" s="122"/>
+      <c r="E91" s="128" t="s">
+        <v>29</v>
+      </c>
+      <c r="F91" s="128"/>
+      <c r="G91" s="128" t="s">
+        <v>43</v>
+      </c>
+      <c r="H91" s="128"/>
+      <c r="I91" s="128" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="128"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E92" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F92" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G92" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="H92" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I92" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="J92" s="51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="105">
+        <v>13</v>
+      </c>
+      <c r="B93" s="106">
+        <v>10</v>
+      </c>
+      <c r="C93" s="106">
+        <v>5</v>
+      </c>
+      <c r="D93" s="106">
+        <v>0</v>
+      </c>
+      <c r="E93" s="25">
+        <v>14.57211</v>
+      </c>
+      <c r="F93" s="25">
+        <v>0.83043999999999996</v>
+      </c>
+      <c r="G93" s="25">
+        <v>15.691879999999999</v>
+      </c>
+      <c r="H93" s="25">
+        <v>0.87455000000000005</v>
+      </c>
+      <c r="I93" s="25"/>
+      <c r="J93" s="25"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" s="105">
+        <v>14</v>
+      </c>
+      <c r="B94" s="106">
+        <v>5</v>
+      </c>
+      <c r="C94" s="106">
+        <v>10</v>
+      </c>
+      <c r="D94" s="106">
+        <v>0</v>
+      </c>
+      <c r="E94" s="108">
+        <v>14.76402</v>
+      </c>
+      <c r="F94" s="25">
+        <v>0.83486000000000005</v>
+      </c>
+      <c r="G94" s="25">
+        <v>15.606590000000001</v>
+      </c>
+      <c r="H94" s="25">
+        <v>0.87165000000000004</v>
+      </c>
+      <c r="I94" s="108"/>
+      <c r="J94" s="108"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="105">
+        <v>15</v>
+      </c>
+      <c r="B95" s="106">
+        <v>10</v>
+      </c>
+      <c r="C95" s="106">
+        <v>10</v>
+      </c>
+      <c r="D95" s="106">
+        <v>0</v>
+      </c>
+      <c r="E95" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="F95" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="G95" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="H95" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="I95" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="J95" s="108" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="105">
+        <v>16</v>
+      </c>
+      <c r="B96" s="106">
+        <v>10</v>
+      </c>
+      <c r="C96" s="106">
+        <v>0</v>
+      </c>
+      <c r="D96" s="106">
+        <v>0</v>
+      </c>
+      <c r="E96" s="108">
+        <v>14.853590000000001</v>
+      </c>
+      <c r="F96" s="108">
+        <v>0.83582000000000001</v>
+      </c>
+      <c r="G96" s="108">
+        <v>15.93506</v>
+      </c>
+      <c r="H96" s="108">
+        <v>0.87771999999999994</v>
+      </c>
+      <c r="I96" s="109"/>
+      <c r="J96" s="108"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="94">
+        <v>17</v>
+      </c>
+      <c r="B97" s="92">
+        <v>0</v>
+      </c>
+      <c r="C97" s="93">
+        <v>10</v>
+      </c>
+      <c r="D97" s="92">
+        <v>0</v>
+      </c>
+      <c r="E97" s="103">
+        <v>8.1155799999999996</v>
+      </c>
+      <c r="F97" s="103">
+        <v>0.47349000000000002</v>
+      </c>
+      <c r="G97" s="103">
+        <v>8.3343399999999992</v>
+      </c>
+      <c r="H97" s="103">
+        <v>0.59585999999999995</v>
+      </c>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="94">
+        <v>18</v>
+      </c>
+      <c r="B98" s="92">
+        <v>10</v>
+      </c>
+      <c r="C98" s="92">
+        <v>5</v>
+      </c>
+      <c r="D98" s="91">
+        <v>1</v>
+      </c>
+      <c r="E98" s="13">
+        <v>14.98395</v>
+      </c>
+      <c r="F98" s="13">
+        <v>0.83865000000000001</v>
+      </c>
+      <c r="G98" s="103">
+        <v>15.97369</v>
+      </c>
+      <c r="H98" s="103">
+        <v>0.87992000000000004</v>
+      </c>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="94">
+        <v>19</v>
+      </c>
+      <c r="B99" s="91">
+        <v>5</v>
+      </c>
+      <c r="C99" s="91">
+        <v>10</v>
+      </c>
+      <c r="D99" s="91">
+        <v>1</v>
+      </c>
+      <c r="E99" s="13">
+        <v>14.876709999999999</v>
+      </c>
+      <c r="F99" s="13">
+        <v>0.83791000000000004</v>
+      </c>
+      <c r="G99" s="103">
+        <v>16.149260000000002</v>
+      </c>
+      <c r="H99" s="103">
+        <v>0.88175999999999999</v>
+      </c>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="95">
+        <v>20</v>
+      </c>
+      <c r="B100" s="91">
+        <v>10</v>
+      </c>
+      <c r="C100" s="91">
+        <v>10</v>
+      </c>
+      <c r="D100" s="91">
+        <v>1</v>
+      </c>
+      <c r="E100" s="13">
+        <v>14.89654</v>
+      </c>
+      <c r="F100" s="13">
+        <v>0.83825000000000005</v>
+      </c>
+      <c r="G100" s="103">
+        <v>15.99527</v>
+      </c>
+      <c r="H100" s="103">
+        <v>0.88016000000000005</v>
+      </c>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="95">
+        <v>21</v>
+      </c>
+      <c r="B101" s="92">
+        <v>10</v>
+      </c>
+      <c r="C101" s="92">
+        <v>0</v>
+      </c>
+      <c r="D101" s="91">
+        <v>1</v>
+      </c>
+      <c r="E101" s="13">
+        <v>14.844620000000001</v>
+      </c>
+      <c r="F101" s="13">
+        <v>0.83764000000000005</v>
+      </c>
+      <c r="G101" s="103">
+        <v>15.91649</v>
+      </c>
+      <c r="H101" s="103">
+        <v>0.87902000000000002</v>
+      </c>
+      <c r="I101" s="13"/>
+      <c r="J101" s="13"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="95">
+        <v>22</v>
+      </c>
+      <c r="B102" s="92">
+        <v>0</v>
+      </c>
+      <c r="C102" s="93">
+        <v>10</v>
+      </c>
+      <c r="D102" s="91">
+        <v>1</v>
+      </c>
+      <c r="E102" s="13">
+        <v>14.5959</v>
+      </c>
+      <c r="F102" s="13">
+        <v>0.83413999999999999</v>
+      </c>
+      <c r="G102" s="103">
+        <v>16.394690000000001</v>
+      </c>
+      <c r="H102" s="103">
+        <v>0.88395999999999997</v>
+      </c>
+      <c r="I102" s="13"/>
+      <c r="J102" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="35">
+    <mergeCell ref="N74:O74"/>
+    <mergeCell ref="N79:O79"/>
+    <mergeCell ref="N84:O84"/>
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B27:C27"/>
@@ -6486,63 +7593,130 @@
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="I91:J91"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="I82:J82"/>
   </mergeCells>
   <conditionalFormatting sqref="E41:E46">
-    <cfRule type="top10" dxfId="17" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="37" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:F46">
-    <cfRule type="top10" dxfId="16" priority="18" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="36" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:G46">
-    <cfRule type="top10" dxfId="15" priority="17" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="33" priority="35" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41:H46">
-    <cfRule type="top10" dxfId="14" priority="16" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="32" priority="34" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I46">
-    <cfRule type="top10" dxfId="13" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="33" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:J46">
-    <cfRule type="top10" dxfId="12" priority="14" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="32" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F61">
-    <cfRule type="top10" dxfId="11" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="29" priority="28" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G61">
-    <cfRule type="top10" dxfId="10" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="28" priority="27" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H61">
-    <cfRule type="top10" dxfId="9" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="26" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57:I61">
-    <cfRule type="top10" dxfId="8" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="25" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57">
-    <cfRule type="top10" dxfId="7" priority="151" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="169" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="top10" dxfId="6" priority="152" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="24" priority="170" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D11">
+    <cfRule type="top10" dxfId="23" priority="24" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E11">
+    <cfRule type="top10" dxfId="22" priority="23" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F11">
+    <cfRule type="top10" dxfId="21" priority="22" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G11">
+    <cfRule type="top10" dxfId="20" priority="21" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H11">
+    <cfRule type="top10" dxfId="19" priority="20" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I11">
+    <cfRule type="top10" dxfId="18" priority="19" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E80">
+    <cfRule type="top10" dxfId="17" priority="18" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F80">
+    <cfRule type="top10" dxfId="16" priority="17" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G80">
+    <cfRule type="top10" dxfId="15" priority="16" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="top10" dxfId="14" priority="15" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I80">
+    <cfRule type="top10" dxfId="13" priority="14" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J80">
+    <cfRule type="top10" dxfId="12" priority="13" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E97:E102">
+    <cfRule type="top10" dxfId="11" priority="12" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F97:F102">
+    <cfRule type="top10" dxfId="10" priority="11" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G97:G102">
+    <cfRule type="top10" dxfId="9" priority="10" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H97:H102">
+    <cfRule type="top10" dxfId="8" priority="9" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I97:I102">
+    <cfRule type="top10" dxfId="7" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J97:J102">
+    <cfRule type="top10" dxfId="6" priority="7" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E88">
     <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E11">
+  <conditionalFormatting sqref="F88">
     <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F11">
+  <conditionalFormatting sqref="G88">
     <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G11">
+  <conditionalFormatting sqref="H88">
     <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H11">
+  <conditionalFormatting sqref="I88">
     <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I11">
+  <conditionalFormatting sqref="J88">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>